<commit_message>
Add FY21 & FY22 presentation links to £MHC
</commit_message>
<xml_diff>
--- a/£MHC.xlsx
+++ b/£MHC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F300A499-15EF-4FF3-B6F8-20D7E15858C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E2D1C4D-555A-477B-8CB5-A59E3CD821DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2685" yWindow="495" windowWidth="28800" windowHeight="18900" xr2:uid="{E461C7AA-D693-45DC-846F-4B1D3C8E259B}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="158">
   <si>
     <t>Stock Snapshot</t>
   </si>
@@ -492,6 +492,15 @@
   </si>
   <si>
     <t>Update</t>
+  </si>
+  <si>
+    <t>Presentations</t>
+  </si>
+  <si>
+    <t>FY 22</t>
+  </si>
+  <si>
+    <t>FY 21</t>
   </si>
 </sst>
 </file>
@@ -814,7 +823,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -989,19 +998,31 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1016,29 +1037,29 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1555,10 +1576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A865B090-C0E4-4B85-AA22-AACD646D3083}">
-  <dimension ref="A1:P40"/>
+  <dimension ref="A1:R40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="T26" sqref="T26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1605,10 +1626,10 @@
       <c r="J3" s="92" t="s">
         <v>149</v>
       </c>
-      <c r="K3" s="124" t="s">
+      <c r="K3" s="112" t="s">
         <v>153</v>
       </c>
-      <c r="L3" s="125"/>
+      <c r="L3" s="113"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
@@ -1621,8 +1642,8 @@
       <c r="J4" s="92" t="s">
         <v>150</v>
       </c>
-      <c r="K4" s="124"/>
-      <c r="L4" s="125"/>
+      <c r="K4" s="112"/>
+      <c r="L4" s="113"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -1659,10 +1680,10 @@
       <c r="J6" s="93" t="s">
         <v>151</v>
       </c>
-      <c r="K6" s="126" t="s">
+      <c r="K6" s="114" t="s">
         <v>152</v>
       </c>
-      <c r="L6" s="127"/>
+      <c r="L6" s="115"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
@@ -1860,10 +1881,10 @@
       <c r="B16" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="112" t="s">
+      <c r="C16" s="120" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="113"/>
+      <c r="D16" s="125"/>
       <c r="E16" s="1"/>
       <c r="F16" s="44">
         <v>44317</v>
@@ -1879,14 +1900,14 @@
       <c r="M16" s="25"/>
       <c r="N16" s="26"/>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="112" t="s">
+      <c r="C17" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="113"/>
+      <c r="D17" s="125"/>
       <c r="F17" s="44">
         <v>44348</v>
       </c>
@@ -1901,12 +1922,12 @@
       <c r="M17" s="25"/>
       <c r="N17" s="26"/>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="113"/>
-      <c r="D18" s="113"/>
+      <c r="C18" s="125"/>
+      <c r="D18" s="125"/>
       <c r="F18" s="44">
         <v>44409</v>
       </c>
@@ -1921,10 +1942,10 @@
       <c r="M18" s="25"/>
       <c r="N18" s="26"/>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" s="19"/>
-      <c r="C19" s="113"/>
-      <c r="D19" s="113"/>
+      <c r="C19" s="125"/>
+      <c r="D19" s="125"/>
       <c r="F19" s="44">
         <v>44440</v>
       </c>
@@ -1939,14 +1960,14 @@
       <c r="M19" s="25"/>
       <c r="N19" s="26"/>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B20" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="112" t="s">
+      <c r="C20" s="120" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="113"/>
+      <c r="D20" s="125"/>
       <c r="F20" s="44">
         <v>44501</v>
       </c>
@@ -1961,10 +1982,10 @@
       <c r="M20" s="25"/>
       <c r="N20" s="26"/>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B21" s="19"/>
-      <c r="C21" s="113"/>
-      <c r="D21" s="113"/>
+      <c r="C21" s="125"/>
+      <c r="D21" s="125"/>
       <c r="F21" s="44">
         <v>44652</v>
       </c>
@@ -1979,10 +2000,10 @@
       <c r="M21" s="25"/>
       <c r="N21" s="26"/>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22" s="20"/>
-      <c r="C22" s="114"/>
-      <c r="D22" s="115"/>
+      <c r="C22" s="126"/>
+      <c r="D22" s="127"/>
       <c r="F22" s="44">
         <v>44726</v>
       </c>
@@ -1997,7 +2018,7 @@
       <c r="M22" s="25"/>
       <c r="N22" s="26"/>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F23" s="44"/>
       <c r="G23" s="85" t="s">
         <v>134</v>
@@ -2010,7 +2031,7 @@
       <c r="M23" s="25"/>
       <c r="N23" s="26"/>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F24" s="44">
         <v>44743</v>
       </c>
@@ -2024,8 +2045,13 @@
       <c r="L24" s="25"/>
       <c r="M24" s="25"/>
       <c r="N24" s="26"/>
-    </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P24" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q24" s="110"/>
+      <c r="R24" s="111"/>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F25" s="44">
         <v>44743</v>
       </c>
@@ -2039,8 +2065,15 @@
       <c r="L25" s="25"/>
       <c r="M25" s="25"/>
       <c r="N25" s="26"/>
-    </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P25" s="92" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q25" s="131" t="s">
+        <v>152</v>
+      </c>
+      <c r="R25" s="132"/>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F26" s="45">
         <v>44774</v>
       </c>
@@ -2054,47 +2087,57 @@
       <c r="L26" s="27"/>
       <c r="M26" s="27"/>
       <c r="N26" s="28"/>
-    </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P26" s="92" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q26" s="131" t="s">
+        <v>152</v>
+      </c>
+      <c r="R26" s="132"/>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" s="116" t="s">
         <v>60</v>
       </c>
       <c r="C27" s="110"/>
       <c r="D27" s="111"/>
-    </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P27" s="93"/>
+      <c r="Q27" s="129"/>
+      <c r="R27" s="130"/>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B28" s="29">
         <v>43922</v>
       </c>
-      <c r="C28" s="112" t="s">
+      <c r="C28" s="120" t="s">
         <v>61</v>
       </c>
-      <c r="D28" s="113"/>
-    </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D28" s="125"/>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29" s="30">
         <v>44228</v>
       </c>
-      <c r="C29" s="114" t="s">
+      <c r="C29" s="126" t="s">
         <v>65</v>
       </c>
-      <c r="D29" s="115"/>
-    </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D29" s="127"/>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" s="116" t="s">
         <v>62</v>
       </c>
       <c r="C31" s="110"/>
       <c r="D31" s="111"/>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B32" s="29">
         <v>44136</v>
       </c>
-      <c r="C32" s="112" t="s">
+      <c r="C32" s="120" t="s">
         <v>63</v>
       </c>
-      <c r="D32" s="113"/>
+      <c r="D32" s="125"/>
       <c r="F32" s="109" t="s">
         <v>103</v>
       </c>
@@ -2112,14 +2155,14 @@
       <c r="B33" s="31">
         <v>44348</v>
       </c>
-      <c r="C33" s="114" t="s">
+      <c r="C33" s="126" t="s">
         <v>67</v>
       </c>
-      <c r="D33" s="115"/>
-      <c r="F33" s="117" t="s">
+      <c r="D33" s="127"/>
+      <c r="F33" s="121" t="s">
         <v>104</v>
       </c>
-      <c r="G33" s="118"/>
+      <c r="G33" s="122"/>
       <c r="H33" s="25" t="s">
         <v>108</v>
       </c>
@@ -2132,10 +2175,10 @@
       <c r="O33" s="26"/>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F34" s="117" t="s">
+      <c r="F34" s="121" t="s">
         <v>105</v>
       </c>
-      <c r="G34" s="118"/>
+      <c r="G34" s="122"/>
       <c r="H34" s="25" t="s">
         <v>109</v>
       </c>
@@ -2148,10 +2191,10 @@
       <c r="O34" s="26"/>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F35" s="119" t="s">
+      <c r="F35" s="123" t="s">
         <v>106</v>
       </c>
-      <c r="G35" s="120"/>
+      <c r="G35" s="124"/>
       <c r="H35" s="81" t="s">
         <v>135</v>
       </c>
@@ -2177,75 +2220,81 @@
       <c r="B37" s="88" t="s">
         <v>141</v>
       </c>
-      <c r="C37" s="121">
+      <c r="C37" s="117">
         <f>C6/'Financial Model'!P19</f>
         <v>6.3848982035928081</v>
       </c>
-      <c r="D37" s="122"/>
+      <c r="D37" s="118"/>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B38" s="88" t="s">
         <v>142</v>
       </c>
-      <c r="C38" s="121">
+      <c r="C38" s="117">
         <f>C6/'Financial Model'!I57</f>
         <v>1.6465343727852584</v>
       </c>
-      <c r="D38" s="122"/>
+      <c r="D38" s="118"/>
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B39" s="88"/>
-      <c r="C39" s="123"/>
-      <c r="D39" s="112"/>
+      <c r="C39" s="119"/>
+      <c r="D39" s="120"/>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B40" s="88" t="s">
         <v>145</v>
       </c>
-      <c r="C40" s="121">
+      <c r="C40" s="117">
         <f>C12/'Financial Model'!H18</f>
         <v>3.098319988102372</v>
       </c>
-      <c r="D40" s="122"/>
+      <c r="D40" s="118"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
+  <mergeCells count="33">
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="P24:R24"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
     <mergeCell ref="J2:L2"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="K6:L6"/>
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="B36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="B31:D31"/>
     <mergeCell ref="F33:G33"/>
     <mergeCell ref="F34:G34"/>
     <mergeCell ref="F9:N9"/>
     <mergeCell ref="F35:G35"/>
     <mergeCell ref="F32:O32"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
     <mergeCell ref="B27:D27"/>
     <mergeCell ref="C28:D28"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K6:L6" r:id="rId1" display="Link" xr:uid="{EBABCF04-F876-4DF1-ADF1-1B6F62DC4548}"/>
+    <hyperlink ref="Q25:R25" r:id="rId2" display="Link" xr:uid="{B44AF9A0-26DA-4646-BD16-513FFB8F6C87}"/>
+    <hyperlink ref="Q26:R26" r:id="rId3" display="Link" xr:uid="{95CF8495-03C0-4884-AA67-0EF8E6A9DD47}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="119" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup paperSize="119" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId4"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Update £MHC with news of options granted
</commit_message>
<xml_diff>
--- a/£MHC.xlsx
+++ b/£MHC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E2D1C4D-555A-477B-8CB5-A59E3CD821DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6B7FBD-94A6-4045-B31B-C1A2C7BE5078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="495" windowWidth="28800" windowHeight="18900" xr2:uid="{E461C7AA-D693-45DC-846F-4B1D3C8E259B}"/>
+    <workbookView xWindow="2680" yWindow="500" windowWidth="28800" windowHeight="18900" xr2:uid="{E461C7AA-D693-45DC-846F-4B1D3C8E259B}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -22,12 +22,22 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="159">
   <si>
     <t>Stock Snapshot</t>
   </si>
@@ -501,6 +511,9 @@
   </si>
   <si>
     <t>FY 21</t>
+  </si>
+  <si>
+    <t>16m share options granted to Exec. Dirs @ exercise price of 1.6p per share</t>
   </si>
 </sst>
 </file>
@@ -508,17 +521,17 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="11">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="#,##0.0"/>
-    <numFmt numFmtId="165" formatCode="#,##0.0;[Red]\ \ \-\ #,##0.0\ ;&quot;-&quot;"/>
-    <numFmt numFmtId="166" formatCode="#,##0%"/>
-    <numFmt numFmtId="167" formatCode="#,##0.0000"/>
-    <numFmt numFmtId="168" formatCode="#,##0.0;[Black]\(#,##0.0\)\ "/>
-    <numFmt numFmtId="169" formatCode="#,##0.0_);[Red]\(#,##0.0\)"/>
-    <numFmt numFmtId="170" formatCode="0.000"/>
-    <numFmt numFmtId="171" formatCode="0.0"/>
-    <numFmt numFmtId="172" formatCode="0.0\x"/>
-    <numFmt numFmtId="173" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0;[Red]\ \ \-\ #,##0.0\ ;&quot;-&quot;"/>
+    <numFmt numFmtId="167" formatCode="#,##0%"/>
+    <numFmt numFmtId="168" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="169" formatCode="#,##0.0;[Black]\(#,##0.0\)\ "/>
+    <numFmt numFmtId="170" formatCode="#,##0.0_);[Red]\(#,##0.0\)"/>
+    <numFmt numFmtId="171" formatCode="0.000"/>
+    <numFmt numFmtId="172" formatCode="0.0"/>
+    <numFmt numFmtId="173" formatCode="0.0\x"/>
+    <numFmt numFmtId="174" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -819,7 +832,7 @@
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -830,23 +843,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -857,7 +870,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -881,11 +894,11 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="8" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="8" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="8" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="8" fillId="9" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -902,20 +915,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
@@ -947,7 +960,7 @@
     <xf numFmtId="17" fontId="2" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -979,14 +992,26 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="2" fillId="8" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="2" fillId="8" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -996,6 +1021,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1010,21 +1059,6 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1037,29 +1071,8 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1067,7 +1080,7 @@
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Per cent" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1579,16 +1592,16 @@
   <dimension ref="A1:R40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T26" sqref="T26"/>
+      <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1597,7 +1610,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>8</v>
@@ -1607,13 +1620,13 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="J2" s="109" t="s">
+      <c r="J2" s="113" t="s">
         <v>148</v>
       </c>
-      <c r="K2" s="110"/>
-      <c r="L2" s="111"/>
-    </row>
-    <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K2" s="114"/>
+      <c r="L2" s="115"/>
+    </row>
+    <row r="3" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="3" t="s">
         <v>9</v>
@@ -1626,12 +1639,12 @@
       <c r="J3" s="92" t="s">
         <v>149</v>
       </c>
-      <c r="K3" s="112" t="s">
+      <c r="K3" s="124" t="s">
         <v>153</v>
       </c>
-      <c r="L3" s="113"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L3" s="125"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1642,16 +1655,16 @@
       <c r="J4" s="92" t="s">
         <v>150</v>
       </c>
-      <c r="K4" s="112"/>
-      <c r="L4" s="113"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K4" s="124"/>
+      <c r="L4" s="125"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
-      <c r="B5" s="109" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="110"/>
-      <c r="D5" s="111"/>
+      <c r="B5" s="113" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="114"/>
+      <c r="D5" s="115"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -1665,7 +1678,7 @@
         <v>44825</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="4" t="s">
         <v>1</v>
@@ -1680,12 +1693,12 @@
       <c r="J6" s="93" t="s">
         <v>151</v>
       </c>
-      <c r="K6" s="114" t="s">
+      <c r="K6" s="126" t="s">
         <v>152</v>
       </c>
-      <c r="L6" s="115"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L6" s="127"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="4" t="s">
         <v>2</v>
@@ -1700,7 +1713,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="4" t="s">
         <v>3</v>
@@ -1714,7 +1727,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="4" t="s">
         <v>4</v>
@@ -1726,19 +1739,19 @@
         <v>90</v>
       </c>
       <c r="E9" s="1"/>
-      <c r="F9" s="109" t="s">
+      <c r="F9" s="113" t="s">
         <v>59</v>
       </c>
-      <c r="G9" s="110"/>
-      <c r="H9" s="110"/>
-      <c r="I9" s="110"/>
-      <c r="J9" s="110"/>
-      <c r="K9" s="110"/>
-      <c r="L9" s="110"/>
-      <c r="M9" s="110"/>
-      <c r="N9" s="111"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G9" s="114"/>
+      <c r="H9" s="114"/>
+      <c r="I9" s="114"/>
+      <c r="J9" s="114"/>
+      <c r="K9" s="114"/>
+      <c r="L9" s="114"/>
+      <c r="M9" s="114"/>
+      <c r="N9" s="115"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="4" t="s">
         <v>5</v>
@@ -1764,7 +1777,7 @@
       <c r="M10" s="33"/>
       <c r="N10" s="26"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="4" t="s">
         <v>6</v>
@@ -1789,7 +1802,7 @@
       <c r="M11" s="33"/>
       <c r="N11" s="26"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="9" t="s">
         <v>7</v>
@@ -1814,7 +1827,7 @@
       <c r="M12" s="25"/>
       <c r="N12" s="26"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1834,7 +1847,7 @@
       <c r="M13" s="25"/>
       <c r="N13" s="26"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1854,13 +1867,13 @@
       <c r="M14" s="25"/>
       <c r="N14" s="26"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
-      <c r="B15" s="116" t="s">
+      <c r="B15" s="119" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="110"/>
-      <c r="D15" s="111"/>
+      <c r="C15" s="114"/>
+      <c r="D15" s="115"/>
       <c r="E15" s="1"/>
       <c r="F15" s="44">
         <v>44287</v>
@@ -1876,7 +1889,7 @@
       <c r="M15" s="25"/>
       <c r="N15" s="26"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="19" t="s">
         <v>11</v>
@@ -1884,7 +1897,7 @@
       <c r="C16" s="120" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="125"/>
+      <c r="D16" s="116"/>
       <c r="E16" s="1"/>
       <c r="F16" s="44">
         <v>44317</v>
@@ -1900,14 +1913,14 @@
       <c r="M16" s="25"/>
       <c r="N16" s="26"/>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B17" s="19" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="125"/>
+      <c r="D17" s="116"/>
       <c r="F17" s="44">
         <v>44348</v>
       </c>
@@ -1922,12 +1935,12 @@
       <c r="M17" s="25"/>
       <c r="N17" s="26"/>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B18" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="125"/>
-      <c r="D18" s="125"/>
+      <c r="C18" s="116"/>
+      <c r="D18" s="116"/>
       <c r="F18" s="44">
         <v>44409</v>
       </c>
@@ -1942,10 +1955,10 @@
       <c r="M18" s="25"/>
       <c r="N18" s="26"/>
     </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B19" s="19"/>
-      <c r="C19" s="125"/>
-      <c r="D19" s="125"/>
+      <c r="C19" s="116"/>
+      <c r="D19" s="116"/>
       <c r="F19" s="44">
         <v>44440</v>
       </c>
@@ -1960,14 +1973,14 @@
       <c r="M19" s="25"/>
       <c r="N19" s="26"/>
     </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B20" s="19" t="s">
         <v>52</v>
       </c>
       <c r="C20" s="120" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="125"/>
+      <c r="D20" s="116"/>
       <c r="F20" s="44">
         <v>44501</v>
       </c>
@@ -1982,10 +1995,10 @@
       <c r="M20" s="25"/>
       <c r="N20" s="26"/>
     </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B21" s="19"/>
-      <c r="C21" s="125"/>
-      <c r="D21" s="125"/>
+      <c r="C21" s="116"/>
+      <c r="D21" s="116"/>
       <c r="F21" s="44">
         <v>44652</v>
       </c>
@@ -2000,10 +2013,10 @@
       <c r="M21" s="25"/>
       <c r="N21" s="26"/>
     </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B22" s="20"/>
-      <c r="C22" s="126"/>
-      <c r="D22" s="127"/>
+      <c r="C22" s="117"/>
+      <c r="D22" s="118"/>
       <c r="F22" s="44">
         <v>44726</v>
       </c>
@@ -2018,7 +2031,7 @@
       <c r="M22" s="25"/>
       <c r="N22" s="26"/>
     </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:18" x14ac:dyDescent="0.2">
       <c r="F23" s="44"/>
       <c r="G23" s="85" t="s">
         <v>134</v>
@@ -2031,7 +2044,7 @@
       <c r="M23" s="25"/>
       <c r="N23" s="26"/>
     </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:18" x14ac:dyDescent="0.2">
       <c r="F24" s="44">
         <v>44743</v>
       </c>
@@ -2045,13 +2058,13 @@
       <c r="L24" s="25"/>
       <c r="M24" s="25"/>
       <c r="N24" s="26"/>
-      <c r="P24" s="109" t="s">
+      <c r="P24" s="113" t="s">
         <v>155</v>
       </c>
-      <c r="Q24" s="110"/>
-      <c r="R24" s="111"/>
-    </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="Q24" s="114"/>
+      <c r="R24" s="115"/>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.2">
       <c r="F25" s="44">
         <v>44743</v>
       </c>
@@ -2068,101 +2081,114 @@
       <c r="P25" s="92" t="s">
         <v>156</v>
       </c>
-      <c r="Q25" s="131" t="s">
+      <c r="Q25" s="109" t="s">
         <v>152</v>
       </c>
-      <c r="R25" s="132"/>
-    </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="F26" s="45">
+      <c r="R25" s="110"/>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="F26" s="44">
         <v>44774</v>
       </c>
-      <c r="G26" s="86" t="s">
+      <c r="G26" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="H26" s="27"/>
-      <c r="I26" s="27"/>
-      <c r="J26" s="27"/>
-      <c r="K26" s="27"/>
-      <c r="L26" s="27"/>
-      <c r="M26" s="27"/>
-      <c r="N26" s="28"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="25"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="25"/>
+      <c r="L26" s="25"/>
+      <c r="M26" s="25"/>
+      <c r="N26" s="26"/>
       <c r="P26" s="92" t="s">
         <v>157</v>
       </c>
-      <c r="Q26" s="131" t="s">
+      <c r="Q26" s="109" t="s">
         <v>152</v>
       </c>
-      <c r="R26" s="132"/>
-    </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B27" s="116" t="s">
+      <c r="R26" s="110"/>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B27" s="119" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="110"/>
-      <c r="D27" s="111"/>
+      <c r="C27" s="114"/>
+      <c r="D27" s="115"/>
+      <c r="F27" s="45">
+        <v>44835</v>
+      </c>
+      <c r="G27" s="86" t="s">
+        <v>158</v>
+      </c>
+      <c r="H27" s="27"/>
+      <c r="I27" s="27"/>
+      <c r="J27" s="27"/>
+      <c r="K27" s="27"/>
+      <c r="L27" s="27"/>
+      <c r="M27" s="27"/>
+      <c r="N27" s="28"/>
       <c r="P27" s="93"/>
-      <c r="Q27" s="129"/>
-      <c r="R27" s="130"/>
-    </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="Q27" s="111"/>
+      <c r="R27" s="112"/>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B28" s="29">
         <v>43922</v>
       </c>
       <c r="C28" s="120" t="s">
         <v>61</v>
       </c>
-      <c r="D28" s="125"/>
-    </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="D28" s="116"/>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B29" s="30">
         <v>44228</v>
       </c>
-      <c r="C29" s="126" t="s">
+      <c r="C29" s="117" t="s">
         <v>65</v>
       </c>
-      <c r="D29" s="127"/>
-    </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B31" s="116" t="s">
+      <c r="D29" s="118"/>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B31" s="119" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="110"/>
-      <c r="D31" s="111"/>
-    </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C31" s="114"/>
+      <c r="D31" s="115"/>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B32" s="29">
         <v>44136</v>
       </c>
       <c r="C32" s="120" t="s">
         <v>63</v>
       </c>
-      <c r="D32" s="125"/>
-      <c r="F32" s="109" t="s">
+      <c r="D32" s="116"/>
+      <c r="F32" s="113" t="s">
         <v>103</v>
       </c>
-      <c r="G32" s="110"/>
-      <c r="H32" s="110"/>
-      <c r="I32" s="110"/>
-      <c r="J32" s="110"/>
-      <c r="K32" s="110"/>
-      <c r="L32" s="110"/>
-      <c r="M32" s="110"/>
-      <c r="N32" s="110"/>
-      <c r="O32" s="111"/>
-    </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="G32" s="114"/>
+      <c r="H32" s="114"/>
+      <c r="I32" s="114"/>
+      <c r="J32" s="114"/>
+      <c r="K32" s="114"/>
+      <c r="L32" s="114"/>
+      <c r="M32" s="114"/>
+      <c r="N32" s="114"/>
+      <c r="O32" s="115"/>
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B33" s="31">
         <v>44348</v>
       </c>
-      <c r="C33" s="126" t="s">
+      <c r="C33" s="117" t="s">
         <v>67</v>
       </c>
-      <c r="D33" s="127"/>
-      <c r="F33" s="121" t="s">
+      <c r="D33" s="118"/>
+      <c r="F33" s="128" t="s">
         <v>104</v>
       </c>
-      <c r="G33" s="122"/>
+      <c r="G33" s="129"/>
       <c r="H33" s="25" t="s">
         <v>108</v>
       </c>
@@ -2174,11 +2200,11 @@
       <c r="N33" s="25"/>
       <c r="O33" s="26"/>
     </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F34" s="121" t="s">
+    <row r="34" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="F34" s="128" t="s">
         <v>105</v>
       </c>
-      <c r="G34" s="122"/>
+      <c r="G34" s="129"/>
       <c r="H34" s="25" t="s">
         <v>109</v>
       </c>
@@ -2190,11 +2216,11 @@
       <c r="N34" s="25"/>
       <c r="O34" s="26"/>
     </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F35" s="123" t="s">
+    <row r="35" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="F35" s="130" t="s">
         <v>106</v>
       </c>
-      <c r="G35" s="124"/>
+      <c r="G35" s="131"/>
       <c r="H35" s="81" t="s">
         <v>135</v>
       </c>
@@ -2209,67 +2235,50 @@
         <v>131</v>
       </c>
     </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B36" s="116" t="s">
+    <row r="36" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B36" s="119" t="s">
         <v>140</v>
       </c>
-      <c r="C36" s="110"/>
-      <c r="D36" s="111"/>
-    </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C36" s="114"/>
+      <c r="D36" s="115"/>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B37" s="88" t="s">
         <v>141</v>
       </c>
-      <c r="C37" s="117">
+      <c r="C37" s="121">
         <f>C6/'Financial Model'!P19</f>
         <v>6.3848982035928081</v>
       </c>
-      <c r="D37" s="118"/>
-    </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D37" s="122"/>
+    </row>
+    <row r="38" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B38" s="88" t="s">
         <v>142</v>
       </c>
-      <c r="C38" s="117">
+      <c r="C38" s="121">
         <f>C6/'Financial Model'!I57</f>
         <v>1.6465343727852584</v>
       </c>
-      <c r="D38" s="118"/>
-    </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D38" s="122"/>
+    </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B39" s="88"/>
-      <c r="C39" s="119"/>
+      <c r="C39" s="123"/>
       <c r="D39" s="120"/>
     </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B40" s="88" t="s">
         <v>145</v>
       </c>
-      <c r="C40" s="117">
+      <c r="C40" s="121">
         <f>C12/'Financial Model'!H18</f>
         <v>3.098319988102372</v>
       </c>
-      <c r="D40" s="118"/>
+      <c r="D40" s="122"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="P24:R24"/>
-    <mergeCell ref="Q25:R25"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
     <mergeCell ref="J2:L2"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="K6:L6"/>
@@ -2286,6 +2295,23 @@
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="P24:R24"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C22:D22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K6:L6" r:id="rId1" display="Link" xr:uid="{EBABCF04-F876-4DF1-ADF1-1B6F62DC4548}"/>
@@ -2309,23 +2335,23 @@
       <selection pane="bottomRight" activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="36" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" style="36" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" style="36"/>
-    <col min="13" max="16" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.1640625" customWidth="1"/>
+    <col min="2" max="2" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" style="36" customWidth="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5" style="36" customWidth="1"/>
+    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" style="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.83203125" style="36"/>
+    <col min="13" max="16" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:27" x14ac:dyDescent="0.2">
       <c r="C1" s="13" t="s">
         <v>87</v>
       </c>
@@ -2398,7 +2424,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="2:27" s="100" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:27" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="97"/>
       <c r="C2" s="21">
         <v>43646</v>
@@ -2468,7 +2494,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="2:27" s="83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:27" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="15"/>
       <c r="C3" s="14"/>
       <c r="D3" s="35"/>
@@ -2496,7 +2522,7 @@
       <c r="Z3" s="46"/>
       <c r="AA3" s="46"/>
     </row>
-    <row r="4" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B4" s="12" t="s">
         <v>16</v>
       </c>
@@ -2584,7 +2610,7 @@
         <v>190.64173102378848</v>
       </c>
     </row>
-    <row r="5" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>17</v>
       </c>
@@ -2672,7 +2698,7 @@
         <v>131.54279440641406</v>
       </c>
     </row>
-    <row r="6" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>33</v>
       </c>
@@ -2748,7 +2774,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B7" s="12" t="s">
         <v>18</v>
       </c>
@@ -2844,7 +2870,7 @@
         <v>59.098936617374427</v>
       </c>
     </row>
-    <row r="8" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B8" s="15" t="s">
         <v>34</v>
       </c>
@@ -2921,7 +2947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B9" s="15" t="s">
         <v>35</v>
       </c>
@@ -2998,7 +3024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>19</v>
       </c>
@@ -3086,7 +3112,7 @@
         <v>2.5529999999999999</v>
       </c>
     </row>
-    <row r="11" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>20</v>
       </c>
@@ -3163,7 +3189,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>21</v>
       </c>
@@ -3251,7 +3277,7 @@
         <v>0.112</v>
       </c>
     </row>
-    <row r="13" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>22</v>
       </c>
@@ -3346,7 +3372,7 @@
         <v>3.0790000000000002</v>
       </c>
     </row>
-    <row r="14" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B14" s="12" t="s">
         <v>55</v>
       </c>
@@ -3442,7 +3468,7 @@
         <v>56.019936617374427</v>
       </c>
     </row>
-    <row r="15" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>23</v>
       </c>
@@ -3531,7 +3557,7 @@
         <v>9.7928837876293681E-2</v>
       </c>
     </row>
-    <row r="16" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B16" s="12" t="s">
         <v>26</v>
       </c>
@@ -3627,7 +3653,7 @@
         <v>55.922007779498131</v>
       </c>
     </row>
-    <row r="17" spans="2:60" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:60" x14ac:dyDescent="0.2">
       <c r="B17" s="15" t="s">
         <v>24</v>
       </c>
@@ -3704,7 +3730,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="2:60" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:60" x14ac:dyDescent="0.2">
       <c r="B18" s="12" t="s">
         <v>25</v>
       </c>
@@ -3932,7 +3958,7 @@
         <v>39.426438587991925</v>
       </c>
     </row>
-    <row r="19" spans="2:60" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:60" x14ac:dyDescent="0.2">
       <c r="B19" s="15" t="s">
         <v>32</v>
       </c>
@@ -4028,7 +4054,7 @@
         <v>9.1329851754652344E-2</v>
       </c>
     </row>
-    <row r="20" spans="2:60" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:60" x14ac:dyDescent="0.2">
       <c r="B20" s="15" t="s">
         <v>2</v>
       </c>
@@ -4116,7 +4142,7 @@
         <v>710.85199999999998</v>
       </c>
     </row>
-    <row r="22" spans="2:60" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:60" x14ac:dyDescent="0.2">
       <c r="B22" s="15" t="s">
         <v>28</v>
       </c>
@@ -4214,7 +4240,7 @@
         <v>-1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="23" spans="2:60" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:60" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>29</v>
       </c>
@@ -4313,7 +4339,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="24" spans="2:60" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:60" x14ac:dyDescent="0.2">
       <c r="B24" s="15" t="s">
         <v>30</v>
       </c>
@@ -4413,7 +4439,7 @@
         <v>154.42854876708077</v>
       </c>
     </row>
-    <row r="25" spans="2:60" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:60" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>31</v>
       </c>
@@ -4513,7 +4539,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="2:60" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:60" x14ac:dyDescent="0.2">
       <c r="AC26" s="48" t="s">
         <v>123</v>
       </c>
@@ -4522,7 +4548,7 @@
         <v>161.42854876708077</v>
       </c>
     </row>
-    <row r="27" spans="2:60" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:60" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>93</v>
       </c>
@@ -4562,7 +4588,7 @@
       </c>
       <c r="AF27" s="106"/>
     </row>
-    <row r="28" spans="2:60" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:60" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B28" s="12" t="s">
         <v>97</v>
       </c>
@@ -4660,7 +4686,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="29" spans="2:60" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:60" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>128</v>
       </c>
@@ -4717,7 +4743,7 @@
       <c r="AC29" s="48"/>
       <c r="AD29" s="49"/>
     </row>
-    <row r="30" spans="2:60" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:60" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B30" s="12" t="s">
         <v>129</v>
       </c>
@@ -4777,7 +4803,7 @@
       <c r="AC30" s="50"/>
       <c r="AD30" s="105"/>
     </row>
-    <row r="31" spans="2:60" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:60" x14ac:dyDescent="0.2">
       <c r="C31" s="16"/>
       <c r="D31" s="67"/>
       <c r="E31" s="18"/>
@@ -4802,7 +4828,7 @@
       <c r="AC31" s="48"/>
       <c r="AD31" s="49"/>
     </row>
-    <row r="32" spans="2:60" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:60" x14ac:dyDescent="0.2">
       <c r="AC32" s="51" t="s">
         <v>126</v>
       </c>
@@ -4811,12 +4837,12 @@
         <v>11.496433372152271</v>
       </c>
     </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B33" s="32" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>69</v>
       </c>
@@ -4850,7 +4876,7 @@
         <v>0.16300000000000001</v>
       </c>
     </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>70</v>
       </c>
@@ -4884,7 +4910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>71</v>
       </c>
@@ -4918,7 +4944,7 @@
         <v>2.2890000000000001</v>
       </c>
     </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>72</v>
       </c>
@@ -4952,7 +4978,7 @@
         <v>0.497</v>
       </c>
     </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>73</v>
       </c>
@@ -4986,7 +5012,7 @@
         <v>2.3319999999999999</v>
       </c>
     </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>74</v>
       </c>
@@ -5020,7 +5046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B40" s="12" t="s">
         <v>4</v>
       </c>
@@ -5059,7 +5085,7 @@
         <v>6.3869999999999996</v>
       </c>
     </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>75</v>
       </c>
@@ -5099,7 +5125,7 @@
         <v>11.667999999999999</v>
       </c>
     </row>
-    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:16" x14ac:dyDescent="0.2">
       <c r="D42" s="62"/>
       <c r="E42" s="43"/>
       <c r="F42" s="62">
@@ -5115,7 +5141,7 @@
       <c r="O42" s="43"/>
       <c r="P42" s="43"/>
     </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>76</v>
       </c>
@@ -5149,7 +5175,7 @@
         <v>3.3149999999999999</v>
       </c>
     </row>
-    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>77</v>
       </c>
@@ -5183,7 +5209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>78</v>
       </c>
@@ -5217,7 +5243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>79</v>
       </c>
@@ -5251,7 +5277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>80</v>
       </c>
@@ -5285,7 +5311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>130</v>
       </c>
@@ -5318,7 +5344,7 @@
         <v>1.24</v>
       </c>
     </row>
-    <row r="49" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>82</v>
       </c>
@@ -5355,7 +5381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B50" s="12" t="s">
         <v>83</v>
       </c>
@@ -5396,7 +5422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>84</v>
       </c>
@@ -5436,7 +5462,7 @@
         <v>4.5549999999999997</v>
       </c>
     </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:16" x14ac:dyDescent="0.2">
       <c r="D52" s="62"/>
       <c r="E52" s="43"/>
       <c r="F52" s="62"/>
@@ -5449,7 +5475,7 @@
       <c r="O52" s="43"/>
       <c r="P52" s="43"/>
     </row>
-    <row r="53" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>85</v>
       </c>
@@ -5483,7 +5509,7 @@
         <v>7.1130000000000004</v>
       </c>
     </row>
-    <row r="54" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>86</v>
       </c>
@@ -5523,7 +5549,7 @@
         <v>11.667999999999999</v>
       </c>
     </row>
-    <row r="55" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:16" x14ac:dyDescent="0.2">
       <c r="D55" s="62"/>
       <c r="E55" s="43"/>
       <c r="F55" s="62"/>
@@ -5533,7 +5559,7 @@
       <c r="O55" s="43"/>
       <c r="P55" s="43"/>
     </row>
-    <row r="56" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>143</v>
       </c>
@@ -5574,7 +5600,7 @@
         <v>7.1129999999999995</v>
       </c>
     </row>
-    <row r="57" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>144</v>
       </c>
@@ -5615,7 +5641,7 @@
         <v>1.0006302296399251E-2</v>
       </c>
     </row>
-    <row r="58" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:16" x14ac:dyDescent="0.2">
       <c r="D58" s="62"/>
       <c r="E58" s="43"/>
       <c r="F58" s="62"/>
@@ -5625,7 +5651,7 @@
       <c r="O58" s="43"/>
       <c r="P58" s="43"/>
     </row>
-    <row r="61" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B61" s="32" t="s">
         <v>137</v>
       </c>
@@ -5652,21 +5678,21 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" customWidth="1"/>
-    <col min="2" max="2" width="47.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="2" max="2" width="47.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="128" t="s">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1" s="132" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="128"/>
-      <c r="D1" s="128"/>
-    </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C1" s="132"/>
+      <c r="D1" s="132"/>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C2" s="22">
         <v>44196</v>
       </c>
@@ -5674,7 +5700,7 @@
         <v>44342</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B3" s="41" t="s">
         <v>39</v>
       </c>
@@ -5685,7 +5711,7 @@
         <v>0.126</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" s="15" t="s">
         <v>53</v>
       </c>
@@ -5696,7 +5722,7 @@
         <v>8.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" s="41" t="s">
         <v>40</v>
       </c>
@@ -5707,7 +5733,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="41" t="s">
         <v>41</v>
       </c>
@@ -5718,7 +5744,7 @@
         <v>7.0999999999999994E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" s="41" t="s">
         <v>42</v>
       </c>
@@ -5729,7 +5755,7 @@
         <v>5.6000000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8" s="41" t="s">
         <v>44</v>
       </c>
@@ -5740,7 +5766,7 @@
         <v>3.4000000000000002E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B9" s="41" t="s">
         <v>43</v>
       </c>
@@ -5751,7 +5777,7 @@
         <v>5.3999999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" s="41" t="s">
         <v>45</v>
       </c>
@@ -5762,7 +5788,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B11" s="41" t="s">
         <v>46</v>
       </c>
@@ -5773,7 +5799,7 @@
         <v>3.1E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12" s="41" t="s">
         <v>47</v>
       </c>
@@ -5784,7 +5810,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B13" s="41" t="s">
         <v>48</v>
       </c>
@@ -5795,7 +5821,7 @@
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B14" s="15" t="s">
         <v>107</v>
       </c>
@@ -5806,7 +5832,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B15" s="15" t="s">
         <v>127</v>
       </c>
@@ -5817,7 +5843,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B16" s="15" t="s">
         <v>49</v>
       </c>

</xml_diff>

<commit_message>
Update £MHC P/S & EV/S, Update Trustpilot data
</commit_message>
<xml_diff>
--- a/£MHC.xlsx
+++ b/£MHC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6B7FBD-94A6-4045-B31B-C1A2C7BE5078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E7978C1-C5B0-9343-B8FE-B05DD446CD0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2680" yWindow="500" windowWidth="28800" windowHeight="18900" xr2:uid="{E461C7AA-D693-45DC-846F-4B1D3C8E259B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="161">
   <si>
     <t>Stock Snapshot</t>
   </si>
@@ -514,6 +514,12 @@
   </si>
   <si>
     <t>16m share options granted to Exec. Dirs @ exercise price of 1.6p per share</t>
+  </si>
+  <si>
+    <t>P/S</t>
+  </si>
+  <si>
+    <t>EV/S</t>
   </si>
 </sst>
 </file>
@@ -836,7 +842,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1002,18 +1008,6 @@
     <xf numFmtId="16" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1021,30 +1015,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1059,6 +1029,9 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1069,6 +1042,36 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1589,10 +1592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A865B090-C0E4-4B85-AA22-AACD646D3083}">
-  <dimension ref="A1:R40"/>
+  <dimension ref="A1:R41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K43" sqref="K43"/>
+      <selection activeCell="C41" sqref="C41:D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1620,11 +1623,11 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="J2" s="113" t="s">
+      <c r="J2" s="109" t="s">
         <v>148</v>
       </c>
-      <c r="K2" s="114"/>
-      <c r="L2" s="115"/>
+      <c r="K2" s="110"/>
+      <c r="L2" s="111"/>
     </row>
     <row r="3" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
@@ -1639,10 +1642,10 @@
       <c r="J3" s="92" t="s">
         <v>149</v>
       </c>
-      <c r="K3" s="124" t="s">
+      <c r="K3" s="112" t="s">
         <v>153</v>
       </c>
-      <c r="L3" s="125"/>
+      <c r="L3" s="113"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
@@ -1655,16 +1658,16 @@
       <c r="J4" s="92" t="s">
         <v>150</v>
       </c>
-      <c r="K4" s="124"/>
-      <c r="L4" s="125"/>
+      <c r="K4" s="112"/>
+      <c r="L4" s="113"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
-      <c r="B5" s="113" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="114"/>
-      <c r="D5" s="115"/>
+      <c r="B5" s="109" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="110"/>
+      <c r="D5" s="111"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -1684,7 +1687,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="23">
-        <v>1.7999999999999999E-2</v>
+        <v>1.6500000000000001E-2</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="1"/>
@@ -1693,10 +1696,10 @@
       <c r="J6" s="93" t="s">
         <v>151</v>
       </c>
-      <c r="K6" s="126" t="s">
+      <c r="K6" s="114" t="s">
         <v>152</v>
       </c>
-      <c r="L6" s="127"/>
+      <c r="L6" s="115"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
@@ -1720,7 +1723,7 @@
       </c>
       <c r="C8" s="6">
         <f>C6*C7</f>
-        <v>14.04162</v>
+        <v>12.871485000000002</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="1"/>
@@ -1739,17 +1742,17 @@
         <v>90</v>
       </c>
       <c r="E9" s="1"/>
-      <c r="F9" s="113" t="s">
+      <c r="F9" s="109" t="s">
         <v>59</v>
       </c>
-      <c r="G9" s="114"/>
-      <c r="H9" s="114"/>
-      <c r="I9" s="114"/>
-      <c r="J9" s="114"/>
-      <c r="K9" s="114"/>
-      <c r="L9" s="114"/>
-      <c r="M9" s="114"/>
-      <c r="N9" s="115"/>
+      <c r="G9" s="110"/>
+      <c r="H9" s="110"/>
+      <c r="I9" s="110"/>
+      <c r="J9" s="110"/>
+      <c r="K9" s="110"/>
+      <c r="L9" s="110"/>
+      <c r="M9" s="110"/>
+      <c r="N9" s="111"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
@@ -1809,7 +1812,7 @@
       </c>
       <c r="C12" s="10">
         <f>C8-C9+C10</f>
-        <v>7.04162</v>
+        <v>5.8714850000000016</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="1"/>
@@ -1869,11 +1872,11 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
-      <c r="B15" s="119" t="s">
+      <c r="B15" s="116" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="114"/>
-      <c r="D15" s="115"/>
+      <c r="C15" s="110"/>
+      <c r="D15" s="111"/>
       <c r="E15" s="1"/>
       <c r="F15" s="44">
         <v>44287</v>
@@ -1894,10 +1897,10 @@
       <c r="B16" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="120" t="s">
+      <c r="C16" s="121" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="116"/>
+      <c r="D16" s="122"/>
       <c r="E16" s="1"/>
       <c r="F16" s="44">
         <v>44317</v>
@@ -1917,10 +1920,10 @@
       <c r="B17" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="120" t="s">
+      <c r="C17" s="121" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="116"/>
+      <c r="D17" s="122"/>
       <c r="F17" s="44">
         <v>44348</v>
       </c>
@@ -1939,8 +1942,8 @@
       <c r="B18" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="116"/>
-      <c r="D18" s="116"/>
+      <c r="C18" s="122"/>
+      <c r="D18" s="122"/>
       <c r="F18" s="44">
         <v>44409</v>
       </c>
@@ -1957,8 +1960,8 @@
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B19" s="19"/>
-      <c r="C19" s="116"/>
-      <c r="D19" s="116"/>
+      <c r="C19" s="122"/>
+      <c r="D19" s="122"/>
       <c r="F19" s="44">
         <v>44440</v>
       </c>
@@ -1977,10 +1980,10 @@
       <c r="B20" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="120" t="s">
+      <c r="C20" s="121" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="116"/>
+      <c r="D20" s="122"/>
       <c r="F20" s="44">
         <v>44501</v>
       </c>
@@ -1997,8 +2000,8 @@
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B21" s="19"/>
-      <c r="C21" s="116"/>
-      <c r="D21" s="116"/>
+      <c r="C21" s="122"/>
+      <c r="D21" s="122"/>
       <c r="F21" s="44">
         <v>44652</v>
       </c>
@@ -2015,8 +2018,8 @@
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B22" s="20"/>
-      <c r="C22" s="117"/>
-      <c r="D22" s="118"/>
+      <c r="C22" s="123"/>
+      <c r="D22" s="124"/>
       <c r="F22" s="44">
         <v>44726</v>
       </c>
@@ -2058,11 +2061,11 @@
       <c r="L24" s="25"/>
       <c r="M24" s="25"/>
       <c r="N24" s="26"/>
-      <c r="P24" s="113" t="s">
+      <c r="P24" s="109" t="s">
         <v>155</v>
       </c>
-      <c r="Q24" s="114"/>
-      <c r="R24" s="115"/>
+      <c r="Q24" s="110"/>
+      <c r="R24" s="111"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.2">
       <c r="F25" s="44">
@@ -2081,10 +2084,10 @@
       <c r="P25" s="92" t="s">
         <v>156</v>
       </c>
-      <c r="Q25" s="109" t="s">
+      <c r="Q25" s="127" t="s">
         <v>152</v>
       </c>
-      <c r="R25" s="110"/>
+      <c r="R25" s="128"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.2">
       <c r="F26" s="44">
@@ -2103,17 +2106,17 @@
       <c r="P26" s="92" t="s">
         <v>157</v>
       </c>
-      <c r="Q26" s="109" t="s">
+      <c r="Q26" s="127" t="s">
         <v>152</v>
       </c>
-      <c r="R26" s="110"/>
+      <c r="R26" s="128"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B27" s="119" t="s">
+      <c r="B27" s="116" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="114"/>
-      <c r="D27" s="115"/>
+      <c r="C27" s="110"/>
+      <c r="D27" s="111"/>
       <c r="F27" s="45">
         <v>44835</v>
       </c>
@@ -2128,67 +2131,67 @@
       <c r="M27" s="27"/>
       <c r="N27" s="28"/>
       <c r="P27" s="93"/>
-      <c r="Q27" s="111"/>
-      <c r="R27" s="112"/>
+      <c r="Q27" s="129"/>
+      <c r="R27" s="130"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B28" s="29">
         <v>43922</v>
       </c>
-      <c r="C28" s="120" t="s">
+      <c r="C28" s="121" t="s">
         <v>61</v>
       </c>
-      <c r="D28" s="116"/>
+      <c r="D28" s="122"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B29" s="30">
         <v>44228</v>
       </c>
-      <c r="C29" s="117" t="s">
+      <c r="C29" s="123" t="s">
         <v>65</v>
       </c>
-      <c r="D29" s="118"/>
+      <c r="D29" s="124"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B31" s="119" t="s">
+      <c r="B31" s="116" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="114"/>
-      <c r="D31" s="115"/>
+      <c r="C31" s="110"/>
+      <c r="D31" s="111"/>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B32" s="29">
         <v>44136</v>
       </c>
-      <c r="C32" s="120" t="s">
+      <c r="C32" s="121" t="s">
         <v>63</v>
       </c>
-      <c r="D32" s="116"/>
-      <c r="F32" s="113" t="s">
+      <c r="D32" s="122"/>
+      <c r="F32" s="109" t="s">
         <v>103</v>
       </c>
-      <c r="G32" s="114"/>
-      <c r="H32" s="114"/>
-      <c r="I32" s="114"/>
-      <c r="J32" s="114"/>
-      <c r="K32" s="114"/>
-      <c r="L32" s="114"/>
-      <c r="M32" s="114"/>
-      <c r="N32" s="114"/>
-      <c r="O32" s="115"/>
+      <c r="G32" s="110"/>
+      <c r="H32" s="110"/>
+      <c r="I32" s="110"/>
+      <c r="J32" s="110"/>
+      <c r="K32" s="110"/>
+      <c r="L32" s="110"/>
+      <c r="M32" s="110"/>
+      <c r="N32" s="110"/>
+      <c r="O32" s="111"/>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B33" s="31">
         <v>44348</v>
       </c>
-      <c r="C33" s="117" t="s">
+      <c r="C33" s="123" t="s">
         <v>67</v>
       </c>
-      <c r="D33" s="118"/>
-      <c r="F33" s="128" t="s">
+      <c r="D33" s="124"/>
+      <c r="F33" s="117" t="s">
         <v>104</v>
       </c>
-      <c r="G33" s="129"/>
+      <c r="G33" s="118"/>
       <c r="H33" s="25" t="s">
         <v>108</v>
       </c>
@@ -2201,10 +2204,10 @@
       <c r="O33" s="26"/>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="F34" s="128" t="s">
+      <c r="F34" s="117" t="s">
         <v>105</v>
       </c>
-      <c r="G34" s="129"/>
+      <c r="G34" s="118"/>
       <c r="H34" s="25" t="s">
         <v>109</v>
       </c>
@@ -2217,10 +2220,10 @@
       <c r="O34" s="26"/>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="F35" s="130" t="s">
+      <c r="F35" s="119" t="s">
         <v>106</v>
       </c>
-      <c r="G35" s="131"/>
+      <c r="G35" s="120"/>
       <c r="H35" s="81" t="s">
         <v>135</v>
       </c>
@@ -2236,49 +2239,82 @@
       </c>
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B36" s="119" t="s">
+      <c r="B36" s="116" t="s">
         <v>140</v>
       </c>
-      <c r="C36" s="114"/>
-      <c r="D36" s="115"/>
+      <c r="C36" s="110"/>
+      <c r="D36" s="111"/>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B37" s="88" t="s">
         <v>141</v>
       </c>
-      <c r="C37" s="121">
+      <c r="C37" s="125">
         <f>C6/'Financial Model'!P19</f>
-        <v>6.3848982035928081</v>
-      </c>
-      <c r="D37" s="122"/>
+        <v>5.8528233532934077</v>
+      </c>
+      <c r="D37" s="126"/>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B38" s="88" t="s">
         <v>142</v>
       </c>
-      <c r="C38" s="121">
+      <c r="C38" s="125">
         <f>C6/'Financial Model'!I57</f>
-        <v>1.6465343727852584</v>
-      </c>
-      <c r="D38" s="122"/>
+        <v>1.5093231750531537</v>
+      </c>
+      <c r="D38" s="126"/>
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B39" s="88"/>
-      <c r="C39" s="123"/>
-      <c r="D39" s="120"/>
+      <c r="B39" s="88" t="s">
+        <v>159</v>
+      </c>
+      <c r="C39" s="125">
+        <f>C8/SUM('Financial Model'!H4:I4)</f>
+        <v>0.56124384670610328</v>
+      </c>
+      <c r="D39" s="126"/>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B40" s="88" t="s">
+        <v>160</v>
+      </c>
+      <c r="C40" s="125">
+        <f>C12/SUM('Financial Model'!H4:I4)</f>
+        <v>0.25601823156202919</v>
+      </c>
+      <c r="D40" s="126"/>
+    </row>
+    <row r="41" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B41" s="88" t="s">
         <v>145</v>
       </c>
-      <c r="C40" s="121">
+      <c r="C41" s="125">
         <f>C12/'Financial Model'!H18</f>
-        <v>3.098319988102372</v>
-      </c>
-      <c r="D40" s="122"/>
+        <v>2.5834593936257937</v>
+      </c>
+      <c r="D41" s="126"/>
     </row>
   </sheetData>
-  <mergeCells count="33">
+  <mergeCells count="34">
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="P24:R24"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C40:D40"/>
     <mergeCell ref="J2:L2"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="K6:L6"/>
@@ -2295,23 +2331,6 @@
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="P24:R24"/>
-    <mergeCell ref="Q25:R25"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C22:D22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K6:L6" r:id="rId1" display="Link" xr:uid="{EBABCF04-F876-4DF1-ADF1-1B6F62DC4548}"/>
@@ -2329,7 +2348,7 @@
   <dimension ref="B1:BH61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="D13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="K39" sqref="K39"/>
@@ -4683,7 +4702,7 @@
       </c>
       <c r="AD28" s="105">
         <f>Main!C6</f>
-        <v>1.7999999999999999E-2</v>
+        <v>1.6500000000000001E-2</v>
       </c>
     </row>
     <row r="29" spans="2:60" x14ac:dyDescent="0.2">
@@ -4834,7 +4853,7 @@
       </c>
       <c r="AD32" s="57">
         <f>AD27/AD28</f>
-        <v>11.496433372152271</v>
+        <v>12.541563678711567</v>
       </c>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.2">
@@ -5686,11 +5705,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1" s="132" t="s">
+      <c r="B1" s="131" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="132"/>
-      <c r="D1" s="132"/>
+      <c r="C1" s="131"/>
+      <c r="D1" s="131"/>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C2" s="22">

</xml_diff>

<commit_message>
Start Research List sheet
</commit_message>
<xml_diff>
--- a/£MHC.xlsx
+++ b/£MHC.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\My Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C6B11A4-FC2D-4FDC-B9FF-A82DE4480D9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C5B2D8-FEAE-4475-AFB2-7B36604A2DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{E461C7AA-D693-45DC-846F-4B1D3C8E259B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E461C7AA-D693-45DC-846F-4B1D3C8E259B}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
     <sheet name="Financial Model" sheetId="2" r:id="rId2"/>
-    <sheet name="Substantial Holdings" sheetId="3" r:id="rId3"/>
-    <sheet name="Historical Projections" sheetId="4" r:id="rId4"/>
+    <sheet name="Revenue Breakdown" sheetId="5" r:id="rId3"/>
+    <sheet name="Substantial Holdings" sheetId="3" r:id="rId4"/>
+    <sheet name="Historical Projections" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="253">
   <si>
     <t>Stock Snapshot</t>
   </si>
@@ -784,6 +785,18 @@
   </si>
   <si>
     <t>Projected</t>
+  </si>
+  <si>
+    <t>COVID</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>COVID Y/Y</t>
+  </si>
+  <si>
+    <t>Other Y/Y</t>
   </si>
 </sst>
 </file>
@@ -1160,7 +1173,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="160">
+  <cellXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1348,19 +1361,72 @@
     <xf numFmtId="17" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="15" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="173" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="173" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="4" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="17" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="15" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="15" fillId="10" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="15" fillId="10" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="15" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1387,62 +1453,11 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="15" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="17" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="15" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="15" fillId="10" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="15" fillId="10" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="15" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Accent3" xfId="1" builtinId="38"/>
@@ -1960,8 +1975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A865B090-C0E4-4B85-AA22-AACD646D3083}">
   <dimension ref="A1:AC105"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1989,11 +2004,11 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="J2" s="123" t="s">
+      <c r="J2" s="140" t="s">
         <v>148</v>
       </c>
-      <c r="K2" s="124"/>
-      <c r="L2" s="125"/>
+      <c r="K2" s="136"/>
+      <c r="L2" s="137"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -2008,10 +2023,10 @@
       <c r="J3" s="82" t="s">
         <v>149</v>
       </c>
-      <c r="K3" s="126" t="s">
+      <c r="K3" s="151" t="s">
         <v>153</v>
       </c>
-      <c r="L3" s="127"/>
+      <c r="L3" s="152"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
@@ -2024,16 +2039,16 @@
       <c r="J4" s="82" t="s">
         <v>150</v>
       </c>
-      <c r="K4" s="126"/>
-      <c r="L4" s="127"/>
+      <c r="K4" s="151"/>
+      <c r="L4" s="152"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="123" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="124"/>
-      <c r="D5" s="125"/>
+      <c r="B5" s="140" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="136"/>
+      <c r="D5" s="137"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -2062,10 +2077,10 @@
       <c r="J6" s="83" t="s">
         <v>151</v>
       </c>
-      <c r="K6" s="128" t="s">
+      <c r="K6" s="153" t="s">
         <v>152</v>
       </c>
-      <c r="L6" s="129"/>
+      <c r="L6" s="154"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
@@ -2109,17 +2124,17 @@
         <v>244</v>
       </c>
       <c r="E9" s="1"/>
-      <c r="F9" s="123" t="s">
+      <c r="F9" s="140" t="s">
         <v>59</v>
       </c>
-      <c r="G9" s="124"/>
-      <c r="H9" s="124"/>
-      <c r="I9" s="124"/>
-      <c r="J9" s="124"/>
-      <c r="K9" s="124"/>
-      <c r="L9" s="124"/>
-      <c r="M9" s="124"/>
-      <c r="N9" s="125"/>
+      <c r="G9" s="136"/>
+      <c r="H9" s="136"/>
+      <c r="I9" s="136"/>
+      <c r="J9" s="136"/>
+      <c r="K9" s="136"/>
+      <c r="L9" s="136"/>
+      <c r="M9" s="136"/>
+      <c r="N9" s="137"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
@@ -2239,11 +2254,11 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="134" t="s">
+      <c r="B15" s="135" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="124"/>
-      <c r="D15" s="125"/>
+      <c r="C15" s="136"/>
+      <c r="D15" s="137"/>
       <c r="E15" s="1"/>
       <c r="F15" s="114">
         <v>44287</v>
@@ -2264,10 +2279,10 @@
       <c r="B16" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="135" t="s">
+      <c r="C16" s="139" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="136"/>
+      <c r="D16" s="138"/>
       <c r="E16" s="1"/>
       <c r="F16" s="114">
         <v>44317</v>
@@ -2287,10 +2302,10 @@
       <c r="B17" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="135" t="s">
+      <c r="C17" s="139" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="136"/>
+      <c r="D17" s="138"/>
       <c r="F17" s="114">
         <v>44348</v>
       </c>
@@ -2309,8 +2324,8 @@
       <c r="B18" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="136"/>
-      <c r="D18" s="136"/>
+      <c r="C18" s="138"/>
+      <c r="D18" s="138"/>
       <c r="F18" s="114">
         <v>44409</v>
       </c>
@@ -2327,8 +2342,8 @@
     </row>
     <row r="19" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B19" s="18"/>
-      <c r="C19" s="136"/>
-      <c r="D19" s="136"/>
+      <c r="C19" s="138"/>
+      <c r="D19" s="138"/>
       <c r="F19" s="114">
         <v>44440</v>
       </c>
@@ -2347,10 +2362,10 @@
       <c r="B20" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="135" t="s">
+      <c r="C20" s="139" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="136"/>
+      <c r="D20" s="138"/>
       <c r="F20" s="114">
         <v>44501</v>
       </c>
@@ -2367,8 +2382,8 @@
     </row>
     <row r="21" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B21" s="18"/>
-      <c r="C21" s="136"/>
-      <c r="D21" s="136"/>
+      <c r="C21" s="138"/>
+      <c r="D21" s="138"/>
       <c r="F21" s="114">
         <v>44652</v>
       </c>
@@ -2385,8 +2400,8 @@
     </row>
     <row r="22" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B22" s="19"/>
-      <c r="C22" s="137"/>
-      <c r="D22" s="138"/>
+      <c r="C22" s="145"/>
+      <c r="D22" s="144"/>
       <c r="F22" s="114">
         <v>44726</v>
       </c>
@@ -2415,11 +2430,11 @@
       <c r="N23" s="23"/>
     </row>
     <row r="24" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B24" s="123" t="s">
+      <c r="B24" s="140" t="s">
         <v>237</v>
       </c>
-      <c r="C24" s="124"/>
-      <c r="D24" s="125"/>
+      <c r="C24" s="136"/>
+      <c r="D24" s="137"/>
       <c r="F24" s="114">
         <v>44743</v>
       </c>
@@ -2433,29 +2448,29 @@
       <c r="L24" s="22"/>
       <c r="M24" s="22"/>
       <c r="N24" s="23"/>
-      <c r="P24" s="123" t="s">
+      <c r="P24" s="140" t="s">
         <v>155</v>
       </c>
-      <c r="Q24" s="124"/>
-      <c r="R24" s="125"/>
-      <c r="W24" s="123" t="s">
+      <c r="Q24" s="136"/>
+      <c r="R24" s="137"/>
+      <c r="W24" s="140" t="s">
         <v>163</v>
       </c>
-      <c r="X24" s="124"/>
-      <c r="Y24" s="124"/>
-      <c r="Z24" s="124"/>
-      <c r="AA24" s="124"/>
-      <c r="AB24" s="124"/>
-      <c r="AC24" s="125"/>
+      <c r="X24" s="136"/>
+      <c r="Y24" s="136"/>
+      <c r="Z24" s="136"/>
+      <c r="AA24" s="136"/>
+      <c r="AB24" s="136"/>
+      <c r="AC24" s="137"/>
     </row>
     <row r="25" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B25" s="120">
         <v>45047</v>
       </c>
-      <c r="C25" s="141" t="s">
+      <c r="C25" s="143" t="s">
         <v>238</v>
       </c>
-      <c r="D25" s="138"/>
+      <c r="D25" s="144"/>
       <c r="F25" s="114">
         <v>44743</v>
       </c>
@@ -2472,10 +2487,10 @@
       <c r="P25" s="82" t="s">
         <v>156</v>
       </c>
-      <c r="Q25" s="142" t="s">
+      <c r="Q25" s="146" t="s">
         <v>152</v>
       </c>
-      <c r="R25" s="143"/>
+      <c r="R25" s="147"/>
       <c r="W25" s="112" t="s">
         <v>164</v>
       </c>
@@ -2503,10 +2518,10 @@
       <c r="P26" s="82" t="s">
         <v>157</v>
       </c>
-      <c r="Q26" s="142" t="s">
+      <c r="Q26" s="146" t="s">
         <v>152</v>
       </c>
-      <c r="R26" s="143"/>
+      <c r="R26" s="147"/>
       <c r="W26" s="112" t="s">
         <v>169</v>
       </c>
@@ -2518,11 +2533,11 @@
       <c r="AC26" s="23"/>
     </row>
     <row r="27" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B27" s="134" t="s">
+      <c r="B27" s="135" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="124"/>
-      <c r="D27" s="125"/>
+      <c r="C27" s="136"/>
+      <c r="D27" s="137"/>
       <c r="F27" s="114">
         <v>44835</v>
       </c>
@@ -2537,8 +2552,8 @@
       <c r="M27" s="22"/>
       <c r="N27" s="23"/>
       <c r="P27" s="83"/>
-      <c r="Q27" s="144"/>
-      <c r="R27" s="122"/>
+      <c r="Q27" s="148"/>
+      <c r="R27" s="149"/>
       <c r="W27" s="112" t="s">
         <v>165</v>
       </c>
@@ -2553,10 +2568,10 @@
       <c r="B28" s="26">
         <v>43922</v>
       </c>
-      <c r="C28" s="135" t="s">
+      <c r="C28" s="139" t="s">
         <v>61</v>
       </c>
-      <c r="D28" s="136"/>
+      <c r="D28" s="138"/>
       <c r="F28" s="114">
         <v>45047</v>
       </c>
@@ -2584,10 +2599,10 @@
       <c r="B29" s="27">
         <v>44228</v>
       </c>
-      <c r="C29" s="137" t="s">
+      <c r="C29" s="145" t="s">
         <v>65</v>
       </c>
-      <c r="D29" s="138"/>
+      <c r="D29" s="144"/>
       <c r="F29" s="114">
         <v>45047</v>
       </c>
@@ -2636,11 +2651,11 @@
       <c r="AC30" s="23"/>
     </row>
     <row r="31" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B31" s="134" t="s">
+      <c r="B31" s="135" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="124"/>
-      <c r="D31" s="125"/>
+      <c r="C31" s="136"/>
+      <c r="D31" s="137"/>
       <c r="F31" s="115">
         <v>45292</v>
       </c>
@@ -2668,10 +2683,10 @@
       <c r="B32" s="26">
         <v>44136</v>
       </c>
-      <c r="C32" s="135" t="s">
+      <c r="C32" s="139" t="s">
         <v>63</v>
       </c>
-      <c r="D32" s="136"/>
+      <c r="D32" s="138"/>
       <c r="W32" s="117" t="s">
         <v>171</v>
       </c>
@@ -2686,10 +2701,10 @@
       <c r="B33" s="28">
         <v>44348</v>
       </c>
-      <c r="C33" s="137" t="s">
+      <c r="C33" s="145" t="s">
         <v>67</v>
       </c>
-      <c r="D33" s="138"/>
+      <c r="D33" s="144"/>
       <c r="W33" s="112" t="s">
         <v>172</v>
       </c>
@@ -2723,23 +2738,23 @@
       <c r="AC35" s="23"/>
     </row>
     <row r="36" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B36" s="123" t="s">
+      <c r="B36" s="140" t="s">
         <v>140</v>
       </c>
-      <c r="C36" s="124"/>
-      <c r="D36" s="125"/>
-      <c r="F36" s="123" t="s">
+      <c r="C36" s="136"/>
+      <c r="D36" s="137"/>
+      <c r="F36" s="140" t="s">
         <v>103</v>
       </c>
-      <c r="G36" s="124"/>
-      <c r="H36" s="124"/>
-      <c r="I36" s="124"/>
-      <c r="J36" s="124"/>
-      <c r="K36" s="124"/>
-      <c r="L36" s="124"/>
-      <c r="M36" s="124"/>
-      <c r="N36" s="124"/>
-      <c r="O36" s="125"/>
+      <c r="G36" s="136"/>
+      <c r="H36" s="136"/>
+      <c r="I36" s="136"/>
+      <c r="J36" s="136"/>
+      <c r="K36" s="136"/>
+      <c r="L36" s="136"/>
+      <c r="M36" s="136"/>
+      <c r="N36" s="136"/>
+      <c r="O36" s="137"/>
       <c r="W36" s="112" t="s">
         <v>175</v>
       </c>
@@ -2754,15 +2769,15 @@
       <c r="B37" s="96" t="s">
         <v>141</v>
       </c>
-      <c r="C37" s="139">
+      <c r="C37" s="141">
         <f>C6/SUM('Financial Model'!H20:I20)</f>
         <v>39.329321190103592</v>
       </c>
-      <c r="D37" s="140"/>
-      <c r="F37" s="130" t="s">
+      <c r="D37" s="142"/>
+      <c r="F37" s="155" t="s">
         <v>104</v>
       </c>
-      <c r="G37" s="131"/>
+      <c r="G37" s="156"/>
       <c r="H37" s="22" t="s">
         <v>108</v>
       </c>
@@ -2787,15 +2802,15 @@
       <c r="B38" s="96" t="s">
         <v>142</v>
       </c>
-      <c r="C38" s="139">
+      <c r="C38" s="141">
         <f>C6/'Financial Model'!I58</f>
         <v>11.54403543586109</v>
       </c>
-      <c r="D38" s="140"/>
-      <c r="F38" s="130" t="s">
+      <c r="D38" s="142"/>
+      <c r="F38" s="155" t="s">
         <v>105</v>
       </c>
-      <c r="G38" s="131"/>
+      <c r="G38" s="156"/>
       <c r="H38" s="22" t="s">
         <v>109</v>
       </c>
@@ -2820,15 +2835,15 @@
       <c r="B39" s="96" t="s">
         <v>159</v>
       </c>
-      <c r="C39" s="139">
+      <c r="C39" s="141">
         <f>C8/SUM('Financial Model'!H4:I4)</f>
         <v>0.28617767052246557</v>
       </c>
-      <c r="D39" s="140"/>
-      <c r="F39" s="132" t="s">
+      <c r="D39" s="142"/>
+      <c r="F39" s="157" t="s">
         <v>106</v>
       </c>
-      <c r="G39" s="133"/>
+      <c r="G39" s="158"/>
       <c r="H39" s="24" t="s">
         <v>135</v>
       </c>
@@ -2856,11 +2871,11 @@
       <c r="B40" s="96" t="s">
         <v>160</v>
       </c>
-      <c r="C40" s="139">
+      <c r="C40" s="141">
         <f>C12/SUM('Financial Model'!H4:I4)</f>
         <v>-5.1750689101330759E-2</v>
       </c>
-      <c r="D40" s="140"/>
+      <c r="D40" s="142"/>
       <c r="W40" s="118" t="s">
         <v>179</v>
       </c>
@@ -2875,11 +2890,11 @@
       <c r="B41" s="96" t="s">
         <v>145</v>
       </c>
-      <c r="C41" s="139">
+      <c r="C41" s="141">
         <f>C12/SUM('Financial Model'!H19:I19)</f>
         <v>-0.52015223589902682</v>
       </c>
-      <c r="D41" s="140"/>
+      <c r="D41" s="142"/>
       <c r="W41" s="112"/>
       <c r="X41" s="22"/>
       <c r="Y41" s="22"/>
@@ -2892,11 +2907,11 @@
       <c r="B42" s="97" t="s">
         <v>161</v>
       </c>
-      <c r="C42" s="121">
+      <c r="C42" s="150">
         <f>'Financial Model'!I69</f>
         <v>0.17112763138524958</v>
       </c>
-      <c r="D42" s="122"/>
+      <c r="D42" s="149"/>
       <c r="W42" s="119" t="s">
         <v>180</v>
       </c>
@@ -3588,28 +3603,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="W24:AC24"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="P24:R24"/>
-    <mergeCell ref="Q25:R25"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C40:D40"/>
     <mergeCell ref="C42:D42"/>
     <mergeCell ref="J2:L2"/>
     <mergeCell ref="K3:L3"/>
@@ -3626,6 +3619,28 @@
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="C16:D16"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="P24:R24"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="W24:AC24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K6:L6" r:id="rId1" display="Link" xr:uid="{EBABCF04-F876-4DF1-ADF1-1B6F62DC4548}"/>
@@ -3642,7 +3657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80596E7F-DECF-497C-AD87-2DA392DA01F4}">
   <dimension ref="B1:BK72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="I4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -3664,7 +3679,7 @@
     <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.42578125" style="32" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" style="157"/>
+    <col min="14" max="14" width="8.85546875" style="132"/>
     <col min="16" max="21" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="9.140625" bestFit="1" customWidth="1"/>
@@ -3701,10 +3716,10 @@
       <c r="L1" s="30" t="s">
         <v>244</v>
       </c>
-      <c r="M1" s="149" t="s">
+      <c r="M1" s="124" t="s">
         <v>245</v>
       </c>
-      <c r="N1" s="151" t="s">
+      <c r="N1" s="126" t="s">
         <v>247</v>
       </c>
       <c r="O1" s="13"/>
@@ -3723,7 +3738,7 @@
       <c r="T1" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="U1" s="149" t="s">
+      <c r="U1" s="124" t="s">
         <v>110</v>
       </c>
       <c r="V1" s="13" t="s">
@@ -3791,7 +3806,7 @@
       <c r="M2" s="20">
         <v>45473</v>
       </c>
-      <c r="N2" s="152"/>
+      <c r="N2" s="127"/>
       <c r="P2" s="20">
         <v>43465</v>
       </c>
@@ -3854,10 +3869,10 @@
         <v>45146</v>
       </c>
       <c r="L3" s="76"/>
-      <c r="M3" s="146">
+      <c r="M3" s="121">
         <v>45561</v>
       </c>
-      <c r="N3" s="152" t="s">
+      <c r="N3" s="127" t="s">
         <v>248</v>
       </c>
       <c r="P3" s="20"/>
@@ -3904,21 +3919,21 @@
       <c r="I4" s="71">
         <v>9.8320000000000007</v>
       </c>
-      <c r="J4" s="150">
+      <c r="J4" s="125">
         <f>T4-I4</f>
         <v>12.481999999999999</v>
       </c>
       <c r="K4" s="71">
         <v>2.464</v>
       </c>
-      <c r="L4" s="150">
+      <c r="L4" s="125">
         <f>U4-K4</f>
         <v>8.5129999999999999</v>
       </c>
       <c r="M4" s="71">
         <v>0.88100000000000001</v>
       </c>
-      <c r="N4" s="153">
+      <c r="N4" s="128">
         <f>+M4*2.75</f>
         <v>2.4227500000000002</v>
       </c>
@@ -3946,7 +3961,7 @@
         <v>3.30375</v>
       </c>
       <c r="W4" s="71">
-        <f t="shared" ref="U4:AD4" si="0">V4*1.25</f>
+        <f t="shared" ref="W4:AD4" si="0">V4*1.25</f>
         <v>4.1296875000000002</v>
       </c>
       <c r="X4" s="71">
@@ -4020,7 +4035,7 @@
       <c r="M5" s="67">
         <v>1.167</v>
       </c>
-      <c r="N5" s="154"/>
+      <c r="N5" s="129"/>
       <c r="O5" s="67"/>
       <c r="P5" s="64">
         <v>0.54072100000000001</v>
@@ -4041,7 +4056,7 @@
         <v>8.9290000000000003</v>
       </c>
       <c r="V5" s="68">
-        <f t="shared" ref="U5:AD5" si="1">V4-V7</f>
+        <f t="shared" ref="V5:AD5" si="1">V4-V7</f>
         <v>2.2795874999999999</v>
       </c>
       <c r="W5" s="68">
@@ -4118,7 +4133,7 @@
       <c r="M6" s="67">
         <v>0</v>
       </c>
-      <c r="N6" s="154"/>
+      <c r="N6" s="129"/>
       <c r="O6" s="67"/>
       <c r="P6" s="65">
         <v>0</v>
@@ -4198,7 +4213,7 @@
         <f t="shared" si="2"/>
         <v>1.511000000000001</v>
       </c>
-      <c r="J7" s="150">
+      <c r="J7" s="125">
         <f>T7-I7</f>
         <v>3.2739999999999991</v>
       </c>
@@ -4214,7 +4229,7 @@
         <f t="shared" si="2"/>
         <v>-0.28600000000000003</v>
       </c>
-      <c r="N7" s="154">
+      <c r="N7" s="129">
         <f>N4*N23</f>
         <v>0.67837000000000014</v>
       </c>
@@ -4239,12 +4254,12 @@
         <f t="shared" ref="T7:U7" si="3">T4-T5-T6</f>
         <v>4.7850000000000001</v>
       </c>
-      <c r="U7" s="147">
+      <c r="U7" s="122">
         <f t="shared" si="3"/>
         <v>2.048</v>
       </c>
       <c r="V7" s="71">
-        <f t="shared" ref="U7:AD7" si="4">V4*0.31</f>
+        <f t="shared" ref="V7:AD7" si="4">V4*0.31</f>
         <v>1.0241625000000001</v>
       </c>
       <c r="W7" s="71">
@@ -4316,13 +4331,13 @@
         <v>0</v>
       </c>
       <c r="L8" s="70">
-        <f>U8-K8</f>
+        <f t="shared" ref="L8:L14" si="6">U8-K8</f>
         <v>0</v>
       </c>
       <c r="M8" s="67">
         <v>0</v>
       </c>
-      <c r="N8" s="154"/>
+      <c r="N8" s="129"/>
       <c r="O8" s="67"/>
       <c r="P8" s="65">
         <v>0</v>
@@ -4406,13 +4421,13 @@
         <v>0</v>
       </c>
       <c r="L9" s="70">
-        <f>U9-K9</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M9" s="67">
         <v>0</v>
       </c>
-      <c r="N9" s="154"/>
+      <c r="N9" s="129"/>
       <c r="O9" s="67"/>
       <c r="P9" s="65">
         <v>0</v>
@@ -4496,13 +4511,13 @@
         <v>0.75600000000000001</v>
       </c>
       <c r="L10" s="70">
-        <f>U10-K10</f>
+        <f t="shared" si="6"/>
         <v>0.87999999999999989</v>
       </c>
       <c r="M10" s="67">
         <v>0.76</v>
       </c>
-      <c r="N10" s="155"/>
+      <c r="N10" s="130"/>
       <c r="O10" s="67"/>
       <c r="P10" s="66">
         <v>2.213695</v>
@@ -4523,39 +4538,39 @@
         <v>1.6359999999999999</v>
       </c>
       <c r="V10" s="67">
-        <f t="shared" ref="U10:AD10" si="6">U10*1</f>
+        <f t="shared" ref="V10:AD10" si="7">U10*1</f>
         <v>1.6359999999999999</v>
       </c>
       <c r="W10" s="67">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.6359999999999999</v>
       </c>
       <c r="X10" s="67">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.6359999999999999</v>
       </c>
       <c r="Y10" s="67">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.6359999999999999</v>
       </c>
       <c r="Z10" s="67">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.6359999999999999</v>
       </c>
       <c r="AA10" s="67">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.6359999999999999</v>
       </c>
       <c r="AB10" s="67">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.6359999999999999</v>
       </c>
       <c r="AC10" s="67">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.6359999999999999</v>
       </c>
       <c r="AD10" s="67">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.6359999999999999</v>
       </c>
     </row>
@@ -4595,13 +4610,13 @@
         <v>0</v>
       </c>
       <c r="L11" s="70">
-        <f>U11-K11</f>
+        <f t="shared" si="6"/>
         <v>0.114</v>
       </c>
       <c r="M11" s="67">
         <v>0</v>
       </c>
-      <c r="N11" s="154"/>
+      <c r="N11" s="129"/>
       <c r="O11" s="67"/>
       <c r="P11" s="65">
         <v>0</v>
@@ -4686,13 +4701,13 @@
         <v>1.9E-2</v>
       </c>
       <c r="L12" s="70">
-        <f>U12-K12</f>
+        <f t="shared" si="6"/>
         <v>1.9E-2</v>
       </c>
       <c r="M12" s="67">
         <v>0.03</v>
       </c>
-      <c r="N12" s="154"/>
+      <c r="N12" s="129"/>
       <c r="O12" s="67"/>
       <c r="P12" s="66">
         <v>9.2290999999999998E-2</v>
@@ -4713,39 +4728,39 @@
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="V12" s="66">
-        <f t="shared" ref="U12:AD12" si="7">U12</f>
+        <f t="shared" ref="V12:AD12" si="8">U12</f>
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="W12" s="66">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="X12" s="66">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="Y12" s="66">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="Z12" s="66">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="AA12" s="66">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="AB12" s="66">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="AC12" s="66">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="AD12" s="66">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
@@ -4754,27 +4769,27 @@
         <v>22</v>
       </c>
       <c r="C13" s="66">
-        <f t="shared" ref="C13:H13" si="8">SUM(C8:C12)</f>
+        <f t="shared" ref="C13:H13" si="9">SUM(C8:C12)</f>
         <v>1.0944259999999999</v>
       </c>
       <c r="D13" s="72">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.91399000000000008</v>
       </c>
       <c r="E13" s="66">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.1855410000000002</v>
       </c>
       <c r="F13" s="72">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.9321486000000003</v>
       </c>
       <c r="G13" s="66">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.3668140000000002</v>
       </c>
       <c r="H13" s="72">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.7121859999999998</v>
       </c>
       <c r="I13" s="67">
@@ -4788,72 +4803,72 @@
         <v>0.77500000000000002</v>
       </c>
       <c r="L13" s="70">
-        <f>U13-K13</f>
+        <f t="shared" si="6"/>
         <v>1.0129999999999999</v>
       </c>
       <c r="M13" s="67">
         <v>0.79</v>
       </c>
-      <c r="N13" s="154"/>
+      <c r="N13" s="129"/>
       <c r="O13" s="67"/>
       <c r="P13" s="66">
-        <f>SUM(P8:P12)</f>
+        <f t="shared" ref="P13:U13" si="10">SUM(P8:P12)</f>
         <v>2.3059859999999999</v>
       </c>
       <c r="Q13" s="66">
-        <f>SUM(Q8:Q12)</f>
+        <f t="shared" si="10"/>
         <v>2.008416</v>
       </c>
       <c r="R13" s="66">
-        <f>SUM(R8:R12)</f>
+        <f t="shared" si="10"/>
         <v>3.1176895999999998</v>
       </c>
       <c r="S13" s="66">
-        <f>SUM(S8:S12)</f>
+        <f t="shared" si="10"/>
         <v>3.0790000000000002</v>
       </c>
-      <c r="T13" s="148">
-        <f>SUM(T8:T12)</f>
+      <c r="T13" s="123">
+        <f t="shared" si="10"/>
         <v>2.3430000000000004</v>
       </c>
       <c r="U13" s="66">
-        <f>SUM(U8:U12)</f>
+        <f t="shared" si="10"/>
         <v>1.788</v>
       </c>
       <c r="V13" s="67">
-        <f t="shared" ref="U13:AD13" si="9">U13</f>
+        <f t="shared" ref="V13:AD13" si="11">U13</f>
         <v>1.788</v>
       </c>
       <c r="W13" s="67">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.788</v>
       </c>
       <c r="X13" s="67">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.788</v>
       </c>
       <c r="Y13" s="67">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.788</v>
       </c>
       <c r="Z13" s="67">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.788</v>
       </c>
       <c r="AA13" s="67">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.788</v>
       </c>
       <c r="AB13" s="67">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.788</v>
       </c>
       <c r="AC13" s="67">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.788</v>
       </c>
       <c r="AD13" s="67">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.788</v>
       </c>
     </row>
@@ -4890,13 +4905,13 @@
         <v>0.23</v>
       </c>
       <c r="L14" s="70">
-        <f>U14-K14</f>
+        <f t="shared" si="6"/>
         <v>0.39100000000000001</v>
       </c>
       <c r="M14" s="67">
         <v>0.27200000000000002</v>
       </c>
-      <c r="N14" s="154"/>
+      <c r="N14" s="129"/>
       <c r="O14" s="67"/>
       <c r="P14" s="66">
         <v>0</v>
@@ -4921,35 +4936,35 @@
         <v>0.16518750000000001</v>
       </c>
       <c r="W14" s="67">
-        <f t="shared" ref="W14:AD14" si="10">W4*0.05</f>
+        <f t="shared" ref="W14:AD14" si="12">W4*0.05</f>
         <v>0.20648437500000003</v>
       </c>
       <c r="X14" s="67">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.25810546875000001</v>
       </c>
       <c r="Y14" s="67">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.3226318359375</v>
       </c>
       <c r="Z14" s="67">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.403289794921875</v>
       </c>
       <c r="AA14" s="67">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.50411224365234375</v>
       </c>
       <c r="AB14" s="67">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.63014030456542969</v>
       </c>
       <c r="AC14" s="67">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.78767538070678711</v>
       </c>
       <c r="AD14" s="67">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.98459422588348389</v>
       </c>
     </row>
@@ -4958,31 +4973,31 @@
         <v>55</v>
       </c>
       <c r="C15" s="63">
-        <f t="shared" ref="C15:M15" si="11">C7-C13</f>
+        <f t="shared" ref="C15:I15" si="13">C7-C13</f>
         <v>-1.3187889999999998</v>
       </c>
       <c r="D15" s="69">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-1.1497930000000001</v>
       </c>
       <c r="E15" s="63">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-1.3469010000000001</v>
       </c>
       <c r="F15" s="69">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-2.4110906000000005</v>
       </c>
       <c r="G15" s="63">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-0.2669400000000004</v>
       </c>
       <c r="H15" s="69">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>2.3129400000000002</v>
       </c>
       <c r="I15" s="63">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1.2000000000000899E-2</v>
       </c>
       <c r="J15" s="69">
@@ -5001,7 +5016,7 @@
         <f>M7-M13-M14</f>
         <v>-1.3480000000000001</v>
       </c>
-      <c r="N15" s="154"/>
+      <c r="N15" s="129"/>
       <c r="O15" s="67"/>
       <c r="P15" s="63">
         <f>P7-P13</f>
@@ -5028,39 +5043,39 @@
         <v>-0.36099999999999999</v>
       </c>
       <c r="V15" s="63">
-        <f t="shared" ref="V15:AD15" si="12">V7-V13-V14</f>
+        <f t="shared" ref="V15:AD15" si="14">V7-V13-V14</f>
         <v>-0.92902499999999999</v>
       </c>
       <c r="W15" s="63">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>-0.71428124999999998</v>
       </c>
       <c r="X15" s="63">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>-0.44585156249999996</v>
       </c>
       <c r="Y15" s="63">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>-0.11031445312500021</v>
       </c>
       <c r="Z15" s="63">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.30910693359374997</v>
       </c>
       <c r="AA15" s="63">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.83338366699218747</v>
       </c>
       <c r="AB15" s="63">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1.4887295837402341</v>
       </c>
       <c r="AC15" s="63">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>2.3079119796752927</v>
       </c>
       <c r="AD15" s="63">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>3.331889974594116</v>
       </c>
     </row>
@@ -5108,7 +5123,7 @@
         <f>0.001-0.15</f>
         <v>-0.14899999999999999</v>
       </c>
-      <c r="N16" s="154"/>
+      <c r="N16" s="129"/>
       <c r="O16" s="67"/>
       <c r="P16" s="66">
         <v>2.3914999999999999E-2</v>
@@ -5132,39 +5147,39 @@
         <v>-0.16600000000000001</v>
       </c>
       <c r="V16" s="67">
-        <f t="shared" ref="U16:AD16" si="13">U16*1.08</f>
+        <f t="shared" ref="V16:AD16" si="15">U16*1.08</f>
         <v>-0.17928000000000002</v>
       </c>
       <c r="W16" s="67">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>-0.19362240000000003</v>
       </c>
       <c r="X16" s="67">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>-0.20911219200000003</v>
       </c>
       <c r="Y16" s="67">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>-0.22584116736000004</v>
       </c>
       <c r="Z16" s="67">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>-0.24390846074880007</v>
       </c>
       <c r="AA16" s="67">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>-0.26342113760870411</v>
       </c>
       <c r="AB16" s="67">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>-0.28449482861740044</v>
       </c>
       <c r="AC16" s="67">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>-0.30725441490679251</v>
       </c>
       <c r="AD16" s="67">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>-0.33183476809933593</v>
       </c>
     </row>
@@ -5173,50 +5188,50 @@
         <v>26</v>
       </c>
       <c r="C17" s="63">
-        <f t="shared" ref="C17:M17" si="14">C15-C16</f>
+        <f t="shared" ref="C17:M17" si="16">C15-C16</f>
         <v>-1.3302649999999998</v>
       </c>
       <c r="D17" s="69">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>-1.1646640000000001</v>
       </c>
       <c r="E17" s="63">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>-1.3488820000000001</v>
       </c>
       <c r="F17" s="69">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>-2.4136676000000006</v>
       </c>
       <c r="G17" s="63">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>-0.2687220000000004</v>
       </c>
       <c r="H17" s="69">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>2.2727220000000004</v>
       </c>
       <c r="I17" s="63">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>9.0000000000008996E-3</v>
       </c>
       <c r="J17" s="69">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.5079999999999989</v>
       </c>
       <c r="K17" s="63">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>-0.35500000000000004</v>
       </c>
       <c r="L17" s="69">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.15999999999999925</v>
       </c>
       <c r="M17" s="63">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>-1.1990000000000001</v>
       </c>
-      <c r="N17" s="154"/>
+      <c r="N17" s="129"/>
       <c r="O17" s="67"/>
       <c r="P17" s="63">
         <f>P15-P16</f>
@@ -5235,47 +5250,47 @@
         <v>2.0040000000000018</v>
       </c>
       <c r="T17" s="63">
-        <f t="shared" ref="T17:U17" si="15">T15-T16</f>
+        <f t="shared" ref="T17:U17" si="17">T15-T16</f>
         <v>1.5169999999999999</v>
       </c>
       <c r="U17" s="63">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>-0.19499999999999998</v>
       </c>
       <c r="V17" s="63">
-        <f t="shared" ref="U17:AD17" si="16">V15-V16</f>
+        <f t="shared" ref="V17:AD17" si="18">V15-V16</f>
         <v>-0.74974499999999999</v>
       </c>
       <c r="W17" s="63">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>-0.52065885000000001</v>
       </c>
       <c r="X17" s="63">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>-0.23673937049999993</v>
       </c>
       <c r="Y17" s="63">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.11552671423499983</v>
       </c>
       <c r="Z17" s="63">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.55301539434254998</v>
       </c>
       <c r="AA17" s="63">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.0968048046008916</v>
       </c>
       <c r="AB17" s="63">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.7732244123576346</v>
       </c>
       <c r="AC17" s="63">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>2.6151663945820851</v>
       </c>
       <c r="AD17" s="63">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>3.6637247426934518</v>
       </c>
     </row>
@@ -5321,7 +5336,7 @@
       <c r="M18" s="66">
         <v>0</v>
       </c>
-      <c r="N18" s="156"/>
+      <c r="N18" s="131"/>
       <c r="O18" s="66"/>
       <c r="P18" s="66">
         <v>5.2276999999999997E-2</v>
@@ -5374,50 +5389,50 @@
         <v>25</v>
       </c>
       <c r="C19" s="63">
-        <f t="shared" ref="C19:M19" si="17">C17+C18</f>
+        <f t="shared" ref="C19:M19" si="19">C17+C18</f>
         <v>-1.2607869999999999</v>
       </c>
       <c r="D19" s="69">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-0.88926600000000011</v>
       </c>
       <c r="E19" s="63">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-1.3488820000000001</v>
       </c>
       <c r="F19" s="69">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-2.4136676000000006</v>
       </c>
       <c r="G19" s="63">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-0.2687220000000004</v>
       </c>
       <c r="H19" s="69">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>2.2727220000000004</v>
       </c>
       <c r="I19" s="63">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>9.0000000000008996E-3</v>
       </c>
       <c r="J19" s="69">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>1.5079999999999989</v>
       </c>
       <c r="K19" s="63">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-0.31900000000000006</v>
       </c>
       <c r="L19" s="69">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.15999999999999925</v>
       </c>
       <c r="M19" s="63">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-1.1990000000000001</v>
       </c>
-      <c r="N19" s="154"/>
+      <c r="N19" s="129"/>
       <c r="O19" s="67"/>
       <c r="P19" s="63">
         <f>P17+P18</f>
@@ -5436,179 +5451,179 @@
         <v>2.0040000000000018</v>
       </c>
       <c r="T19" s="63">
-        <f t="shared" ref="T19:U19" si="18">T17+T18</f>
+        <f t="shared" ref="T19:U19" si="20">T17+T18</f>
         <v>1.5169999999999999</v>
       </c>
       <c r="U19" s="63">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>-0.15899999999999997</v>
       </c>
       <c r="V19" s="63">
-        <f t="shared" ref="U19:AD19" si="19">V17+V18</f>
+        <f t="shared" ref="V19:AD19" si="21">V17+V18</f>
         <v>0.25025500000000001</v>
       </c>
       <c r="W19" s="63">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>1.47934115</v>
       </c>
       <c r="X19" s="63">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>2.7632606295</v>
       </c>
       <c r="Y19" s="63">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>4.115526714235</v>
       </c>
       <c r="Z19" s="63">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>5.55301539434255</v>
       </c>
       <c r="AA19" s="63">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>7.0968048046008914</v>
       </c>
       <c r="AB19" s="63">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>8.7732244123576351</v>
       </c>
       <c r="AC19" s="63">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>10.615166394582085</v>
       </c>
       <c r="AD19" s="63">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>12.663724742693452</v>
       </c>
       <c r="AE19" s="53">
-        <f t="shared" ref="AE19:BK19" si="20">AD19*(1+$AG$23)</f>
+        <f t="shared" ref="AE19:BK19" si="22">AD19*(1+$AG$23)</f>
         <v>12.47376887155305</v>
       </c>
       <c r="AF19" s="53">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>12.286662338479754</v>
       </c>
       <c r="AG19" s="53">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>12.102362403402557</v>
       </c>
       <c r="AH19" s="53">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>11.920826967351518</v>
       </c>
       <c r="AI19" s="53">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>11.742014562841245</v>
       </c>
       <c r="AJ19" s="53">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>11.565884344398626</v>
       </c>
       <c r="AK19" s="53">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>11.392396079232647</v>
       </c>
       <c r="AL19" s="53">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>11.221510138044158</v>
       </c>
       <c r="AM19" s="53">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>11.053187485973496</v>
       </c>
       <c r="AN19" s="53">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>10.887389673683893</v>
       </c>
       <c r="AO19" s="53">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>10.724078828578635</v>
       </c>
       <c r="AP19" s="53">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>10.563217646149957</v>
       </c>
       <c r="AQ19" s="53">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>10.404769381457706</v>
       </c>
       <c r="AR19" s="53">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>10.24869784073584</v>
       </c>
       <c r="AS19" s="53">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>10.094967373124803</v>
       </c>
       <c r="AT19" s="53">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>9.9435428625279307</v>
       </c>
       <c r="AU19" s="53">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>9.7943897195900114</v>
       </c>
       <c r="AV19" s="53">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>9.6474738737961605</v>
       </c>
       <c r="AW19" s="53">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>9.5027617656892183</v>
       </c>
       <c r="AX19" s="53">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>9.3602203392038792</v>
       </c>
       <c r="AY19" s="53">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>9.2198170341158203</v>
       </c>
       <c r="AZ19" s="53">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>9.0815197786040827</v>
       </c>
       <c r="BA19" s="53">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>8.9452969819250221</v>
       </c>
       <c r="BB19" s="53">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>8.8111175271961475</v>
       </c>
       <c r="BC19" s="53">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>8.6789507642882047</v>
       </c>
       <c r="BD19" s="53">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>8.5487665028238808</v>
       </c>
       <c r="BE19" s="53">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>8.420535005281522</v>
       </c>
       <c r="BF19" s="53">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>8.2942269802022999</v>
       </c>
       <c r="BG19" s="53">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>8.1698135754992656</v>
       </c>
       <c r="BH19" s="53">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>8.0472663718667761</v>
       </c>
       <c r="BI19" s="53">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>7.9265573762887742</v>
       </c>
       <c r="BJ19" s="53">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>7.8076590156444423</v>
       </c>
       <c r="BK19" s="53">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>7.6905441304097755</v>
       </c>
     </row>
@@ -5617,31 +5632,31 @@
         <v>32</v>
       </c>
       <c r="C20" s="66">
-        <f t="shared" ref="C20:I20" si="21">(C19/C21)</f>
+        <f t="shared" ref="C20:I20" si="23">(C19/C21)</f>
         <v>-5.8309467350935564E-3</v>
       </c>
       <c r="D20" s="72">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>-3.6932717437238396E-3</v>
       </c>
       <c r="E20" s="66">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>-3.9258307454951135E-3</v>
       </c>
       <c r="F20" s="72">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>-4.6611916836287381E-3</v>
       </c>
       <c r="G20" s="66">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>-4.0439192608093311E-4</v>
       </c>
       <c r="H20" s="72">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>3.1971802850663715E-3</v>
       </c>
       <c r="I20" s="66">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>1.1621600681801736E-5</v>
       </c>
       <c r="J20" s="70">
@@ -5649,7 +5664,7 @@
         <v>2.9213369959821909E-2</v>
       </c>
       <c r="K20" s="66">
-        <f t="shared" ref="K20:M20" si="22">(K19/K21)</f>
+        <f t="shared" ref="K20:M20" si="24">(K19/K21)</f>
         <v>-6.1339156463920321E-3</v>
       </c>
       <c r="L20" s="70">
@@ -5657,10 +5672,10 @@
         <v>3.0765721110430104E-3</v>
       </c>
       <c r="M20" s="66">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>-2.3055062257128667E-2</v>
       </c>
-      <c r="N20" s="154"/>
+      <c r="N20" s="129"/>
       <c r="O20" s="67"/>
       <c r="P20" s="66">
         <f>(P19/P21)</f>
@@ -5679,47 +5694,47 @@
         <v>2.8191522285932963E-3</v>
       </c>
       <c r="T20" s="66">
-        <f t="shared" ref="T20:AD20" si="23">(T19/T21)</f>
+        <f t="shared" ref="T20:AD20" si="25">(T19/T21)</f>
         <v>2.9387720311041025E-2</v>
       </c>
       <c r="U20" s="66">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>-3.0573435353490053E-3</v>
       </c>
       <c r="V20" s="66">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>4.8120472103067007E-3</v>
       </c>
       <c r="W20" s="66">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>2.8445623280051974E-2</v>
       </c>
       <c r="X20" s="66">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>5.3133566176643075E-2</v>
       </c>
       <c r="Y20" s="66">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>7.9135716945424608E-2</v>
       </c>
       <c r="Z20" s="66">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0.10677657684016796</v>
       </c>
       <c r="AA20" s="66">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0.13646144837094529</v>
       </c>
       <c r="AB20" s="66">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0.16869660969363331</v>
       </c>
       <c r="AC20" s="66">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0.20411453052282735</v>
       </c>
       <c r="AD20" s="66">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0.24350538978310113</v>
       </c>
     </row>
@@ -5765,7 +5780,7 @@
       <c r="M21" s="67">
         <v>52.005932000000001</v>
       </c>
-      <c r="N21" s="154"/>
+      <c r="N21" s="129"/>
       <c r="O21" s="67"/>
       <c r="P21" s="66">
         <v>158.321675</v>
@@ -5786,39 +5801,39 @@
         <v>52.005932000000001</v>
       </c>
       <c r="V21" s="66">
-        <f t="shared" ref="U21:AD21" si="24">U21</f>
+        <f t="shared" ref="V21:AD21" si="26">U21</f>
         <v>52.005932000000001</v>
       </c>
       <c r="W21" s="66">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>52.005932000000001</v>
       </c>
       <c r="X21" s="66">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>52.005932000000001</v>
       </c>
       <c r="Y21" s="66">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>52.005932000000001</v>
       </c>
       <c r="Z21" s="66">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>52.005932000000001</v>
       </c>
       <c r="AA21" s="66">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>52.005932000000001</v>
       </c>
       <c r="AB21" s="66">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>52.005932000000001</v>
       </c>
       <c r="AC21" s="66">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>52.005932000000001</v>
       </c>
       <c r="AD21" s="66">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>52.005932000000001</v>
       </c>
     </row>
@@ -5827,47 +5842,47 @@
         <v>28</v>
       </c>
       <c r="C23" s="16">
-        <f t="shared" ref="C23:H23" si="25">C7/C4</f>
+        <f t="shared" ref="C23:H23" si="27">C7/C4</f>
         <v>-14.275179741680983</v>
       </c>
       <c r="D23" s="33">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>-14.508275395311639</v>
       </c>
       <c r="E23" s="16">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>-12.698512630833399</v>
       </c>
       <c r="F23" s="33">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>-13.024284121502188</v>
       </c>
       <c r="G23" s="16">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>0.33592708936226096</v>
       </c>
       <c r="H23" s="33">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>0.30721802370732998</v>
       </c>
       <c r="I23" s="36">
         <v>0.31</v>
       </c>
       <c r="J23" s="33">
-        <f t="shared" ref="J23" si="26">J7/J4</f>
+        <f t="shared" ref="J23" si="28">J7/J4</f>
         <v>0.26229770870052871</v>
       </c>
       <c r="K23" s="36">
         <v>0.31</v>
       </c>
       <c r="L23" s="33">
-        <f t="shared" ref="L23" si="27">L7/L4</f>
+        <f t="shared" ref="L23" si="29">L7/L4</f>
         <v>0.1699753318454128</v>
       </c>
       <c r="M23" s="36">
         <v>0.31</v>
       </c>
-      <c r="N23" s="159">
+      <c r="N23" s="134">
         <v>0.28000000000000003</v>
       </c>
       <c r="P23" s="16">
@@ -5887,47 +5902,47 @@
         <v>0.31295798729848567</v>
       </c>
       <c r="T23" s="16">
-        <f t="shared" ref="T23:U23" si="28">T7/T4</f>
+        <f t="shared" ref="T23:U23" si="30">T7/T4</f>
         <v>0.21443936542081204</v>
       </c>
       <c r="U23" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>0.18657192311196139</v>
       </c>
       <c r="V23" s="16">
-        <f t="shared" ref="U23:AD23" si="29">V7/V4</f>
+        <f t="shared" ref="V23:AD23" si="31">V7/V4</f>
         <v>0.31000000000000005</v>
       </c>
       <c r="W23" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0.31</v>
       </c>
       <c r="X23" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0.31</v>
       </c>
       <c r="Y23" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0.31</v>
       </c>
       <c r="Z23" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0.31</v>
       </c>
       <c r="AA23" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0.31</v>
       </c>
       <c r="AB23" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0.31</v>
       </c>
       <c r="AC23" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0.31</v>
       </c>
       <c r="AD23" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0.31</v>
       </c>
       <c r="AF23" s="41" t="s">
@@ -5942,47 +5957,47 @@
         <v>29</v>
       </c>
       <c r="C24" s="16">
-        <f t="shared" ref="C24:H24" si="30">C15/C4</f>
+        <f t="shared" ref="C24:H24" si="32">C15/C4</f>
         <v>-83.908443087103137</v>
       </c>
       <c r="D24" s="33">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>-70.743431981787978</v>
       </c>
       <c r="E24" s="16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>-105.99677343196664</v>
       </c>
       <c r="F24" s="33">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>-65.566872433578993</v>
       </c>
       <c r="G24" s="16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>-8.1529681794789297E-2</v>
       </c>
       <c r="H24" s="33">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0.1765353074049438</v>
       </c>
       <c r="I24" s="16">
-        <f t="shared" ref="I24:J24" si="31">I15/I4</f>
+        <f t="shared" ref="I24:J24" si="33">I15/I4</f>
         <v>1.220504475183167E-3</v>
       </c>
       <c r="J24" s="33">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.11969235699407138</v>
       </c>
       <c r="K24" s="16">
-        <f t="shared" ref="K24:M24" si="32">K15/K4</f>
+        <f t="shared" ref="K24:M24" si="34">K15/K4</f>
         <v>-0.16396103896103897</v>
       </c>
       <c r="L24" s="33">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>5.0510983202160529E-3</v>
       </c>
       <c r="M24" s="16">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>-1.5300794551645858</v>
       </c>
       <c r="P24" s="16">
@@ -6002,47 +6017,47 @@
         <v>0.12493893502686867</v>
       </c>
       <c r="T24" s="16">
-        <f t="shared" ref="T24:U24" si="33">T15/T4</f>
+        <f t="shared" ref="T24:U24" si="35">T15/T4</f>
         <v>6.7491261091691304E-2</v>
       </c>
       <c r="U24" s="16">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>-3.2886945431356472E-2</v>
       </c>
       <c r="V24" s="16">
-        <f t="shared" ref="U24:AD24" si="34">V15/V4</f>
+        <f t="shared" ref="V24:AD24" si="36">V15/V4</f>
         <v>-0.28120317820658342</v>
       </c>
       <c r="W24" s="16">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>-0.17296254256526672</v>
       </c>
       <c r="X24" s="16">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>-8.6370034052213385E-2</v>
       </c>
       <c r="Y24" s="16">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>-1.7096027241770749E-2</v>
       </c>
       <c r="Z24" s="16">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>3.8323178206583423E-2</v>
       </c>
       <c r="AA24" s="16">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>8.2658542565266738E-2</v>
       </c>
       <c r="AB24" s="16">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>0.11812683405221337</v>
       </c>
       <c r="AC24" s="16">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>0.14650146724177071</v>
       </c>
       <c r="AD24" s="16">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>0.16920117379341656</v>
       </c>
       <c r="AF24" s="42" t="s">
@@ -6057,47 +6072,47 @@
         <v>30</v>
       </c>
       <c r="C25" s="16">
-        <f t="shared" ref="C25:H25" si="35">C19/C4</f>
+        <f t="shared" ref="C25:H25" si="37">C19/C4</f>
         <v>-80.218044156009412</v>
       </c>
       <c r="D25" s="33">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>-54.713960499600077</v>
       </c>
       <c r="E25" s="16">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>-106.15267175572521</v>
       </c>
       <c r="F25" s="33">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>-65.636951023849036</v>
       </c>
       <c r="G25" s="16">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>-8.2073946022549527E-2</v>
       </c>
       <c r="H25" s="33">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>0.17346566573969871</v>
       </c>
       <c r="I25" s="16">
-        <f t="shared" ref="I25:J25" si="36">I19/I4</f>
+        <f t="shared" ref="I25:J25" si="38">I19/I4</f>
         <v>9.1537835638739822E-4</v>
       </c>
       <c r="J25" s="33">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>0.12081397211985251</v>
       </c>
       <c r="K25" s="16">
-        <f t="shared" ref="K25:M25" si="37">K19/K4</f>
+        <f t="shared" ref="K25:M25" si="39">K19/K4</f>
         <v>-0.12946428571428575</v>
       </c>
       <c r="L25" s="33">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>1.8794784447315784E-2</v>
       </c>
       <c r="M25" s="16">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>-1.3609534619750285</v>
       </c>
       <c r="P25" s="16">
@@ -6117,47 +6132,47 @@
         <v>0.12237420615534939</v>
       </c>
       <c r="T25" s="16">
-        <f t="shared" ref="T25:U25" si="38">T19/T4</f>
+        <f t="shared" ref="T25:U25" si="40">T19/T4</f>
         <v>6.7984225150129959E-2</v>
       </c>
       <c r="U25" s="16">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v>-1.4484831921289968E-2</v>
       </c>
       <c r="V25" s="16">
-        <f t="shared" ref="U25:AD25" si="39">V19/V4</f>
+        <f t="shared" ref="V25:AD25" si="41">V19/V4</f>
         <v>7.5748770336738561E-2</v>
       </c>
       <c r="W25" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>0.35822108815739689</v>
       </c>
       <c r="X25" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>0.53529679996367763</v>
       </c>
       <c r="Y25" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>0.63780542646638516</v>
       </c>
       <c r="Z25" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>0.68846465547414559</v>
       </c>
       <c r="AA25" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>0.70389133511059254</v>
       </c>
       <c r="AB25" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>0.69613261910044033</v>
       </c>
       <c r="AC25" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>0.67382875322680613</v>
       </c>
       <c r="AD25" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>0.64309359174487313</v>
       </c>
       <c r="AF25" s="42" t="s">
@@ -6173,47 +6188,47 @@
         <v>31</v>
       </c>
       <c r="C26" s="16">
-        <f t="shared" ref="C26:H26" si="40">C18/C17</f>
+        <f t="shared" ref="C26:H26" si="42">C18/C17</f>
         <v>-5.222869127579844E-2</v>
       </c>
       <c r="D26" s="33">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>-0.23646133133676323</v>
       </c>
       <c r="E26" s="16">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="F26" s="33">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="G26" s="16">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="H26" s="33">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="I26" s="16">
-        <f t="shared" ref="I26:J26" si="41">I18/I17</f>
+        <f t="shared" ref="I26:J26" si="43">I18/I17</f>
         <v>0</v>
       </c>
       <c r="J26" s="33">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="K26" s="16">
-        <f t="shared" ref="K26:M26" si="42">K18/K17</f>
+        <f t="shared" ref="K26:M26" si="44">K18/K17</f>
         <v>-0.10140845070422533</v>
       </c>
       <c r="L26" s="33">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="M26" s="16">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="P26" s="16">
@@ -6233,47 +6248,47 @@
         <v>0</v>
       </c>
       <c r="T26" s="16">
-        <f t="shared" ref="T26:U26" si="43">T18/T17</f>
+        <f t="shared" ref="T26:U26" si="45">T18/T17</f>
         <v>0</v>
       </c>
       <c r="U26" s="16">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>-0.18461538461538463</v>
       </c>
       <c r="V26" s="16">
-        <f t="shared" ref="U26:AD26" si="44">V18/V17</f>
+        <f t="shared" ref="V26:AD26" si="46">V18/V17</f>
         <v>-1.3337868208524231</v>
       </c>
       <c r="W26" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>-3.8412868618290075</v>
       </c>
       <c r="X26" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>-12.672163458337829</v>
       </c>
       <c r="Y26" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>34.624026369029764</v>
       </c>
       <c r="Z26" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>9.0413396284279379</v>
       </c>
       <c r="AA26" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>5.470435555015003</v>
       </c>
       <c r="AB26" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>3.9476108896408526</v>
       </c>
       <c r="AC26" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>3.0590787708857947</v>
       </c>
       <c r="AD26" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>2.4565164230606178</v>
       </c>
       <c r="AF26" s="42" t="s">
@@ -6301,43 +6316,43 @@
         <v>0</v>
       </c>
       <c r="D28" s="34">
-        <f t="shared" ref="D28:M28" si="45">D4/C4-1</f>
+        <f t="shared" ref="D28:M28" si="47">D4/C4-1</f>
         <v>3.410320035630221E-2</v>
       </c>
       <c r="E28" s="36">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>-0.21817510613425217</v>
       </c>
       <c r="F28" s="34">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>1.893916738805383</v>
       </c>
       <c r="G28" s="17">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>88.036657330106323</v>
       </c>
       <c r="H28" s="34">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>3.0016111076326801</v>
       </c>
       <c r="I28" s="17">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>-0.24957191176363958</v>
       </c>
       <c r="J28" s="34">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>0.26952807160292913</v>
       </c>
       <c r="K28" s="17">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>-0.80259573786252203</v>
       </c>
       <c r="L28" s="34">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>2.4549512987012987</v>
       </c>
       <c r="M28" s="17">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>-0.89651121813696699</v>
       </c>
       <c r="AF28" s="44" t="s">
@@ -6360,42 +6375,42 @@
         <v>0</v>
       </c>
       <c r="E29" s="91">
-        <f>E4/C4-1</f>
+        <f t="shared" ref="E29:M29" si="48">E4/C4-1</f>
         <v>-0.19151237513520392</v>
       </c>
       <c r="F29" s="92">
-        <f>F4/D4-1</f>
+        <f t="shared" si="48"/>
         <v>1.2625361471728298</v>
       </c>
       <c r="G29" s="91">
-        <f>G4/E4-1</f>
+        <f t="shared" si="48"/>
         <v>256.6646730148737</v>
       </c>
       <c r="H29" s="92">
-        <f>H4/F4-1</f>
+        <f t="shared" si="48"/>
         <v>355.29007695863817</v>
       </c>
       <c r="I29" s="91">
-        <f>I4/G4-1</f>
+        <f t="shared" si="48"/>
         <v>2.0029213733661768</v>
       </c>
       <c r="J29" s="92">
-        <f>J4/H4-1</f>
+        <f t="shared" si="48"/>
         <v>-4.7310476264620593E-2</v>
       </c>
       <c r="K29" s="91">
-        <f>K4/I4-1</f>
+        <f t="shared" si="48"/>
         <v>-0.74938974776240852</v>
       </c>
       <c r="L29" s="92">
-        <f>L4/J4-1</f>
+        <f t="shared" si="48"/>
         <v>-0.3179778881589489</v>
       </c>
       <c r="M29" s="91">
-        <f>M4/K4-1</f>
+        <f t="shared" si="48"/>
         <v>-0.64245129870129869</v>
       </c>
-      <c r="N29" s="158"/>
+      <c r="N29" s="133"/>
       <c r="P29" s="89">
         <v>0</v>
       </c>
@@ -6412,47 +6427,47 @@
         <v>329.9620048504446</v>
       </c>
       <c r="T29" s="91">
-        <f t="shared" ref="T29:U29" si="46">T4/S4-1</f>
+        <f t="shared" ref="T29:U29" si="49">T4/S4-1</f>
         <v>0.36260381045432322</v>
       </c>
       <c r="U29" s="91">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>-0.50806668459263249</v>
       </c>
       <c r="V29" s="91">
-        <f t="shared" ref="U29:V29" si="47">V4/U4-1</f>
+        <f t="shared" ref="V29" si="50">V4/U4-1</f>
         <v>-0.69902978955998907</v>
       </c>
       <c r="W29" s="91">
-        <f t="shared" ref="W29:AD29" si="48">W4/V4-1</f>
+        <f t="shared" ref="W29:AD29" si="51">W4/V4-1</f>
         <v>0.25</v>
       </c>
       <c r="X29" s="91">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>0.25</v>
       </c>
       <c r="Y29" s="91">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>0.25</v>
       </c>
       <c r="Z29" s="91">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>0.25</v>
       </c>
       <c r="AA29" s="91">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>0.25</v>
       </c>
       <c r="AB29" s="91">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>0.25</v>
       </c>
       <c r="AC29" s="91">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>0.25</v>
       </c>
       <c r="AD29" s="91">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>0.25</v>
       </c>
       <c r="AF29" s="44" t="s">
@@ -6471,43 +6486,43 @@
         <v>0</v>
       </c>
       <c r="D30" s="35">
-        <f t="shared" ref="D30:M30" si="49">D19/C19-1</f>
+        <f t="shared" ref="D30:M30" si="52">D19/C19-1</f>
         <v>-0.29467388226560065</v>
       </c>
       <c r="E30" s="17">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>0.51684872692760098</v>
       </c>
       <c r="F30" s="35">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>0.78938380080689075</v>
       </c>
       <c r="G30" s="17">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>-0.8886665255812356</v>
       </c>
       <c r="H30" s="35">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>-9.4575211556924881</v>
       </c>
       <c r="I30" s="17">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>-0.99603999081277828</v>
       </c>
       <c r="J30" s="35">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>166.55555555553869</v>
       </c>
       <c r="K30" s="17">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>-1.2115384615384617</v>
       </c>
       <c r="L30" s="35">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>-1.5015673981191198</v>
       </c>
       <c r="M30" s="17">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>-8.4937500000000341</v>
       </c>
       <c r="P30" s="15">
@@ -6551,42 +6566,42 @@
         <v>0</v>
       </c>
       <c r="E31" s="91">
-        <f>E19/C19-1</f>
+        <f t="shared" ref="E31:M31" si="53">E19/C19-1</f>
         <v>6.9873023754210895E-2</v>
       </c>
       <c r="F31" s="92">
-        <f>F19/D19-1</f>
+        <f t="shared" si="53"/>
         <v>1.7142245402388041</v>
       </c>
       <c r="G31" s="91">
-        <f>G19/E19-1</f>
+        <f t="shared" si="53"/>
         <v>-0.80078168438751474</v>
       </c>
       <c r="H31" s="92">
-        <f>H19/F19-1</f>
+        <f t="shared" si="53"/>
         <v>-1.941605215233448</v>
       </c>
       <c r="I31" s="91">
-        <f>I19/G19-1</f>
+        <f t="shared" si="53"/>
         <v>-1.0334918614776643</v>
       </c>
       <c r="J31" s="92">
-        <f>J19/H19-1</f>
+        <f t="shared" si="53"/>
         <v>-0.33647846063002929</v>
       </c>
       <c r="K31" s="91">
-        <f>K19/I19-1</f>
+        <f t="shared" si="53"/>
         <v>-36.444444444440911</v>
       </c>
       <c r="L31" s="92">
-        <f>L19/J19-1</f>
+        <f t="shared" si="53"/>
         <v>-0.89389920424403224</v>
       </c>
       <c r="M31" s="91">
-        <f>M19/K19-1</f>
+        <f t="shared" si="53"/>
         <v>2.7586206896551717</v>
       </c>
-      <c r="N31" s="158"/>
+      <c r="N31" s="133"/>
       <c r="P31" s="89">
         <v>0</v>
       </c>
@@ -6603,11 +6618,11 @@
         <v>-1.5326175633671386</v>
       </c>
       <c r="T31" s="91">
-        <f t="shared" ref="T31:U31" si="50">T19/S19-1</f>
+        <f t="shared" ref="T31:U31" si="54">T19/S19-1</f>
         <v>-0.24301397205588893</v>
       </c>
       <c r="U31" s="91">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>-1.1048121292023731</v>
       </c>
       <c r="V31" s="91"/>
@@ -6672,7 +6687,7 @@
         <v>7.0184999999999997E-2</v>
       </c>
       <c r="F35" s="56">
-        <f t="shared" ref="F35:F41" si="51">R35</f>
+        <f t="shared" ref="F35:F41" si="55">R35</f>
         <v>5.5516999999999997E-2</v>
       </c>
       <c r="G35" s="54">
@@ -6706,7 +6721,7 @@
         <v>0</v>
       </c>
       <c r="F36" s="56">
-        <f t="shared" si="51"/>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
       <c r="G36" s="55">
@@ -6740,7 +6755,7 @@
         <v>0.74207100000000004</v>
       </c>
       <c r="F37" s="56">
-        <f t="shared" si="51"/>
+        <f t="shared" si="55"/>
         <v>0.61656</v>
       </c>
       <c r="G37" s="54">
@@ -6774,14 +6789,14 @@
         <v>0.476802</v>
       </c>
       <c r="F38" s="56">
-        <f t="shared" si="51"/>
+        <f t="shared" si="55"/>
         <v>2.8080000000000002E-3</v>
       </c>
       <c r="G38" s="54">
         <v>0.78258399999999995</v>
       </c>
       <c r="H38" s="56">
-        <f t="shared" ref="H38:H55" si="52">S38</f>
+        <f t="shared" ref="H38:H55" si="56">S38</f>
         <v>0.497</v>
       </c>
       <c r="I38" s="54">
@@ -6808,14 +6823,14 @@
         <v>0.22198100000000001</v>
       </c>
       <c r="F39" s="56">
-        <f t="shared" si="51"/>
+        <f t="shared" si="55"/>
         <v>0.19489699999999999</v>
       </c>
       <c r="G39" s="54">
         <v>3.1137700000000001</v>
       </c>
       <c r="H39" s="56">
-        <f t="shared" si="52"/>
+        <f t="shared" si="56"/>
         <v>2.3319999999999999</v>
       </c>
       <c r="I39" s="54">
@@ -6842,14 +6857,14 @@
         <v>0.17830199999999999</v>
       </c>
       <c r="F40" s="56">
-        <f t="shared" si="51"/>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
       <c r="G40" s="54">
         <v>0</v>
       </c>
       <c r="H40" s="56">
-        <f t="shared" si="52"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="I40" s="54">
@@ -6877,14 +6892,14 @@
         <v>1.3517459999999999</v>
       </c>
       <c r="F41" s="57">
-        <f t="shared" si="51"/>
+        <f t="shared" si="55"/>
         <v>0.465671</v>
       </c>
       <c r="G41" s="58">
         <v>2.214496</v>
       </c>
       <c r="H41" s="57">
-        <f t="shared" si="52"/>
+        <f t="shared" si="56"/>
         <v>6.3869999999999996</v>
       </c>
       <c r="I41" s="80">
@@ -6894,7 +6909,7 @@
       <c r="K41" s="12"/>
       <c r="L41" s="60"/>
       <c r="M41" s="12"/>
-      <c r="N41" s="158"/>
+      <c r="N41" s="133"/>
       <c r="O41" s="12"/>
       <c r="P41" s="12"/>
       <c r="Q41" s="58">
@@ -6927,7 +6942,7 @@
         <v>6.7660130000000009</v>
       </c>
       <c r="H42" s="56">
-        <f t="shared" si="52"/>
+        <f t="shared" si="56"/>
         <v>11.667999999999999</v>
       </c>
       <c r="I42" s="39">
@@ -6951,12 +6966,12 @@
       <c r="D43" s="56"/>
       <c r="E43" s="39"/>
       <c r="F43" s="56">
-        <f t="shared" ref="F43:F48" si="53">R43</f>
+        <f t="shared" ref="F43:F48" si="57">R43</f>
         <v>0</v>
       </c>
       <c r="G43" s="39"/>
       <c r="H43" s="56">
-        <f t="shared" si="52"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="Q43" s="39"/>
@@ -6974,14 +6989,14 @@
         <v>0.31251600000000002</v>
       </c>
       <c r="F44" s="56">
-        <f t="shared" si="53"/>
+        <f t="shared" si="57"/>
         <v>0.38318600000000003</v>
       </c>
       <c r="G44" s="39">
         <v>2.9940030000000002</v>
       </c>
       <c r="H44" s="56">
-        <f t="shared" si="52"/>
+        <f t="shared" si="56"/>
         <v>3.3149999999999999</v>
       </c>
       <c r="I44" s="39">
@@ -7008,14 +7023,14 @@
         <v>0</v>
       </c>
       <c r="F45" s="56">
-        <f t="shared" si="53"/>
+        <f t="shared" si="57"/>
         <v>8.7378999999999998E-2</v>
       </c>
       <c r="G45" s="39">
         <v>0</v>
       </c>
       <c r="H45" s="56">
-        <f t="shared" si="52"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="I45" s="39">
@@ -7042,14 +7057,14 @@
         <v>0</v>
       </c>
       <c r="F46" s="56">
-        <f t="shared" si="53"/>
+        <f t="shared" si="57"/>
         <v>4.895E-3</v>
       </c>
       <c r="G46" s="39">
         <v>0</v>
       </c>
       <c r="H46" s="56">
-        <f t="shared" si="52"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="I46" s="39">
@@ -7076,14 +7091,14 @@
         <v>0.102697</v>
       </c>
       <c r="F47" s="56">
-        <f t="shared" si="53"/>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="G47" s="39">
         <v>0</v>
       </c>
       <c r="H47" s="56">
-        <f t="shared" si="52"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="I47" s="39">
@@ -7110,14 +7125,14 @@
         <v>0</v>
       </c>
       <c r="F48" s="56">
-        <f t="shared" si="53"/>
+        <f t="shared" si="57"/>
         <v>0.22625000000000001</v>
       </c>
       <c r="G48" s="39">
         <v>0.22625000000000001</v>
       </c>
       <c r="H48" s="56">
-        <f t="shared" si="52"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="I48" s="39">
@@ -7150,7 +7165,7 @@
         <v>0</v>
       </c>
       <c r="H49" s="56">
-        <f t="shared" si="52"/>
+        <f t="shared" si="56"/>
         <v>1.24</v>
       </c>
       <c r="I49" s="39">
@@ -7187,7 +7202,7 @@
         <v>0</v>
       </c>
       <c r="H50" s="56">
-        <f t="shared" si="52"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="I50" s="39">
@@ -7224,7 +7239,7 @@
         <v>0</v>
       </c>
       <c r="H51" s="56">
-        <f t="shared" si="52"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="I51" s="59">
@@ -7234,7 +7249,7 @@
       <c r="K51" s="12"/>
       <c r="L51" s="60"/>
       <c r="M51" s="12"/>
-      <c r="N51" s="158"/>
+      <c r="N51" s="133"/>
       <c r="O51" s="12"/>
       <c r="P51" s="12"/>
       <c r="Q51" s="59">
@@ -7267,7 +7282,7 @@
         <v>3.220253</v>
       </c>
       <c r="H52" s="56">
-        <f t="shared" si="52"/>
+        <f t="shared" si="56"/>
         <v>4.5549999999999997</v>
       </c>
       <c r="I52" s="39">
@@ -7293,7 +7308,7 @@
       <c r="F53" s="56"/>
       <c r="G53" s="39"/>
       <c r="H53" s="56">
-        <f t="shared" si="52"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="Q53" s="39"/>
@@ -7318,7 +7333,7 @@
         <v>3.54576</v>
       </c>
       <c r="H54" s="56">
-        <f t="shared" si="52"/>
+        <f t="shared" si="56"/>
         <v>7.1130000000000004</v>
       </c>
       <c r="I54" s="39">
@@ -7354,7 +7369,7 @@
         <v>6.7660130000000001</v>
       </c>
       <c r="H55" s="56">
-        <f t="shared" si="52"/>
+        <f t="shared" si="56"/>
         <v>11.667999999999999</v>
       </c>
       <c r="I55" s="39">
@@ -7389,35 +7404,35 @@
         <v>143</v>
       </c>
       <c r="D57" s="56">
-        <f t="shared" ref="D57" si="54">D42-D52</f>
+        <f t="shared" ref="D57" si="58">D42-D52</f>
         <v>2.233822</v>
       </c>
       <c r="E57" s="79">
-        <f t="shared" ref="E57:F57" si="55">E42-E52</f>
+        <f t="shared" ref="E57:F57" si="59">E42-E52</f>
         <v>2.625874</v>
       </c>
       <c r="F57" s="56">
-        <f t="shared" si="55"/>
+        <f t="shared" si="59"/>
         <v>0.52937599999999996</v>
       </c>
       <c r="G57" s="79">
-        <f t="shared" ref="G57:H57" si="56">G42-G52</f>
+        <f t="shared" ref="G57:H57" si="60">G42-G52</f>
         <v>3.5457600000000009</v>
       </c>
       <c r="H57" s="56">
-        <f t="shared" si="56"/>
+        <f t="shared" si="60"/>
         <v>7.1129999999999995</v>
       </c>
       <c r="I57" s="79">
-        <f t="shared" ref="I57" si="57">I42-I52</f>
+        <f t="shared" ref="I57" si="61">I42-I52</f>
         <v>8.4660000000000011</v>
       </c>
       <c r="Q57" s="79">
-        <f t="shared" ref="Q57:R57" si="58">Q42-Q52</f>
+        <f t="shared" ref="Q57:R57" si="62">Q42-Q52</f>
         <v>2.233822</v>
       </c>
       <c r="R57" s="79">
-        <f t="shared" si="58"/>
+        <f t="shared" si="62"/>
         <v>0.52937599999999996</v>
       </c>
       <c r="S57" s="79">
@@ -7430,35 +7445,35 @@
         <v>144</v>
       </c>
       <c r="D58" s="56">
-        <f t="shared" ref="D58:H58" si="59">D57/D21</f>
+        <f t="shared" ref="D58:H58" si="63">D57/D21</f>
         <v>9.2774396784636708E-3</v>
       </c>
       <c r="E58" s="39">
-        <f t="shared" ref="E58" si="60">E57/E21</f>
+        <f t="shared" ref="E58" si="64">E57/E21</f>
         <v>7.6424304594443658E-3</v>
       </c>
       <c r="F58" s="56">
-        <f t="shared" si="59"/>
+        <f t="shared" si="63"/>
         <v>1.0223126865988698E-3</v>
       </c>
       <c r="G58" s="39">
-        <f t="shared" si="59"/>
+        <f t="shared" si="63"/>
         <v>5.3359111491456885E-3</v>
       </c>
       <c r="H58" s="56">
-        <f t="shared" si="59"/>
+        <f t="shared" si="63"/>
         <v>1.0006302296399251E-2</v>
       </c>
       <c r="I58" s="39">
-        <f t="shared" ref="I58" si="61">I57/I21</f>
+        <f t="shared" ref="I58" si="65">I57/I21</f>
         <v>1.0932052374680408E-2</v>
       </c>
       <c r="Q58" s="39">
-        <f t="shared" ref="Q58:R58" si="62">Q57/Q21</f>
+        <f t="shared" ref="Q58:R58" si="66">Q57/Q21</f>
         <v>9.2774396784636708E-3</v>
       </c>
       <c r="R58" s="39">
-        <f t="shared" si="62"/>
+        <f t="shared" si="66"/>
         <v>1.0223126865988698E-3</v>
       </c>
       <c r="S58" s="39">
@@ -7571,27 +7586,27 @@
         <v>161</v>
       </c>
       <c r="D69" s="34">
-        <f t="shared" ref="D69:I69" si="63">(D15+C15)/(D42-SUM(D49:D51))</f>
+        <f t="shared" ref="D69:I69" si="67">(D15+C15)/(D42-SUM(D49:D51))</f>
         <v>-0.94713013945390168</v>
       </c>
       <c r="E69" s="36">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>-0.82098736405765438</v>
       </c>
       <c r="F69" s="34">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>-3.0525825165747973</v>
       </c>
       <c r="G69" s="36">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>-0.39580630424446428</v>
       </c>
       <c r="H69" s="34">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>0.19620253164556961</v>
       </c>
       <c r="I69" s="36">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>0.17112763138524958</v>
       </c>
       <c r="S69" s="36">
@@ -7622,6 +7637,81 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09CE0562-FC62-4793-9141-96B57A1A963D}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="99"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="101" t="s">
+        <v>242</v>
+      </c>
+      <c r="C1" s="101" t="s">
+        <v>244</v>
+      </c>
+      <c r="D1" s="101" t="s">
+        <v>245</v>
+      </c>
+      <c r="E1" s="101" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="160" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="160" t="s">
+        <v>249</v>
+      </c>
+      <c r="B3" s="160">
+        <v>2342000</v>
+      </c>
+      <c r="D3" s="160">
+        <v>572000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="160" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="160" t="s">
+        <v>250</v>
+      </c>
+      <c r="B4" s="160">
+        <v>122000</v>
+      </c>
+      <c r="D4" s="160">
+        <v>309000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="161" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="161" t="s">
+        <v>251</v>
+      </c>
+      <c r="D6" s="161">
+        <f>D3/B3-1</f>
+        <v>-0.75576430401366357</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="161" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="161" t="s">
+        <v>252</v>
+      </c>
+      <c r="D7" s="161">
+        <f>D4/B4-1</f>
+        <v>1.5327868852459017</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B616A8F7-A0BD-4E7F-9020-9AE5BBA9C9F8}">
   <dimension ref="B1:D16"/>
   <sheetViews>
@@ -7637,11 +7727,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="145" t="s">
+      <c r="B1" s="159" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="145"/>
-      <c r="D1" s="145"/>
+      <c r="C1" s="159"/>
+      <c r="D1" s="159"/>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C2" s="21">
@@ -7814,7 +7904,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C07E9ED6-1590-4E51-9AEA-DA97942BD76A}">
   <dimension ref="A1:E28"/>
   <sheetViews>

</xml_diff>

<commit_message>
£MHC & £TRLS major news events
</commit_message>
<xml_diff>
--- a/£MHC.xlsx
+++ b/£MHC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\My Drive\Stocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C5B2D8-FEAE-4475-AFB2-7B36604A2DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7177EFA-CFA5-4AA5-9355-ACDDFA4CBB0B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E461C7AA-D693-45DC-846F-4B1D3C8E259B}"/>
   </bookViews>
@@ -24,21 +24,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="254">
   <si>
     <t>Stock Snapshot</t>
   </si>
@@ -797,6 +788,9 @@
   </si>
   <si>
     <t>Other Y/Y</t>
+  </si>
+  <si>
+    <t>MHC receive regulatory approval for Phlebotomy Testing in UK &amp; EU</t>
   </si>
 </sst>
 </file>
@@ -1173,7 +1167,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="162">
+  <cellXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1275,9 +1269,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1321,9 +1312,6 @@
     </xf>
     <xf numFmtId="17" fontId="2" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1381,52 +1369,21 @@
     <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="15" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1453,11 +1410,49 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Accent3" xfId="1" builtinId="38"/>
@@ -1975,8 +1970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A865B090-C0E4-4B85-AA22-AACD646D3083}">
   <dimension ref="A1:AC105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2004,11 +1999,11 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="J2" s="140" t="s">
+      <c r="J2" s="137" t="s">
         <v>148</v>
       </c>
-      <c r="K2" s="136"/>
-      <c r="L2" s="137"/>
+      <c r="K2" s="138"/>
+      <c r="L2" s="139"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -2020,13 +2015,13 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="J3" s="82" t="s">
+      <c r="J3" s="81" t="s">
         <v>149</v>
       </c>
-      <c r="K3" s="151" t="s">
+      <c r="K3" s="140" t="s">
         <v>153</v>
       </c>
-      <c r="L3" s="152"/>
+      <c r="L3" s="141"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
@@ -2036,29 +2031,29 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="J4" s="82" t="s">
+      <c r="J4" s="81" t="s">
         <v>150</v>
       </c>
-      <c r="K4" s="151"/>
-      <c r="L4" s="152"/>
+      <c r="K4" s="140"/>
+      <c r="L4" s="141"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="140" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="136"/>
-      <c r="D5" s="137"/>
+      <c r="B5" s="137" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="138"/>
+      <c r="D5" s="139"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="J5" s="82" t="s">
+      <c r="J5" s="81" t="s">
         <v>154</v>
       </c>
-      <c r="K5" s="81" t="s">
+      <c r="K5" s="80" t="s">
         <v>90</v>
       </c>
-      <c r="L5" s="95">
+      <c r="L5" s="94">
         <v>44825</v>
       </c>
     </row>
@@ -2068,19 +2063,19 @@
         <v>1</v>
       </c>
       <c r="C6" s="65">
-        <v>0.12620000000000001</v>
+        <v>0.17</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="J6" s="83" t="s">
+      <c r="J6" s="82" t="s">
         <v>151</v>
       </c>
-      <c r="K6" s="153" t="s">
+      <c r="K6" s="142" t="s">
         <v>152</v>
       </c>
-      <c r="L6" s="154"/>
+      <c r="L6" s="143"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
@@ -2105,7 +2100,7 @@
       </c>
       <c r="C8" s="6">
         <f>C6*C7</f>
-        <v>6.5631572</v>
+        <v>8.8410200000000003</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="1"/>
@@ -2124,17 +2119,17 @@
         <v>244</v>
       </c>
       <c r="E9" s="1"/>
-      <c r="F9" s="140" t="s">
+      <c r="F9" s="137" t="s">
         <v>59</v>
       </c>
-      <c r="G9" s="136"/>
-      <c r="H9" s="136"/>
-      <c r="I9" s="136"/>
-      <c r="J9" s="136"/>
-      <c r="K9" s="136"/>
-      <c r="L9" s="136"/>
-      <c r="M9" s="136"/>
-      <c r="N9" s="137"/>
+      <c r="G9" s="138"/>
+      <c r="H9" s="138"/>
+      <c r="I9" s="138"/>
+      <c r="J9" s="138"/>
+      <c r="K9" s="138"/>
+      <c r="L9" s="138"/>
+      <c r="M9" s="138"/>
+      <c r="N9" s="139"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
@@ -2148,18 +2143,18 @@
         <v>244</v>
       </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="114">
+      <c r="F10" s="112">
         <v>43770</v>
       </c>
-      <c r="G10" s="22" t="s">
+      <c r="G10" s="160" t="s">
         <v>57</v>
       </c>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
+      <c r="H10" s="160"/>
+      <c r="I10" s="160"/>
+      <c r="J10" s="160"/>
+      <c r="K10" s="160"/>
+      <c r="L10" s="160"/>
+      <c r="M10" s="160"/>
       <c r="N10" s="23"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -2173,18 +2168,18 @@
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="114">
+      <c r="F11" s="112">
         <v>43891</v>
       </c>
-      <c r="G11" s="22" t="s">
+      <c r="G11" s="160" t="s">
         <v>66</v>
       </c>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
+      <c r="H11" s="160"/>
+      <c r="I11" s="160"/>
+      <c r="J11" s="160"/>
+      <c r="K11" s="160"/>
+      <c r="L11" s="160"/>
+      <c r="M11" s="160"/>
       <c r="N11" s="23"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -2194,22 +2189,22 @@
       </c>
       <c r="C12" s="10">
         <f>C8-C9+C10</f>
-        <v>-1.1868428</v>
+        <v>1.0910200000000003</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="114">
+      <c r="F12" s="112">
         <v>44166</v>
       </c>
-      <c r="G12" s="22" t="s">
+      <c r="G12" s="160" t="s">
         <v>58</v>
       </c>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="22"/>
+      <c r="H12" s="160"/>
+      <c r="I12" s="160"/>
+      <c r="J12" s="160"/>
+      <c r="K12" s="160"/>
+      <c r="L12" s="160"/>
+      <c r="M12" s="160"/>
       <c r="N12" s="23"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -2218,18 +2213,18 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="114">
+      <c r="F13" s="112">
         <v>44166</v>
       </c>
-      <c r="G13" s="22" t="s">
+      <c r="G13" s="160" t="s">
         <v>133</v>
       </c>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="22"/>
+      <c r="H13" s="160"/>
+      <c r="I13" s="160"/>
+      <c r="J13" s="160"/>
+      <c r="K13" s="160"/>
+      <c r="L13" s="160"/>
+      <c r="M13" s="160"/>
       <c r="N13" s="23"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -2238,40 +2233,40 @@
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="114">
+      <c r="F14" s="112">
         <v>44197</v>
       </c>
-      <c r="G14" s="22" t="s">
+      <c r="G14" s="160" t="s">
         <v>64</v>
       </c>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="22"/>
+      <c r="H14" s="160"/>
+      <c r="I14" s="160"/>
+      <c r="J14" s="160"/>
+      <c r="K14" s="160"/>
+      <c r="L14" s="160"/>
+      <c r="M14" s="160"/>
       <c r="N14" s="23"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="135" t="s">
+      <c r="B15" s="148" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="136"/>
-      <c r="D15" s="137"/>
+      <c r="C15" s="138"/>
+      <c r="D15" s="139"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="114">
+      <c r="F15" s="112">
         <v>44287</v>
       </c>
-      <c r="G15" s="22" t="s">
+      <c r="G15" s="160" t="s">
         <v>98</v>
       </c>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="22"/>
-      <c r="L15" s="22"/>
-      <c r="M15" s="22"/>
+      <c r="H15" s="160"/>
+      <c r="I15" s="160"/>
+      <c r="J15" s="160"/>
+      <c r="K15" s="160"/>
+      <c r="L15" s="160"/>
+      <c r="M15" s="160"/>
       <c r="N15" s="23"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -2279,219 +2274,219 @@
       <c r="B16" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="139" t="s">
+      <c r="C16" s="149" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="138"/>
+      <c r="D16" s="150"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="114">
+      <c r="F16" s="112">
         <v>44317</v>
       </c>
-      <c r="G16" s="22" t="s">
+      <c r="G16" s="160" t="s">
         <v>99</v>
       </c>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
-      <c r="L16" s="22"/>
-      <c r="M16" s="22"/>
+      <c r="H16" s="160"/>
+      <c r="I16" s="160"/>
+      <c r="J16" s="160"/>
+      <c r="K16" s="160"/>
+      <c r="L16" s="160"/>
+      <c r="M16" s="160"/>
       <c r="N16" s="23"/>
     </row>
     <row r="17" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B17" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="139" t="s">
+      <c r="C17" s="149" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="138"/>
-      <c r="F17" s="114">
+      <c r="D17" s="150"/>
+      <c r="F17" s="112">
         <v>44348</v>
       </c>
-      <c r="G17" s="22" t="s">
+      <c r="G17" s="160" t="s">
         <v>100</v>
       </c>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="22"/>
-      <c r="M17" s="22"/>
+      <c r="H17" s="160"/>
+      <c r="I17" s="160"/>
+      <c r="J17" s="160"/>
+      <c r="K17" s="160"/>
+      <c r="L17" s="160"/>
+      <c r="M17" s="160"/>
       <c r="N17" s="23"/>
     </row>
     <row r="18" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B18" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="138"/>
-      <c r="D18" s="138"/>
-      <c r="F18" s="114">
+      <c r="C18" s="150"/>
+      <c r="D18" s="150"/>
+      <c r="F18" s="112">
         <v>44409</v>
       </c>
-      <c r="G18" s="22" t="s">
+      <c r="G18" s="160" t="s">
         <v>101</v>
       </c>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
+      <c r="H18" s="160"/>
+      <c r="I18" s="160"/>
+      <c r="J18" s="160"/>
+      <c r="K18" s="160"/>
+      <c r="L18" s="160"/>
+      <c r="M18" s="160"/>
       <c r="N18" s="23"/>
     </row>
     <row r="19" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B19" s="18"/>
-      <c r="C19" s="138"/>
-      <c r="D19" s="138"/>
-      <c r="F19" s="114">
+      <c r="C19" s="150"/>
+      <c r="D19" s="150"/>
+      <c r="F19" s="112">
         <v>44440</v>
       </c>
-      <c r="G19" s="22" t="s">
+      <c r="G19" s="160" t="s">
         <v>102</v>
       </c>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
+      <c r="H19" s="160"/>
+      <c r="I19" s="160"/>
+      <c r="J19" s="160"/>
+      <c r="K19" s="160"/>
+      <c r="L19" s="160"/>
+      <c r="M19" s="160"/>
       <c r="N19" s="23"/>
     </row>
     <row r="20" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B20" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="139" t="s">
+      <c r="C20" s="149" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="138"/>
-      <c r="F20" s="114">
+      <c r="D20" s="150"/>
+      <c r="F20" s="112">
         <v>44501</v>
       </c>
-      <c r="G20" s="22" t="s">
+      <c r="G20" s="160" t="s">
         <v>147</v>
       </c>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
-      <c r="K20" s="22"/>
-      <c r="L20" s="22"/>
-      <c r="M20" s="22"/>
+      <c r="H20" s="160"/>
+      <c r="I20" s="160"/>
+      <c r="J20" s="160"/>
+      <c r="K20" s="160"/>
+      <c r="L20" s="160"/>
+      <c r="M20" s="160"/>
       <c r="N20" s="23"/>
     </row>
     <row r="21" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B21" s="18"/>
-      <c r="C21" s="138"/>
-      <c r="D21" s="138"/>
-      <c r="F21" s="114">
+      <c r="C21" s="150"/>
+      <c r="D21" s="150"/>
+      <c r="F21" s="112">
         <v>44652</v>
       </c>
-      <c r="G21" s="22" t="s">
+      <c r="G21" s="160" t="s">
         <v>146</v>
       </c>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="22"/>
-      <c r="L21" s="22"/>
-      <c r="M21" s="22"/>
+      <c r="H21" s="160"/>
+      <c r="I21" s="160"/>
+      <c r="J21" s="160"/>
+      <c r="K21" s="160"/>
+      <c r="L21" s="160"/>
+      <c r="M21" s="160"/>
       <c r="N21" s="23"/>
     </row>
     <row r="22" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B22" s="19"/>
-      <c r="C22" s="145"/>
-      <c r="D22" s="144"/>
-      <c r="F22" s="114">
+      <c r="C22" s="151"/>
+      <c r="D22" s="152"/>
+      <c r="F22" s="112">
         <v>44726</v>
       </c>
-      <c r="G22" s="22" t="s">
+      <c r="G22" s="160" t="s">
         <v>132</v>
       </c>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="22"/>
-      <c r="L22" s="22"/>
-      <c r="M22" s="22"/>
+      <c r="H22" s="160"/>
+      <c r="I22" s="160"/>
+      <c r="J22" s="160"/>
+      <c r="K22" s="160"/>
+      <c r="L22" s="160"/>
+      <c r="M22" s="160"/>
       <c r="N22" s="23"/>
     </row>
     <row r="23" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="F23" s="114"/>
-      <c r="G23" s="77" t="s">
+      <c r="F23" s="112"/>
+      <c r="G23" s="161" t="s">
         <v>134</v>
       </c>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="22"/>
-      <c r="L23" s="22"/>
-      <c r="M23" s="22"/>
+      <c r="H23" s="160"/>
+      <c r="I23" s="160"/>
+      <c r="J23" s="160"/>
+      <c r="K23" s="160"/>
+      <c r="L23" s="160"/>
+      <c r="M23" s="160"/>
       <c r="N23" s="23"/>
     </row>
     <row r="24" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B24" s="140" t="s">
+      <c r="B24" s="137" t="s">
         <v>237</v>
       </c>
-      <c r="C24" s="136"/>
-      <c r="D24" s="137"/>
-      <c r="F24" s="114">
+      <c r="C24" s="138"/>
+      <c r="D24" s="139"/>
+      <c r="F24" s="112">
         <v>44743</v>
       </c>
-      <c r="G24" s="77" t="s">
+      <c r="G24" s="161" t="s">
         <v>136</v>
       </c>
-      <c r="H24" s="22"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="22"/>
-      <c r="K24" s="22"/>
-      <c r="L24" s="22"/>
-      <c r="M24" s="22"/>
+      <c r="H24" s="160"/>
+      <c r="I24" s="160"/>
+      <c r="J24" s="160"/>
+      <c r="K24" s="160"/>
+      <c r="L24" s="160"/>
+      <c r="M24" s="160"/>
       <c r="N24" s="23"/>
-      <c r="P24" s="140" t="s">
+      <c r="P24" s="137" t="s">
         <v>155</v>
       </c>
-      <c r="Q24" s="136"/>
-      <c r="R24" s="137"/>
-      <c r="W24" s="140" t="s">
+      <c r="Q24" s="138"/>
+      <c r="R24" s="139"/>
+      <c r="W24" s="137" t="s">
         <v>163</v>
       </c>
-      <c r="X24" s="136"/>
-      <c r="Y24" s="136"/>
-      <c r="Z24" s="136"/>
-      <c r="AA24" s="136"/>
-      <c r="AB24" s="136"/>
-      <c r="AC24" s="137"/>
+      <c r="X24" s="138"/>
+      <c r="Y24" s="138"/>
+      <c r="Z24" s="138"/>
+      <c r="AA24" s="138"/>
+      <c r="AB24" s="138"/>
+      <c r="AC24" s="139"/>
     </row>
     <row r="25" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B25" s="120">
+      <c r="B25" s="118">
         <v>45047</v>
       </c>
-      <c r="C25" s="143" t="s">
+      <c r="C25" s="158" t="s">
         <v>238</v>
       </c>
-      <c r="D25" s="144"/>
-      <c r="F25" s="114">
+      <c r="D25" s="152"/>
+      <c r="F25" s="112">
         <v>44743</v>
       </c>
-      <c r="G25" s="22" t="s">
+      <c r="G25" s="160" t="s">
         <v>139</v>
       </c>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="22"/>
-      <c r="K25" s="22"/>
-      <c r="L25" s="22"/>
-      <c r="M25" s="22"/>
+      <c r="H25" s="160"/>
+      <c r="I25" s="160"/>
+      <c r="J25" s="160"/>
+      <c r="K25" s="160"/>
+      <c r="L25" s="160"/>
+      <c r="M25" s="160"/>
       <c r="N25" s="23"/>
-      <c r="P25" s="82" t="s">
+      <c r="P25" s="81" t="s">
         <v>156</v>
       </c>
-      <c r="Q25" s="146" t="s">
+      <c r="Q25" s="153" t="s">
         <v>152</v>
       </c>
-      <c r="R25" s="147"/>
-      <c r="W25" s="112" t="s">
+      <c r="R25" s="154"/>
+      <c r="W25" s="110" t="s">
         <v>164</v>
       </c>
       <c r="X25" s="22"/>
@@ -2502,27 +2497,27 @@
       <c r="AC25" s="23"/>
     </row>
     <row r="26" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="F26" s="114">
+      <c r="F26" s="112">
         <v>44774</v>
       </c>
-      <c r="G26" s="22" t="s">
+      <c r="G26" s="160" t="s">
         <v>138</v>
       </c>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="22"/>
-      <c r="K26" s="22"/>
-      <c r="L26" s="22"/>
-      <c r="M26" s="22"/>
+      <c r="H26" s="160"/>
+      <c r="I26" s="160"/>
+      <c r="J26" s="160"/>
+      <c r="K26" s="160"/>
+      <c r="L26" s="160"/>
+      <c r="M26" s="160"/>
       <c r="N26" s="23"/>
-      <c r="P26" s="82" t="s">
+      <c r="P26" s="81" t="s">
         <v>157</v>
       </c>
-      <c r="Q26" s="146" t="s">
+      <c r="Q26" s="153" t="s">
         <v>152</v>
       </c>
-      <c r="R26" s="147"/>
-      <c r="W26" s="112" t="s">
+      <c r="R26" s="154"/>
+      <c r="W26" s="110" t="s">
         <v>169</v>
       </c>
       <c r="X26" s="22"/>
@@ -2533,28 +2528,28 @@
       <c r="AC26" s="23"/>
     </row>
     <row r="27" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B27" s="135" t="s">
+      <c r="B27" s="148" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="136"/>
-      <c r="D27" s="137"/>
-      <c r="F27" s="114">
+      <c r="C27" s="138"/>
+      <c r="D27" s="139"/>
+      <c r="F27" s="112">
         <v>44835</v>
       </c>
-      <c r="G27" s="98" t="s">
+      <c r="G27" s="162" t="s">
         <v>158</v>
       </c>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
-      <c r="K27" s="22"/>
-      <c r="L27" s="22"/>
-      <c r="M27" s="22"/>
+      <c r="H27" s="160"/>
+      <c r="I27" s="160"/>
+      <c r="J27" s="160"/>
+      <c r="K27" s="160"/>
+      <c r="L27" s="160"/>
+      <c r="M27" s="160"/>
       <c r="N27" s="23"/>
-      <c r="P27" s="83"/>
-      <c r="Q27" s="148"/>
-      <c r="R27" s="149"/>
-      <c r="W27" s="112" t="s">
+      <c r="P27" s="82"/>
+      <c r="Q27" s="155"/>
+      <c r="R27" s="136"/>
+      <c r="W27" s="110" t="s">
         <v>165</v>
       </c>
       <c r="X27" s="22"/>
@@ -2568,24 +2563,24 @@
       <c r="B28" s="26">
         <v>43922</v>
       </c>
-      <c r="C28" s="139" t="s">
+      <c r="C28" s="149" t="s">
         <v>61</v>
       </c>
-      <c r="D28" s="138"/>
-      <c r="F28" s="114">
+      <c r="D28" s="150"/>
+      <c r="F28" s="112">
         <v>45047</v>
       </c>
-      <c r="G28" s="98" t="s">
+      <c r="G28" s="162" t="s">
         <v>240</v>
       </c>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22"/>
-      <c r="K28" s="22"/>
-      <c r="L28" s="22"/>
-      <c r="M28" s="22"/>
+      <c r="H28" s="160"/>
+      <c r="I28" s="160"/>
+      <c r="J28" s="160"/>
+      <c r="K28" s="160"/>
+      <c r="L28" s="160"/>
+      <c r="M28" s="160"/>
       <c r="N28" s="23"/>
-      <c r="W28" s="112" t="s">
+      <c r="W28" s="110" t="s">
         <v>166</v>
       </c>
       <c r="X28" s="22"/>
@@ -2599,24 +2594,24 @@
       <c r="B29" s="27">
         <v>44228</v>
       </c>
-      <c r="C29" s="145" t="s">
+      <c r="C29" s="151" t="s">
         <v>65</v>
       </c>
-      <c r="D29" s="144"/>
-      <c r="F29" s="114">
+      <c r="D29" s="152"/>
+      <c r="F29" s="112">
         <v>45047</v>
       </c>
-      <c r="G29" s="98" t="s">
+      <c r="G29" s="162" t="s">
         <v>239</v>
       </c>
-      <c r="H29" s="22"/>
-      <c r="I29" s="22"/>
-      <c r="J29" s="22"/>
-      <c r="K29" s="22"/>
-      <c r="L29" s="22"/>
-      <c r="M29" s="22"/>
+      <c r="H29" s="160"/>
+      <c r="I29" s="160"/>
+      <c r="J29" s="160"/>
+      <c r="K29" s="160"/>
+      <c r="L29" s="160"/>
+      <c r="M29" s="160"/>
       <c r="N29" s="23"/>
-      <c r="W29" s="112" t="s">
+      <c r="W29" s="110" t="s">
         <v>167</v>
       </c>
       <c r="X29" s="22"/>
@@ -2627,20 +2622,20 @@
       <c r="AC29" s="23"/>
     </row>
     <row r="30" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="F30" s="114">
+      <c r="F30" s="112">
         <v>45108</v>
       </c>
-      <c r="G30" s="98" t="s">
+      <c r="G30" s="162" t="s">
         <v>241</v>
       </c>
-      <c r="H30" s="22"/>
-      <c r="I30" s="22"/>
-      <c r="J30" s="22"/>
-      <c r="K30" s="22"/>
-      <c r="L30" s="22"/>
-      <c r="M30" s="22"/>
+      <c r="H30" s="160"/>
+      <c r="I30" s="160"/>
+      <c r="J30" s="160"/>
+      <c r="K30" s="160"/>
+      <c r="L30" s="160"/>
+      <c r="M30" s="160"/>
       <c r="N30" s="23"/>
-      <c r="W30" s="112" t="s">
+      <c r="W30" s="110" t="s">
         <v>168</v>
       </c>
       <c r="X30" s="22"/>
@@ -2651,25 +2646,25 @@
       <c r="AC30" s="23"/>
     </row>
     <row r="31" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B31" s="135" t="s">
+      <c r="B31" s="148" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="136"/>
-      <c r="D31" s="137"/>
-      <c r="F31" s="115">
+      <c r="C31" s="138"/>
+      <c r="D31" s="139"/>
+      <c r="F31" s="112">
         <v>45292</v>
       </c>
-      <c r="G31" s="78" t="s">
+      <c r="G31" s="162" t="s">
         <v>243</v>
       </c>
-      <c r="H31" s="24"/>
-      <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
-      <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
-      <c r="M31" s="24"/>
-      <c r="N31" s="25"/>
-      <c r="W31" s="112" t="s">
+      <c r="H31" s="160"/>
+      <c r="I31" s="160"/>
+      <c r="J31" s="160"/>
+      <c r="K31" s="160"/>
+      <c r="L31" s="160"/>
+      <c r="M31" s="160"/>
+      <c r="N31" s="23"/>
+      <c r="W31" s="110" t="s">
         <v>170</v>
       </c>
       <c r="X31" s="22"/>
@@ -2683,11 +2678,24 @@
       <c r="B32" s="26">
         <v>44136</v>
       </c>
-      <c r="C32" s="139" t="s">
+      <c r="C32" s="149" t="s">
         <v>63</v>
       </c>
-      <c r="D32" s="138"/>
-      <c r="W32" s="117" t="s">
+      <c r="D32" s="150"/>
+      <c r="F32" s="113">
+        <v>45658</v>
+      </c>
+      <c r="G32" s="77" t="s">
+        <v>253</v>
+      </c>
+      <c r="H32" s="24"/>
+      <c r="I32" s="24"/>
+      <c r="J32" s="24"/>
+      <c r="K32" s="24"/>
+      <c r="L32" s="24"/>
+      <c r="M32" s="24"/>
+      <c r="N32" s="25"/>
+      <c r="W32" s="115" t="s">
         <v>171</v>
       </c>
       <c r="X32" s="22"/>
@@ -2701,11 +2709,11 @@
       <c r="B33" s="28">
         <v>44348</v>
       </c>
-      <c r="C33" s="145" t="s">
+      <c r="C33" s="151" t="s">
         <v>67</v>
       </c>
-      <c r="D33" s="144"/>
-      <c r="W33" s="112" t="s">
+      <c r="D33" s="152"/>
+      <c r="W33" s="110" t="s">
         <v>172</v>
       </c>
       <c r="X33" s="22"/>
@@ -2716,7 +2724,7 @@
       <c r="AC33" s="23"/>
     </row>
     <row r="34" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="W34" s="112" t="s">
+      <c r="W34" s="110" t="s">
         <v>173</v>
       </c>
       <c r="X34" s="22"/>
@@ -2727,7 +2735,7 @@
       <c r="AC34" s="23"/>
     </row>
     <row r="35" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="W35" s="117" t="s">
+      <c r="W35" s="115" t="s">
         <v>174</v>
       </c>
       <c r="X35" s="22"/>
@@ -2738,24 +2746,24 @@
       <c r="AC35" s="23"/>
     </row>
     <row r="36" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B36" s="140" t="s">
+      <c r="B36" s="137" t="s">
         <v>140</v>
       </c>
-      <c r="C36" s="136"/>
-      <c r="D36" s="137"/>
-      <c r="F36" s="140" t="s">
+      <c r="C36" s="138"/>
+      <c r="D36" s="139"/>
+      <c r="F36" s="137" t="s">
         <v>103</v>
       </c>
-      <c r="G36" s="136"/>
-      <c r="H36" s="136"/>
-      <c r="I36" s="136"/>
-      <c r="J36" s="136"/>
-      <c r="K36" s="136"/>
-      <c r="L36" s="136"/>
-      <c r="M36" s="136"/>
-      <c r="N36" s="136"/>
-      <c r="O36" s="137"/>
-      <c r="W36" s="112" t="s">
+      <c r="G36" s="138"/>
+      <c r="H36" s="138"/>
+      <c r="I36" s="138"/>
+      <c r="J36" s="138"/>
+      <c r="K36" s="138"/>
+      <c r="L36" s="138"/>
+      <c r="M36" s="138"/>
+      <c r="N36" s="138"/>
+      <c r="O36" s="139"/>
+      <c r="W36" s="110" t="s">
         <v>175</v>
       </c>
       <c r="X36" s="22"/>
@@ -2766,18 +2774,18 @@
       <c r="AC36" s="23"/>
     </row>
     <row r="37" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B37" s="96" t="s">
+      <c r="B37" s="95" t="s">
         <v>141</v>
       </c>
-      <c r="C37" s="141">
+      <c r="C37" s="156">
         <f>C6/SUM('Financial Model'!H20:I20)</f>
-        <v>39.329321190103592</v>
-      </c>
-      <c r="D37" s="142"/>
-      <c r="F37" s="155" t="s">
+        <v>52.979275771137964</v>
+      </c>
+      <c r="D37" s="157"/>
+      <c r="F37" s="144" t="s">
         <v>104</v>
       </c>
-      <c r="G37" s="156"/>
+      <c r="G37" s="145"/>
       <c r="H37" s="22" t="s">
         <v>108</v>
       </c>
@@ -2788,7 +2796,7 @@
       <c r="M37" s="22"/>
       <c r="N37" s="22"/>
       <c r="O37" s="23"/>
-      <c r="W37" s="117" t="s">
+      <c r="W37" s="115" t="s">
         <v>176</v>
       </c>
       <c r="X37" s="22"/>
@@ -2799,18 +2807,18 @@
       <c r="AC37" s="23"/>
     </row>
     <row r="38" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B38" s="96" t="s">
+      <c r="B38" s="95" t="s">
         <v>142</v>
       </c>
-      <c r="C38" s="141">
+      <c r="C38" s="156">
         <f>C6/'Financial Model'!I58</f>
-        <v>11.54403543586109</v>
-      </c>
-      <c r="D38" s="142"/>
-      <c r="F38" s="155" t="s">
+        <v>15.550602409638554</v>
+      </c>
+      <c r="D38" s="157"/>
+      <c r="F38" s="144" t="s">
         <v>105</v>
       </c>
-      <c r="G38" s="156"/>
+      <c r="G38" s="145"/>
       <c r="H38" s="22" t="s">
         <v>109</v>
       </c>
@@ -2821,7 +2829,7 @@
       <c r="M38" s="22"/>
       <c r="N38" s="22"/>
       <c r="O38" s="23"/>
-      <c r="W38" s="117" t="s">
+      <c r="W38" s="115" t="s">
         <v>177</v>
       </c>
       <c r="X38" s="22"/>
@@ -2832,18 +2840,18 @@
       <c r="AC38" s="23"/>
     </row>
     <row r="39" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B39" s="96" t="s">
+      <c r="B39" s="95" t="s">
         <v>159</v>
       </c>
-      <c r="C39" s="141">
+      <c r="C39" s="156">
         <f>C8/SUM('Financial Model'!H4:I4)</f>
-        <v>0.28617767052246557</v>
-      </c>
-      <c r="D39" s="142"/>
-      <c r="F39" s="157" t="s">
+        <v>0.38550082400015173</v>
+      </c>
+      <c r="D39" s="157"/>
+      <c r="F39" s="146" t="s">
         <v>106</v>
       </c>
-      <c r="G39" s="158"/>
+      <c r="G39" s="147"/>
       <c r="H39" s="24" t="s">
         <v>135</v>
       </c>
@@ -2857,7 +2865,7 @@
       <c r="P39" s="74" t="s">
         <v>131</v>
       </c>
-      <c r="W39" s="112" t="s">
+      <c r="W39" s="110" t="s">
         <v>178</v>
       </c>
       <c r="X39" s="22"/>
@@ -2868,15 +2876,15 @@
       <c r="AC39" s="23"/>
     </row>
     <row r="40" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B40" s="96" t="s">
+      <c r="B40" s="95" t="s">
         <v>160</v>
       </c>
-      <c r="C40" s="141">
+      <c r="C40" s="156">
         <f>C12/SUM('Financial Model'!H4:I4)</f>
-        <v>-5.1750689101330759E-2</v>
-      </c>
-      <c r="D40" s="142"/>
-      <c r="W40" s="118" t="s">
+        <v>4.7572464376355407E-2</v>
+      </c>
+      <c r="D40" s="157"/>
+      <c r="W40" s="116" t="s">
         <v>179</v>
       </c>
       <c r="X40" s="22"/>
@@ -2887,15 +2895,15 @@
       <c r="AC40" s="23"/>
     </row>
     <row r="41" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B41" s="96" t="s">
+      <c r="B41" s="95" t="s">
         <v>145</v>
       </c>
-      <c r="C41" s="141">
+      <c r="C41" s="156">
         <f>C12/SUM('Financial Model'!H19:I19)</f>
-        <v>-0.52015223589902682</v>
-      </c>
-      <c r="D41" s="142"/>
-      <c r="W41" s="112"/>
+        <v>0.47815640993951047</v>
+      </c>
+      <c r="D41" s="157"/>
+      <c r="W41" s="110"/>
       <c r="X41" s="22"/>
       <c r="Y41" s="22"/>
       <c r="Z41" s="22"/>
@@ -2904,15 +2912,15 @@
       <c r="AC41" s="23"/>
     </row>
     <row r="42" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B42" s="97" t="s">
+      <c r="B42" s="96" t="s">
         <v>161</v>
       </c>
-      <c r="C42" s="150">
+      <c r="C42" s="135">
         <f>'Financial Model'!I69</f>
         <v>0.17112763138524958</v>
       </c>
-      <c r="D42" s="149"/>
-      <c r="W42" s="119" t="s">
+      <c r="D42" s="136"/>
+      <c r="W42" s="117" t="s">
         <v>180</v>
       </c>
       <c r="X42" s="22"/>
@@ -2923,7 +2931,7 @@
       <c r="AC42" s="23"/>
     </row>
     <row r="43" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="W43" s="112" t="s">
+      <c r="W43" s="110" t="s">
         <v>181</v>
       </c>
       <c r="X43" s="22"/>
@@ -2934,7 +2942,7 @@
       <c r="AC43" s="23"/>
     </row>
     <row r="44" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="W44" s="112" t="s">
+      <c r="W44" s="110" t="s">
         <v>182</v>
       </c>
       <c r="X44" s="22"/>
@@ -2945,7 +2953,7 @@
       <c r="AC44" s="23"/>
     </row>
     <row r="45" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="W45" s="112" t="s">
+      <c r="W45" s="110" t="s">
         <v>183</v>
       </c>
       <c r="X45" s="22"/>
@@ -2956,7 +2964,7 @@
       <c r="AC45" s="23"/>
     </row>
     <row r="46" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="W46" s="112" t="s">
+      <c r="W46" s="110" t="s">
         <v>184</v>
       </c>
       <c r="X46" s="22"/>
@@ -2967,7 +2975,7 @@
       <c r="AC46" s="23"/>
     </row>
     <row r="47" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="W47" s="112" t="s">
+      <c r="W47" s="110" t="s">
         <v>185</v>
       </c>
       <c r="X47" s="22"/>
@@ -2978,7 +2986,7 @@
       <c r="AC47" s="23"/>
     </row>
     <row r="48" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="W48" s="112" t="s">
+      <c r="W48" s="110" t="s">
         <v>186</v>
       </c>
       <c r="X48" s="22"/>
@@ -2989,7 +2997,7 @@
       <c r="AC48" s="23"/>
     </row>
     <row r="49" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W49" s="112" t="s">
+      <c r="W49" s="110" t="s">
         <v>187</v>
       </c>
       <c r="X49" s="22"/>
@@ -3000,7 +3008,7 @@
       <c r="AC49" s="23"/>
     </row>
     <row r="50" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W50" s="112" t="s">
+      <c r="W50" s="110" t="s">
         <v>188</v>
       </c>
       <c r="X50" s="22"/>
@@ -3011,7 +3019,7 @@
       <c r="AC50" s="23"/>
     </row>
     <row r="51" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W51" s="112" t="s">
+      <c r="W51" s="110" t="s">
         <v>189</v>
       </c>
       <c r="X51" s="22"/>
@@ -3022,7 +3030,7 @@
       <c r="AC51" s="23"/>
     </row>
     <row r="52" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W52" s="112"/>
+      <c r="W52" s="110"/>
       <c r="X52" s="22"/>
       <c r="Y52" s="22"/>
       <c r="Z52" s="22"/>
@@ -3031,7 +3039,7 @@
       <c r="AC52" s="23"/>
     </row>
     <row r="53" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W53" s="112" t="s">
+      <c r="W53" s="110" t="s">
         <v>190</v>
       </c>
       <c r="X53" s="22"/>
@@ -3042,7 +3050,7 @@
       <c r="AC53" s="23"/>
     </row>
     <row r="54" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W54" s="112" t="s">
+      <c r="W54" s="110" t="s">
         <v>191</v>
       </c>
       <c r="X54" s="22"/>
@@ -3053,7 +3061,7 @@
       <c r="AC54" s="23"/>
     </row>
     <row r="55" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W55" s="112"/>
+      <c r="W55" s="110"/>
       <c r="X55" s="22"/>
       <c r="Y55" s="22"/>
       <c r="Z55" s="22"/>
@@ -3062,7 +3070,7 @@
       <c r="AC55" s="23"/>
     </row>
     <row r="56" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W56" s="119" t="s">
+      <c r="W56" s="117" t="s">
         <v>192</v>
       </c>
       <c r="X56" s="22"/>
@@ -3073,7 +3081,7 @@
       <c r="AC56" s="23"/>
     </row>
     <row r="57" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W57" s="112" t="s">
+      <c r="W57" s="110" t="s">
         <v>193</v>
       </c>
       <c r="X57" s="22"/>
@@ -3084,7 +3092,7 @@
       <c r="AC57" s="23"/>
     </row>
     <row r="58" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W58" s="112" t="s">
+      <c r="W58" s="110" t="s">
         <v>194</v>
       </c>
       <c r="X58" s="22"/>
@@ -3095,7 +3103,7 @@
       <c r="AC58" s="23"/>
     </row>
     <row r="59" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W59" s="112" t="s">
+      <c r="W59" s="110" t="s">
         <v>195</v>
       </c>
       <c r="X59" s="22"/>
@@ -3106,7 +3114,7 @@
       <c r="AC59" s="23"/>
     </row>
     <row r="60" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W60" s="112" t="s">
+      <c r="W60" s="110" t="s">
         <v>196</v>
       </c>
       <c r="X60" s="22"/>
@@ -3117,7 +3125,7 @@
       <c r="AC60" s="23"/>
     </row>
     <row r="61" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W61" s="116" t="s">
+      <c r="W61" s="114" t="s">
         <v>197</v>
       </c>
       <c r="X61" s="22"/>
@@ -3128,7 +3136,7 @@
       <c r="AC61" s="23"/>
     </row>
     <row r="62" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W62" s="112" t="s">
+      <c r="W62" s="110" t="s">
         <v>198</v>
       </c>
       <c r="X62" s="22"/>
@@ -3139,7 +3147,7 @@
       <c r="AC62" s="23"/>
     </row>
     <row r="63" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W63" s="112" t="s">
+      <c r="W63" s="110" t="s">
         <v>199</v>
       </c>
       <c r="X63" s="22"/>
@@ -3150,7 +3158,7 @@
       <c r="AC63" s="23"/>
     </row>
     <row r="64" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W64" s="112"/>
+      <c r="W64" s="110"/>
       <c r="X64" s="22"/>
       <c r="Y64" s="22"/>
       <c r="Z64" s="22"/>
@@ -3159,7 +3167,7 @@
       <c r="AC64" s="23"/>
     </row>
     <row r="65" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W65" s="119" t="s">
+      <c r="W65" s="117" t="s">
         <v>200</v>
       </c>
       <c r="X65" s="22"/>
@@ -3170,7 +3178,7 @@
       <c r="AC65" s="23"/>
     </row>
     <row r="66" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W66" s="112" t="s">
+      <c r="W66" s="110" t="s">
         <v>201</v>
       </c>
       <c r="X66" s="22"/>
@@ -3181,7 +3189,7 @@
       <c r="AC66" s="23"/>
     </row>
     <row r="67" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W67" s="112" t="s">
+      <c r="W67" s="110" t="s">
         <v>202</v>
       </c>
       <c r="X67" s="22"/>
@@ -3192,7 +3200,7 @@
       <c r="AC67" s="23"/>
     </row>
     <row r="68" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W68" s="112" t="s">
+      <c r="W68" s="110" t="s">
         <v>203</v>
       </c>
       <c r="X68" s="22"/>
@@ -3203,7 +3211,7 @@
       <c r="AC68" s="23"/>
     </row>
     <row r="69" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W69" s="112" t="s">
+      <c r="W69" s="110" t="s">
         <v>204</v>
       </c>
       <c r="X69" s="22"/>
@@ -3214,7 +3222,7 @@
       <c r="AC69" s="23"/>
     </row>
     <row r="70" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W70" s="116" t="s">
+      <c r="W70" s="114" t="s">
         <v>205</v>
       </c>
       <c r="X70" s="22"/>
@@ -3225,7 +3233,7 @@
       <c r="AC70" s="23"/>
     </row>
     <row r="71" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W71" s="112"/>
+      <c r="W71" s="110"/>
       <c r="X71" s="22"/>
       <c r="Y71" s="22"/>
       <c r="Z71" s="22"/>
@@ -3234,7 +3242,7 @@
       <c r="AC71" s="23"/>
     </row>
     <row r="72" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W72" s="119" t="s">
+      <c r="W72" s="117" t="s">
         <v>206</v>
       </c>
       <c r="X72" s="22"/>
@@ -3245,7 +3253,7 @@
       <c r="AC72" s="23"/>
     </row>
     <row r="73" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W73" s="112" t="s">
+      <c r="W73" s="110" t="s">
         <v>207</v>
       </c>
       <c r="X73" s="22"/>
@@ -3256,7 +3264,7 @@
       <c r="AC73" s="23"/>
     </row>
     <row r="74" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W74" s="116" t="s">
+      <c r="W74" s="114" t="s">
         <v>208</v>
       </c>
       <c r="X74" s="22"/>
@@ -3267,7 +3275,7 @@
       <c r="AC74" s="23"/>
     </row>
     <row r="75" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W75" s="112" t="s">
+      <c r="W75" s="110" t="s">
         <v>209</v>
       </c>
       <c r="X75" s="22"/>
@@ -3278,7 +3286,7 @@
       <c r="AC75" s="23"/>
     </row>
     <row r="76" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W76" s="116" t="s">
+      <c r="W76" s="114" t="s">
         <v>210</v>
       </c>
       <c r="X76" s="22"/>
@@ -3289,7 +3297,7 @@
       <c r="AC76" s="23"/>
     </row>
     <row r="77" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W77" s="112" t="s">
+      <c r="W77" s="110" t="s">
         <v>211</v>
       </c>
       <c r="X77" s="22"/>
@@ -3300,7 +3308,7 @@
       <c r="AC77" s="23"/>
     </row>
     <row r="78" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W78" s="112" t="s">
+      <c r="W78" s="110" t="s">
         <v>212</v>
       </c>
       <c r="X78" s="22"/>
@@ -3311,7 +3319,7 @@
       <c r="AC78" s="23"/>
     </row>
     <row r="79" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W79" s="116" t="s">
+      <c r="W79" s="114" t="s">
         <v>213</v>
       </c>
       <c r="X79" s="22"/>
@@ -3322,7 +3330,7 @@
       <c r="AC79" s="23"/>
     </row>
     <row r="80" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W80" s="112" t="s">
+      <c r="W80" s="110" t="s">
         <v>214</v>
       </c>
       <c r="X80" s="22"/>
@@ -3333,7 +3341,7 @@
       <c r="AC80" s="23"/>
     </row>
     <row r="81" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W81" s="112" t="s">
+      <c r="W81" s="110" t="s">
         <v>215</v>
       </c>
       <c r="X81" s="22"/>
@@ -3344,7 +3352,7 @@
       <c r="AC81" s="23"/>
     </row>
     <row r="82" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W82" s="112" t="s">
+      <c r="W82" s="110" t="s">
         <v>216</v>
       </c>
       <c r="X82" s="22"/>
@@ -3355,7 +3363,7 @@
       <c r="AC82" s="23"/>
     </row>
     <row r="83" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W83" s="112"/>
+      <c r="W83" s="110"/>
       <c r="X83" s="22"/>
       <c r="Y83" s="22"/>
       <c r="Z83" s="22"/>
@@ -3364,7 +3372,7 @@
       <c r="AC83" s="23"/>
     </row>
     <row r="84" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W84" s="119" t="s">
+      <c r="W84" s="117" t="s">
         <v>217</v>
       </c>
       <c r="X84" s="22"/>
@@ -3375,7 +3383,7 @@
       <c r="AC84" s="23"/>
     </row>
     <row r="85" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W85" s="112" t="s">
+      <c r="W85" s="110" t="s">
         <v>218</v>
       </c>
       <c r="X85" s="22"/>
@@ -3386,7 +3394,7 @@
       <c r="AC85" s="23"/>
     </row>
     <row r="86" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W86" s="112" t="s">
+      <c r="W86" s="110" t="s">
         <v>219</v>
       </c>
       <c r="X86" s="22"/>
@@ -3397,7 +3405,7 @@
       <c r="AC86" s="23"/>
     </row>
     <row r="87" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W87" s="116" t="s">
+      <c r="W87" s="114" t="s">
         <v>220</v>
       </c>
       <c r="X87" s="22"/>
@@ -3408,7 +3416,7 @@
       <c r="AC87" s="23"/>
     </row>
     <row r="88" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W88" s="112" t="s">
+      <c r="W88" s="110" t="s">
         <v>221</v>
       </c>
       <c r="X88" s="22"/>
@@ -3419,7 +3427,7 @@
       <c r="AC88" s="23"/>
     </row>
     <row r="89" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W89" s="116" t="s">
+      <c r="W89" s="114" t="s">
         <v>222</v>
       </c>
       <c r="X89" s="22"/>
@@ -3430,7 +3438,7 @@
       <c r="AC89" s="23"/>
     </row>
     <row r="90" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W90" s="112" t="s">
+      <c r="W90" s="110" t="s">
         <v>223</v>
       </c>
       <c r="X90" s="22"/>
@@ -3441,7 +3449,7 @@
       <c r="AC90" s="23"/>
     </row>
     <row r="91" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W91" s="112" t="s">
+      <c r="W91" s="110" t="s">
         <v>224</v>
       </c>
       <c r="X91" s="22"/>
@@ -3452,7 +3460,7 @@
       <c r="AC91" s="23"/>
     </row>
     <row r="92" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W92" s="116" t="s">
+      <c r="W92" s="114" t="s">
         <v>225</v>
       </c>
       <c r="X92" s="22"/>
@@ -3463,7 +3471,7 @@
       <c r="AC92" s="23"/>
     </row>
     <row r="93" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W93" s="112"/>
+      <c r="W93" s="110"/>
       <c r="X93" s="22"/>
       <c r="Y93" s="22"/>
       <c r="Z93" s="22"/>
@@ -3472,7 +3480,7 @@
       <c r="AC93" s="23"/>
     </row>
     <row r="94" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W94" s="112"/>
+      <c r="W94" s="110"/>
       <c r="X94" s="22"/>
       <c r="Y94" s="22"/>
       <c r="Z94" s="22"/>
@@ -3481,7 +3489,7 @@
       <c r="AC94" s="23"/>
     </row>
     <row r="95" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W95" s="119" t="s">
+      <c r="W95" s="117" t="s">
         <v>226</v>
       </c>
       <c r="X95" s="22"/>
@@ -3492,7 +3500,7 @@
       <c r="AC95" s="23"/>
     </row>
     <row r="96" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W96" s="112" t="s">
+      <c r="W96" s="110" t="s">
         <v>227</v>
       </c>
       <c r="X96" s="22"/>
@@ -3503,7 +3511,7 @@
       <c r="AC96" s="23"/>
     </row>
     <row r="97" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W97" s="112" t="s">
+      <c r="W97" s="110" t="s">
         <v>228</v>
       </c>
       <c r="X97" s="22"/>
@@ -3514,7 +3522,7 @@
       <c r="AC97" s="23"/>
     </row>
     <row r="98" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W98" s="112" t="s">
+      <c r="W98" s="110" t="s">
         <v>229</v>
       </c>
       <c r="X98" s="22"/>
@@ -3525,7 +3533,7 @@
       <c r="AC98" s="23"/>
     </row>
     <row r="99" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W99" s="112" t="s">
+      <c r="W99" s="110" t="s">
         <v>230</v>
       </c>
       <c r="X99" s="22"/>
@@ -3536,7 +3544,7 @@
       <c r="AC99" s="23"/>
     </row>
     <row r="100" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W100" s="112" t="s">
+      <c r="W100" s="110" t="s">
         <v>231</v>
       </c>
       <c r="X100" s="22"/>
@@ -3547,7 +3555,7 @@
       <c r="AC100" s="23"/>
     </row>
     <row r="101" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W101" s="112" t="s">
+      <c r="W101" s="110" t="s">
         <v>232</v>
       </c>
       <c r="X101" s="22"/>
@@ -3558,7 +3566,7 @@
       <c r="AC101" s="23"/>
     </row>
     <row r="102" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W102" s="112" t="s">
+      <c r="W102" s="110" t="s">
         <v>233</v>
       </c>
       <c r="X102" s="22"/>
@@ -3569,7 +3577,7 @@
       <c r="AC102" s="23"/>
     </row>
     <row r="103" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W103" s="112" t="s">
+      <c r="W103" s="110" t="s">
         <v>234</v>
       </c>
       <c r="X103" s="22"/>
@@ -3580,7 +3588,7 @@
       <c r="AC103" s="23"/>
     </row>
     <row r="104" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W104" s="112" t="s">
+      <c r="W104" s="110" t="s">
         <v>235</v>
       </c>
       <c r="X104" s="22"/>
@@ -3591,7 +3599,7 @@
       <c r="AC104" s="23"/>
     </row>
     <row r="105" spans="23:29" x14ac:dyDescent="0.25">
-      <c r="W105" s="113" t="s">
+      <c r="W105" s="111" t="s">
         <v>236</v>
       </c>
       <c r="X105" s="24"/>
@@ -3603,6 +3611,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="W24:AC24"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="P24:R24"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C37:D37"/>
     <mergeCell ref="C42:D42"/>
     <mergeCell ref="J2:L2"/>
     <mergeCell ref="K3:L3"/>
@@ -3619,28 +3649,6 @@
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="C16:D16"/>
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="P24:R24"/>
-    <mergeCell ref="Q25:R25"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="W24:AC24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K6:L6" r:id="rId1" display="Link" xr:uid="{EBABCF04-F876-4DF1-ADF1-1B6F62DC4548}"/>
@@ -3679,7 +3687,7 @@
     <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.42578125" style="32" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" style="132"/>
+    <col min="14" max="14" width="8.85546875" style="130"/>
     <col min="16" max="21" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="9.140625" bestFit="1" customWidth="1"/>
@@ -3704,7 +3712,7 @@
       <c r="H1" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="I1" s="84" t="s">
+      <c r="I1" s="83" t="s">
         <v>90</v>
       </c>
       <c r="J1" s="30" t="s">
@@ -3716,10 +3724,10 @@
       <c r="L1" s="30" t="s">
         <v>244</v>
       </c>
-      <c r="M1" s="124" t="s">
+      <c r="M1" s="122" t="s">
         <v>245</v>
       </c>
-      <c r="N1" s="126" t="s">
+      <c r="N1" s="124" t="s">
         <v>247</v>
       </c>
       <c r="O1" s="13"/>
@@ -3738,7 +3746,7 @@
       <c r="T1" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="U1" s="124" t="s">
+      <c r="U1" s="122" t="s">
         <v>110</v>
       </c>
       <c r="V1" s="13" t="s">
@@ -3769,44 +3777,44 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="2:30" s="88" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="86"/>
+    <row r="2" spans="2:30" s="87" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="85"/>
       <c r="C2" s="20">
         <v>43646</v>
       </c>
-      <c r="D2" s="87" t="s">
+      <c r="D2" s="86" t="s">
         <v>92</v>
       </c>
       <c r="E2" s="20">
         <v>44012</v>
       </c>
-      <c r="F2" s="87">
+      <c r="F2" s="86">
         <v>44196</v>
       </c>
       <c r="G2" s="20">
         <v>44377</v>
       </c>
-      <c r="H2" s="87">
+      <c r="H2" s="86">
         <v>44561</v>
       </c>
       <c r="I2" s="20">
         <v>44742</v>
       </c>
-      <c r="J2" s="87">
+      <c r="J2" s="86">
         <f>T2</f>
         <v>44926</v>
       </c>
       <c r="K2" s="20">
         <v>45107</v>
       </c>
-      <c r="L2" s="87">
+      <c r="L2" s="86">
         <f>U2</f>
         <v>45291</v>
       </c>
       <c r="M2" s="20">
         <v>45473</v>
       </c>
-      <c r="N2" s="127"/>
+      <c r="N2" s="125"/>
       <c r="P2" s="20">
         <v>43465</v>
       </c>
@@ -3861,18 +3869,18 @@
       <c r="F3" s="31"/>
       <c r="G3" s="14"/>
       <c r="H3" s="31"/>
-      <c r="I3" s="85">
+      <c r="I3" s="84">
         <v>44825</v>
       </c>
       <c r="J3" s="76"/>
-      <c r="K3" s="85">
+      <c r="K3" s="84">
         <v>45146</v>
       </c>
       <c r="L3" s="76"/>
-      <c r="M3" s="121">
+      <c r="M3" s="119">
         <v>45561</v>
       </c>
-      <c r="N3" s="127" t="s">
+      <c r="N3" s="125" t="s">
         <v>248</v>
       </c>
       <c r="P3" s="20"/>
@@ -3919,21 +3927,21 @@
       <c r="I4" s="71">
         <v>9.8320000000000007</v>
       </c>
-      <c r="J4" s="125">
+      <c r="J4" s="123">
         <f>T4-I4</f>
         <v>12.481999999999999</v>
       </c>
       <c r="K4" s="71">
         <v>2.464</v>
       </c>
-      <c r="L4" s="125">
+      <c r="L4" s="123">
         <f>U4-K4</f>
         <v>8.5129999999999999</v>
       </c>
       <c r="M4" s="71">
         <v>0.88100000000000001</v>
       </c>
-      <c r="N4" s="128">
+      <c r="N4" s="126">
         <f>+M4*2.75</f>
         <v>2.4227500000000002</v>
       </c>
@@ -4035,7 +4043,7 @@
       <c r="M5" s="67">
         <v>1.167</v>
       </c>
-      <c r="N5" s="129"/>
+      <c r="N5" s="127"/>
       <c r="O5" s="67"/>
       <c r="P5" s="64">
         <v>0.54072100000000001</v>
@@ -4133,7 +4141,7 @@
       <c r="M6" s="67">
         <v>0</v>
       </c>
-      <c r="N6" s="129"/>
+      <c r="N6" s="127"/>
       <c r="O6" s="67"/>
       <c r="P6" s="65">
         <v>0</v>
@@ -4213,7 +4221,7 @@
         <f t="shared" si="2"/>
         <v>1.511000000000001</v>
       </c>
-      <c r="J7" s="125">
+      <c r="J7" s="123">
         <f>T7-I7</f>
         <v>3.2739999999999991</v>
       </c>
@@ -4229,7 +4237,7 @@
         <f t="shared" si="2"/>
         <v>-0.28600000000000003</v>
       </c>
-      <c r="N7" s="129">
+      <c r="N7" s="127">
         <f>N4*N23</f>
         <v>0.67837000000000014</v>
       </c>
@@ -4254,7 +4262,7 @@
         <f t="shared" ref="T7:U7" si="3">T4-T5-T6</f>
         <v>4.7850000000000001</v>
       </c>
-      <c r="U7" s="122">
+      <c r="U7" s="120">
         <f t="shared" si="3"/>
         <v>2.048</v>
       </c>
@@ -4337,7 +4345,7 @@
       <c r="M8" s="67">
         <v>0</v>
       </c>
-      <c r="N8" s="129"/>
+      <c r="N8" s="127"/>
       <c r="O8" s="67"/>
       <c r="P8" s="65">
         <v>0</v>
@@ -4427,7 +4435,7 @@
       <c r="M9" s="67">
         <v>0</v>
       </c>
-      <c r="N9" s="129"/>
+      <c r="N9" s="127"/>
       <c r="O9" s="67"/>
       <c r="P9" s="65">
         <v>0</v>
@@ -4517,7 +4525,7 @@
       <c r="M10" s="67">
         <v>0.76</v>
       </c>
-      <c r="N10" s="130"/>
+      <c r="N10" s="128"/>
       <c r="O10" s="67"/>
       <c r="P10" s="66">
         <v>2.213695</v>
@@ -4616,7 +4624,7 @@
       <c r="M11" s="67">
         <v>0</v>
       </c>
-      <c r="N11" s="129"/>
+      <c r="N11" s="127"/>
       <c r="O11" s="67"/>
       <c r="P11" s="65">
         <v>0</v>
@@ -4707,7 +4715,7 @@
       <c r="M12" s="67">
         <v>0.03</v>
       </c>
-      <c r="N12" s="129"/>
+      <c r="N12" s="127"/>
       <c r="O12" s="67"/>
       <c r="P12" s="66">
         <v>9.2290999999999998E-2</v>
@@ -4809,7 +4817,7 @@
       <c r="M13" s="67">
         <v>0.79</v>
       </c>
-      <c r="N13" s="129"/>
+      <c r="N13" s="127"/>
       <c r="O13" s="67"/>
       <c r="P13" s="66">
         <f t="shared" ref="P13:U13" si="10">SUM(P8:P12)</f>
@@ -4827,7 +4835,7 @@
         <f t="shared" si="10"/>
         <v>3.0790000000000002</v>
       </c>
-      <c r="T13" s="123">
+      <c r="T13" s="121">
         <f t="shared" si="10"/>
         <v>2.3430000000000004</v>
       </c>
@@ -4911,7 +4919,7 @@
       <c r="M14" s="67">
         <v>0.27200000000000002</v>
       </c>
-      <c r="N14" s="129"/>
+      <c r="N14" s="127"/>
       <c r="O14" s="67"/>
       <c r="P14" s="66">
         <v>0</v>
@@ -5016,7 +5024,7 @@
         <f>M7-M13-M14</f>
         <v>-1.3480000000000001</v>
       </c>
-      <c r="N15" s="129"/>
+      <c r="N15" s="127"/>
       <c r="O15" s="67"/>
       <c r="P15" s="63">
         <f>P7-P13</f>
@@ -5123,7 +5131,7 @@
         <f>0.001-0.15</f>
         <v>-0.14899999999999999</v>
       </c>
-      <c r="N16" s="129"/>
+      <c r="N16" s="127"/>
       <c r="O16" s="67"/>
       <c r="P16" s="66">
         <v>2.3914999999999999E-2</v>
@@ -5231,7 +5239,7 @@
         <f t="shared" si="16"/>
         <v>-1.1990000000000001</v>
       </c>
-      <c r="N17" s="129"/>
+      <c r="N17" s="127"/>
       <c r="O17" s="67"/>
       <c r="P17" s="63">
         <f>P15-P16</f>
@@ -5336,7 +5344,7 @@
       <c r="M18" s="66">
         <v>0</v>
       </c>
-      <c r="N18" s="131"/>
+      <c r="N18" s="129"/>
       <c r="O18" s="66"/>
       <c r="P18" s="66">
         <v>5.2276999999999997E-2</v>
@@ -5432,7 +5440,7 @@
         <f t="shared" si="19"/>
         <v>-1.1990000000000001</v>
       </c>
-      <c r="N19" s="129"/>
+      <c r="N19" s="127"/>
       <c r="O19" s="67"/>
       <c r="P19" s="63">
         <f>P17+P18</f>
@@ -5675,7 +5683,7 @@
         <f t="shared" si="24"/>
         <v>-2.3055062257128667E-2</v>
       </c>
-      <c r="N20" s="129"/>
+      <c r="N20" s="127"/>
       <c r="O20" s="67"/>
       <c r="P20" s="66">
         <f>(P19/P21)</f>
@@ -5780,7 +5788,7 @@
       <c r="M21" s="67">
         <v>52.005932000000001</v>
       </c>
-      <c r="N21" s="129"/>
+      <c r="N21" s="127"/>
       <c r="O21" s="67"/>
       <c r="P21" s="66">
         <v>158.321675</v>
@@ -5882,7 +5890,7 @@
       <c r="M23" s="36">
         <v>0.31</v>
       </c>
-      <c r="N23" s="134">
+      <c r="N23" s="132">
         <v>0.28000000000000003</v>
       </c>
       <c r="P23" s="16">
@@ -6362,120 +6370,120 @@
         <f>AG27/Main!C7</f>
         <v>0.74703074912372858</v>
       </c>
-      <c r="AI28" s="94"/>
+      <c r="AI28" s="93"/>
     </row>
     <row r="29" spans="2:63" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="C29" s="89">
-        <v>0</v>
-      </c>
-      <c r="D29" s="90">
-        <v>0</v>
-      </c>
-      <c r="E29" s="91">
+      <c r="C29" s="88">
+        <v>0</v>
+      </c>
+      <c r="D29" s="89">
+        <v>0</v>
+      </c>
+      <c r="E29" s="90">
         <f t="shared" ref="E29:M29" si="48">E4/C4-1</f>
         <v>-0.19151237513520392</v>
       </c>
-      <c r="F29" s="92">
+      <c r="F29" s="91">
         <f t="shared" si="48"/>
         <v>1.2625361471728298</v>
       </c>
-      <c r="G29" s="91">
+      <c r="G29" s="90">
         <f t="shared" si="48"/>
         <v>256.6646730148737</v>
       </c>
-      <c r="H29" s="92">
+      <c r="H29" s="91">
         <f t="shared" si="48"/>
         <v>355.29007695863817</v>
       </c>
-      <c r="I29" s="91">
+      <c r="I29" s="90">
         <f t="shared" si="48"/>
         <v>2.0029213733661768</v>
       </c>
-      <c r="J29" s="92">
+      <c r="J29" s="91">
         <f t="shared" si="48"/>
         <v>-4.7310476264620593E-2</v>
       </c>
-      <c r="K29" s="91">
+      <c r="K29" s="90">
         <f t="shared" si="48"/>
         <v>-0.74938974776240852</v>
       </c>
-      <c r="L29" s="92">
+      <c r="L29" s="91">
         <f t="shared" si="48"/>
         <v>-0.3179778881589489</v>
       </c>
-      <c r="M29" s="91">
+      <c r="M29" s="90">
         <f t="shared" si="48"/>
         <v>-0.64245129870129869</v>
       </c>
-      <c r="N29" s="133"/>
-      <c r="P29" s="89">
-        <v>0</v>
-      </c>
-      <c r="Q29" s="91">
+      <c r="N29" s="131"/>
+      <c r="P29" s="88">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="90">
         <f>Q4/P4-1</f>
         <v>5.6081025217031826</v>
       </c>
-      <c r="R29" s="91">
+      <c r="R29" s="90">
         <f>R4/Q4-1</f>
         <v>0.54770096965905557</v>
       </c>
-      <c r="S29" s="91">
+      <c r="S29" s="90">
         <f>S4/R4-1</f>
         <v>329.9620048504446</v>
       </c>
-      <c r="T29" s="91">
+      <c r="T29" s="90">
         <f t="shared" ref="T29:U29" si="49">T4/S4-1</f>
         <v>0.36260381045432322</v>
       </c>
-      <c r="U29" s="91">
+      <c r="U29" s="90">
         <f t="shared" si="49"/>
         <v>-0.50806668459263249</v>
       </c>
-      <c r="V29" s="91">
+      <c r="V29" s="90">
         <f t="shared" ref="V29" si="50">V4/U4-1</f>
         <v>-0.69902978955998907</v>
       </c>
-      <c r="W29" s="91">
+      <c r="W29" s="90">
         <f t="shared" ref="W29:AD29" si="51">W4/V4-1</f>
         <v>0.25</v>
       </c>
-      <c r="X29" s="91">
+      <c r="X29" s="90">
         <f t="shared" si="51"/>
         <v>0.25</v>
       </c>
-      <c r="Y29" s="91">
+      <c r="Y29" s="90">
         <f t="shared" si="51"/>
         <v>0.25</v>
       </c>
-      <c r="Z29" s="91">
+      <c r="Z29" s="90">
         <f t="shared" si="51"/>
         <v>0.25</v>
       </c>
-      <c r="AA29" s="91">
+      <c r="AA29" s="90">
         <f t="shared" si="51"/>
         <v>0.25</v>
       </c>
-      <c r="AB29" s="91">
+      <c r="AB29" s="90">
         <f t="shared" si="51"/>
         <v>0.25</v>
       </c>
-      <c r="AC29" s="91">
+      <c r="AC29" s="90">
         <f t="shared" si="51"/>
         <v>0.25</v>
       </c>
-      <c r="AD29" s="91">
+      <c r="AD29" s="90">
         <f t="shared" si="51"/>
         <v>0.25</v>
       </c>
       <c r="AF29" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="AG29" s="93">
+      <c r="AG29" s="92">
         <f>Main!C6</f>
-        <v>0.12620000000000001</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="30" spans="2:63" x14ac:dyDescent="0.25">
@@ -6559,83 +6567,83 @@
       <c r="B31" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="C31" s="89">
-        <v>0</v>
-      </c>
-      <c r="D31" s="90">
-        <v>0</v>
-      </c>
-      <c r="E31" s="91">
+      <c r="C31" s="88">
+        <v>0</v>
+      </c>
+      <c r="D31" s="89">
+        <v>0</v>
+      </c>
+      <c r="E31" s="90">
         <f t="shared" ref="E31:M31" si="53">E19/C19-1</f>
         <v>6.9873023754210895E-2</v>
       </c>
-      <c r="F31" s="92">
+      <c r="F31" s="91">
         <f t="shared" si="53"/>
         <v>1.7142245402388041</v>
       </c>
-      <c r="G31" s="91">
+      <c r="G31" s="90">
         <f t="shared" si="53"/>
         <v>-0.80078168438751474</v>
       </c>
-      <c r="H31" s="92">
+      <c r="H31" s="91">
         <f t="shared" si="53"/>
         <v>-1.941605215233448</v>
       </c>
-      <c r="I31" s="91">
+      <c r="I31" s="90">
         <f t="shared" si="53"/>
         <v>-1.0334918614776643</v>
       </c>
-      <c r="J31" s="92">
+      <c r="J31" s="91">
         <f t="shared" si="53"/>
         <v>-0.33647846063002929</v>
       </c>
-      <c r="K31" s="91">
+      <c r="K31" s="90">
         <f t="shared" si="53"/>
         <v>-36.444444444440911</v>
       </c>
-      <c r="L31" s="92">
+      <c r="L31" s="91">
         <f t="shared" si="53"/>
         <v>-0.89389920424403224</v>
       </c>
-      <c r="M31" s="91">
+      <c r="M31" s="90">
         <f t="shared" si="53"/>
         <v>2.7586206896551717</v>
       </c>
-      <c r="N31" s="133"/>
-      <c r="P31" s="89">
-        <v>0</v>
-      </c>
-      <c r="Q31" s="91">
+      <c r="N31" s="131"/>
+      <c r="P31" s="88">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="90">
         <f>Q19/P19-1</f>
         <v>-0.23581032497875432</v>
       </c>
-      <c r="R31" s="91">
+      <c r="R31" s="90">
         <f>R19/Q19-1</f>
         <v>0.74997993072728897</v>
       </c>
-      <c r="S31" s="91">
+      <c r="S31" s="90">
         <f>S19/R19-1</f>
         <v>-1.5326175633671386</v>
       </c>
-      <c r="T31" s="91">
+      <c r="T31" s="90">
         <f t="shared" ref="T31:U31" si="54">T19/S19-1</f>
         <v>-0.24301397205588893</v>
       </c>
-      <c r="U31" s="91">
+      <c r="U31" s="90">
         <f t="shared" si="54"/>
         <v>-1.1048121292023731</v>
       </c>
-      <c r="V31" s="91"/>
-      <c r="W31" s="91"/>
-      <c r="X31" s="91"/>
-      <c r="Y31" s="91"/>
-      <c r="Z31" s="91"/>
-      <c r="AA31" s="91"/>
-      <c r="AB31" s="91"/>
-      <c r="AC31" s="91"/>
-      <c r="AD31" s="91"/>
+      <c r="V31" s="90"/>
+      <c r="W31" s="90"/>
+      <c r="X31" s="90"/>
+      <c r="Y31" s="90"/>
+      <c r="Z31" s="90"/>
+      <c r="AA31" s="90"/>
+      <c r="AB31" s="90"/>
+      <c r="AC31" s="90"/>
+      <c r="AD31" s="90"/>
       <c r="AF31" s="44"/>
-      <c r="AG31" s="93"/>
+      <c r="AG31" s="92"/>
     </row>
     <row r="32" spans="2:63" x14ac:dyDescent="0.25">
       <c r="C32" s="15"/>
@@ -6668,7 +6676,7 @@
       </c>
       <c r="AG33" s="51">
         <f>AG28/AG29</f>
-        <v>5.9194195651642518</v>
+        <v>4.394298524257227</v>
       </c>
     </row>
     <row r="34" spans="2:33" x14ac:dyDescent="0.25">
@@ -6902,14 +6910,14 @@
         <f t="shared" si="56"/>
         <v>6.3869999999999996</v>
       </c>
-      <c r="I41" s="80">
+      <c r="I41" s="79">
         <v>6.9950000000000001</v>
       </c>
       <c r="J41" s="60"/>
       <c r="K41" s="12"/>
       <c r="L41" s="60"/>
       <c r="M41" s="12"/>
-      <c r="N41" s="133"/>
+      <c r="N41" s="131"/>
       <c r="O41" s="12"/>
       <c r="P41" s="12"/>
       <c r="Q41" s="58">
@@ -7249,7 +7257,7 @@
       <c r="K51" s="12"/>
       <c r="L51" s="60"/>
       <c r="M51" s="12"/>
-      <c r="N51" s="133"/>
+      <c r="N51" s="131"/>
       <c r="O51" s="12"/>
       <c r="P51" s="12"/>
       <c r="Q51" s="59">
@@ -7407,7 +7415,7 @@
         <f t="shared" ref="D57" si="58">D42-D52</f>
         <v>2.233822</v>
       </c>
-      <c r="E57" s="79">
+      <c r="E57" s="78">
         <f t="shared" ref="E57:F57" si="59">E42-E52</f>
         <v>2.625874</v>
       </c>
@@ -7415,7 +7423,7 @@
         <f t="shared" si="59"/>
         <v>0.52937599999999996</v>
       </c>
-      <c r="G57" s="79">
+      <c r="G57" s="78">
         <f t="shared" ref="G57:H57" si="60">G42-G52</f>
         <v>3.5457600000000009</v>
       </c>
@@ -7423,19 +7431,19 @@
         <f t="shared" si="60"/>
         <v>7.1129999999999995</v>
       </c>
-      <c r="I57" s="79">
+      <c r="I57" s="78">
         <f t="shared" ref="I57" si="61">I42-I52</f>
         <v>8.4660000000000011</v>
       </c>
-      <c r="Q57" s="79">
+      <c r="Q57" s="78">
         <f t="shared" ref="Q57:R57" si="62">Q42-Q52</f>
         <v>2.233822</v>
       </c>
-      <c r="R57" s="79">
+      <c r="R57" s="78">
         <f t="shared" si="62"/>
         <v>0.52937599999999996</v>
       </c>
-      <c r="S57" s="79">
+      <c r="S57" s="78">
         <f>S42-S52</f>
         <v>7.1129999999999995</v>
       </c>
@@ -7649,59 +7657,59 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="99"/>
+    <col min="1" max="16384" width="9.140625" style="97"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="101" t="s">
+    <row r="1" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="99" t="s">
         <v>242</v>
       </c>
-      <c r="C1" s="101" t="s">
+      <c r="C1" s="99" t="s">
         <v>244</v>
       </c>
-      <c r="D1" s="101" t="s">
+      <c r="D1" s="99" t="s">
         <v>245</v>
       </c>
-      <c r="E1" s="101" t="s">
+      <c r="E1" s="99" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="160" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="160" t="s">
+    <row r="3" spans="1:5" s="133" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="133" t="s">
         <v>249</v>
       </c>
-      <c r="B3" s="160">
+      <c r="B3" s="133">
         <v>2342000</v>
       </c>
-      <c r="D3" s="160">
+      <c r="D3" s="133">
         <v>572000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="160" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="160" t="s">
+    <row r="4" spans="1:5" s="133" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="133" t="s">
         <v>250</v>
       </c>
-      <c r="B4" s="160">
+      <c r="B4" s="133">
         <v>122000</v>
       </c>
-      <c r="D4" s="160">
+      <c r="D4" s="133">
         <v>309000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="161" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="161" t="s">
+    <row r="6" spans="1:5" s="134" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="134" t="s">
         <v>251</v>
       </c>
-      <c r="D6" s="161">
+      <c r="D6" s="134">
         <f>D3/B3-1</f>
         <v>-0.75576430401366357</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="161" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="161" t="s">
+    <row r="7" spans="1:5" s="134" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="134" t="s">
         <v>252</v>
       </c>
-      <c r="D7" s="161">
+      <c r="D7" s="134">
         <f>D4/B4-1</f>
         <v>1.5327868852459017</v>
       </c>
@@ -7914,217 +7922,217 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" style="99" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="99"/>
+    <col min="1" max="1" width="30.85546875" style="97" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="97"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="D1" s="102" t="s">
+    <row r="1" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D1" s="100" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="101" t="s">
+      <c r="E1" s="99" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="100" t="s">
+      <c r="A2" s="98" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="103">
+      <c r="D2" s="101">
         <v>20.470000000000002</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="99" t="s">
+      <c r="A3" s="97" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="104">
+      <c r="D3" s="102">
         <v>14.124300000000002</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="99" t="s">
+      <c r="A4" s="97" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="105">
+      <c r="D4" s="103">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="100" t="s">
+      <c r="A5" s="98" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="103">
+      <c r="D5" s="101">
         <v>6.3457000000000008</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="99" t="s">
+      <c r="A6" s="97" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="105">
+      <c r="D6" s="103">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="99" t="s">
+      <c r="A7" s="97" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="105">
+      <c r="D7" s="103">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="99" t="s">
+      <c r="A8" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="105">
+      <c r="D8" s="103">
         <v>2.5529999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="99" t="s">
+      <c r="A9" s="97" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="105">
+      <c r="D9" s="103">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="99" t="s">
+      <c r="A10" s="97" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="106">
+      <c r="D10" s="104">
         <v>0.112</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="99" t="s">
+      <c r="A11" s="97" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="105">
+      <c r="D11" s="103">
         <v>3.0790000000000002</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="100" t="s">
+      <c r="A12" s="98" t="s">
         <v>55</v>
       </c>
-      <c r="D12" s="107">
+      <c r="D12" s="105">
         <v>3.2667000000000006</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="99" t="s">
+      <c r="A13" s="97" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="105">
+      <c r="D13" s="103">
         <v>4.5360000000000004E-2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="100" t="s">
+      <c r="A14" s="98" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="107">
+      <c r="D14" s="105">
         <v>3.2213400000000005</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="99" t="s">
+      <c r="A15" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="106">
+      <c r="D15" s="104">
         <v>-1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="100" t="s">
+      <c r="A16" s="98" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="107">
+      <c r="D16" s="105">
         <v>2.2213400000000005</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="99" t="s">
+      <c r="A17" s="97" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="106">
+      <c r="D17" s="104">
         <v>3.1248980097122897E-3</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="99" t="s">
+      <c r="A18" s="97" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="106">
+      <c r="D18" s="104">
         <v>710.85199999999998</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D19" s="108"/>
+      <c r="D19" s="106"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="99" t="s">
+      <c r="A20" s="97" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="109">
+      <c r="D20" s="107">
         <v>0.31</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="99" t="s">
+      <c r="A21" s="97" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="109">
+      <c r="D21" s="107">
         <v>0.1595847581827064</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="99" t="s">
+      <c r="A22" s="97" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="109">
+      <c r="D22" s="107">
         <v>0.10851685393258428</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="99" t="s">
+      <c r="A23" s="97" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="109">
+      <c r="D23" s="107">
         <v>-0.31042982113033701</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D24" s="108"/>
+      <c r="D24" s="106"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="99" t="s">
+      <c r="A25" s="97" t="s">
         <v>93</v>
       </c>
-      <c r="D25" s="108"/>
+      <c r="D25" s="106"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="100" t="s">
+      <c r="A26" s="98" t="s">
         <v>97</v>
       </c>
-      <c r="D26" s="110">
+      <c r="D26" s="108">
         <v>0.25</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="99" t="s">
+      <c r="A27" s="97" t="s">
         <v>128</v>
       </c>
-      <c r="D27" s="111"/>
+      <c r="D27" s="109"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="100" t="s">
+      <c r="A28" s="98" t="s">
         <v>129</v>
       </c>
-      <c r="D28" s="110"/>
+      <c r="D28" s="108"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>